<commit_message>
add data from december, 16th to 19th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -59,8 +54,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,7 +152,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -192,7 +187,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -369,37 +364,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,1662 +426,1662 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
-        <v>44180</v>
+        <v>44184</v>
       </c>
       <c r="B2" s="2">
-        <v>4147</v>
+        <v>4255</v>
       </c>
       <c r="C2" s="2">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2">
-        <v>790</v>
+        <v>809</v>
       </c>
       <c r="E2" s="2">
-        <v>5037</v>
+        <v>5130</v>
       </c>
       <c r="F2" s="2">
-        <v>718</v>
+        <v>743</v>
       </c>
       <c r="G2" s="2">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H2" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I2" s="2">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J2" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
-        <v>44179</v>
+        <v>44183</v>
       </c>
       <c r="B3" s="2">
-        <v>4111</v>
+        <v>4222</v>
       </c>
       <c r="C3" s="2">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D3" s="2">
-        <v>784</v>
+        <v>805</v>
       </c>
       <c r="E3" s="2">
-        <v>4998</v>
+        <v>5122</v>
       </c>
       <c r="F3" s="2">
-        <v>702</v>
+        <v>735</v>
       </c>
       <c r="G3" s="2">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="H3" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I3" s="2">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="J3" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
-        <v>44178</v>
+        <v>44182</v>
       </c>
       <c r="B4" s="2">
-        <v>4097</v>
+        <v>4181</v>
       </c>
       <c r="C4" s="2">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="D4" s="2">
-        <v>779</v>
+        <v>801</v>
       </c>
       <c r="E4" s="2">
-        <v>4956</v>
+        <v>5087</v>
       </c>
       <c r="F4" s="2">
-        <v>695</v>
+        <v>728</v>
       </c>
       <c r="G4" s="2">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="H4" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I4" s="2">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="J4" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
-        <v>44177</v>
+        <v>44181</v>
       </c>
       <c r="B5" s="2">
-        <v>4060</v>
+        <v>4154</v>
       </c>
       <c r="C5" s="2">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D5" s="2">
-        <v>769</v>
+        <v>790</v>
       </c>
       <c r="E5" s="2">
-        <v>4956</v>
+        <v>5066</v>
       </c>
       <c r="F5" s="2">
-        <v>690</v>
+        <v>723</v>
       </c>
       <c r="G5" s="2">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H5" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I5" s="2">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J5" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
-        <v>44176</v>
+        <v>44180</v>
       </c>
       <c r="B6" s="2">
-        <v>4043</v>
+        <v>4147</v>
       </c>
       <c r="C6" s="2">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2">
-        <v>764</v>
+        <v>790</v>
       </c>
       <c r="E6" s="2">
-        <v>4943</v>
+        <v>5037</v>
       </c>
       <c r="F6" s="2">
-        <v>681</v>
+        <v>718</v>
       </c>
       <c r="G6" s="2">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H6" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I6" s="2">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="J6" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
-        <v>44175</v>
+        <v>44179</v>
       </c>
       <c r="B7" s="2">
-        <v>4003</v>
+        <v>4111</v>
       </c>
       <c r="C7" s="2">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="D7" s="2">
-        <v>753</v>
+        <v>784</v>
       </c>
       <c r="E7" s="2">
-        <v>4896</v>
+        <v>4998</v>
       </c>
       <c r="F7" s="2">
-        <v>674</v>
+        <v>702</v>
       </c>
       <c r="G7" s="2">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H7" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I7" s="2">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J7" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
-        <v>44174</v>
+        <v>44178</v>
       </c>
       <c r="B8" s="2">
-        <v>3960</v>
+        <v>4097</v>
       </c>
       <c r="C8" s="2">
-        <v>153</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2">
-        <v>748</v>
+        <v>779</v>
       </c>
       <c r="E8" s="2">
-        <v>4861</v>
+        <v>4956</v>
       </c>
       <c r="F8" s="2">
-        <v>668</v>
+        <v>695</v>
       </c>
       <c r="G8" s="2">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H8" s="2">
         <v>8</v>
       </c>
       <c r="I8" s="2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J8" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
-        <v>44173</v>
+        <v>44177</v>
       </c>
       <c r="B9" s="2">
-        <v>3803</v>
+        <v>4060</v>
       </c>
       <c r="C9" s="2">
-        <v>300</v>
+        <v>127</v>
       </c>
       <c r="D9" s="2">
-        <v>729</v>
+        <v>769</v>
       </c>
       <c r="E9" s="2">
-        <v>4832</v>
+        <v>4956</v>
       </c>
       <c r="F9" s="2">
-        <v>662</v>
+        <v>690</v>
       </c>
       <c r="G9" s="2">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="H9" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I9" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J9" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
-        <v>44172</v>
+        <v>44176</v>
       </c>
       <c r="B10" s="2">
-        <v>3721</v>
+        <v>4043</v>
       </c>
       <c r="C10" s="2">
-        <v>333</v>
+        <v>136</v>
       </c>
       <c r="D10" s="2">
-        <v>714</v>
+        <v>764</v>
       </c>
       <c r="E10" s="2">
-        <v>4768</v>
+        <v>4943</v>
       </c>
       <c r="F10" s="2">
-        <v>656</v>
+        <v>681</v>
       </c>
       <c r="G10" s="2">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="H10" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I10" s="2">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="J10" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
-        <v>44171</v>
+        <v>44175</v>
       </c>
       <c r="B11" s="2">
-        <v>3708</v>
+        <v>4003</v>
       </c>
       <c r="C11" s="2">
-        <v>227</v>
+        <v>140</v>
       </c>
       <c r="D11" s="2">
-        <v>712</v>
+        <v>753</v>
       </c>
       <c r="E11" s="2">
-        <v>4647</v>
+        <v>4896</v>
       </c>
       <c r="F11" s="2">
-        <v>637</v>
+        <v>674</v>
       </c>
       <c r="G11" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H11" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I11" s="2">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J11" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
-        <v>44170</v>
+        <v>44174</v>
       </c>
       <c r="B12" s="2">
-        <v>3690</v>
+        <v>3960</v>
       </c>
       <c r="C12" s="2">
-        <v>242</v>
+        <v>153</v>
       </c>
       <c r="D12" s="2">
-        <v>702</v>
+        <v>748</v>
       </c>
       <c r="E12" s="2">
-        <v>4634</v>
+        <v>4861</v>
       </c>
       <c r="F12" s="2">
-        <v>635</v>
+        <v>668</v>
       </c>
       <c r="G12" s="2">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="H12" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I12" s="2">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="J12" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
-        <v>44169</v>
+        <v>44173</v>
       </c>
       <c r="B13" s="2">
-        <v>3683</v>
+        <v>3803</v>
       </c>
       <c r="C13" s="2">
-        <v>234</v>
+        <v>300</v>
       </c>
       <c r="D13" s="2">
-        <v>693</v>
+        <v>729</v>
       </c>
       <c r="E13" s="2">
-        <v>4610</v>
+        <v>4832</v>
       </c>
       <c r="F13" s="2">
-        <v>632</v>
+        <v>662</v>
       </c>
       <c r="G13" s="2">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="H13" s="2">
         <v>6</v>
       </c>
       <c r="I13" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="J13" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
-        <v>44168</v>
+        <v>44172</v>
       </c>
       <c r="B14" s="2">
-        <v>3676</v>
+        <v>3721</v>
       </c>
       <c r="C14" s="2">
-        <v>211</v>
+        <v>333</v>
       </c>
       <c r="D14" s="2">
-        <v>688</v>
+        <v>714</v>
       </c>
       <c r="E14" s="2">
-        <v>4575</v>
+        <v>4768</v>
       </c>
       <c r="F14" s="2">
-        <v>612</v>
+        <v>656</v>
       </c>
       <c r="G14" s="2">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="H14" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I14" s="2">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="J14" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
-        <v>44167</v>
+        <v>44171</v>
       </c>
       <c r="B15" s="2">
-        <v>3669</v>
+        <v>3708</v>
       </c>
       <c r="C15" s="2">
-        <v>174</v>
+        <v>227</v>
       </c>
       <c r="D15" s="2">
-        <v>688</v>
+        <v>712</v>
       </c>
       <c r="E15" s="2">
-        <v>4531</v>
+        <v>4647</v>
       </c>
       <c r="F15" s="2">
-        <v>587</v>
+        <v>637</v>
       </c>
       <c r="G15" s="2">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="H15" s="2">
         <v>6</v>
       </c>
       <c r="I15" s="2">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="J15" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
-        <v>44166</v>
+        <v>44170</v>
       </c>
       <c r="B16" s="2">
-        <v>3639</v>
+        <v>3690</v>
       </c>
       <c r="C16" s="2">
-        <v>170</v>
+        <v>242</v>
       </c>
       <c r="D16" s="2">
-        <v>685</v>
+        <v>702</v>
       </c>
       <c r="E16" s="2">
-        <v>4494</v>
+        <v>4634</v>
       </c>
       <c r="F16" s="2">
-        <v>569</v>
+        <v>635</v>
       </c>
       <c r="G16" s="2">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="H16" s="2">
         <v>6</v>
       </c>
       <c r="I16" s="2">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="J16" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
-        <v>44165</v>
+        <v>44169</v>
       </c>
       <c r="B17" s="2">
-        <v>3601</v>
+        <v>3683</v>
       </c>
       <c r="C17" s="2">
-        <v>173</v>
+        <v>234</v>
       </c>
       <c r="D17" s="2">
-        <v>675</v>
+        <v>693</v>
       </c>
       <c r="E17" s="2">
-        <v>4449</v>
+        <v>4610</v>
       </c>
       <c r="F17" s="2">
-        <v>542</v>
+        <v>632</v>
       </c>
       <c r="G17" s="2">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="H17" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I17" s="2">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="J17" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
-        <v>44164</v>
+        <v>44168</v>
       </c>
       <c r="B18" s="2">
-        <v>3529</v>
+        <v>3676</v>
       </c>
       <c r="C18" s="2">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="D18" s="2">
-        <v>651</v>
+        <v>688</v>
       </c>
       <c r="E18" s="2">
-        <v>4372</v>
+        <v>4575</v>
       </c>
       <c r="F18" s="2">
-        <v>530</v>
+        <v>612</v>
       </c>
       <c r="G18" s="2">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="H18" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18" s="2">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="J18" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
-        <v>44163</v>
+        <v>44167</v>
       </c>
       <c r="B19" s="2">
-        <v>3502</v>
+        <v>3669</v>
       </c>
       <c r="C19" s="2">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="D19" s="2">
-        <v>645</v>
+        <v>688</v>
       </c>
       <c r="E19" s="2">
-        <v>4366</v>
+        <v>4531</v>
       </c>
       <c r="F19" s="2">
-        <v>521</v>
+        <v>587</v>
       </c>
       <c r="G19" s="2">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H19" s="2">
         <v>6</v>
       </c>
       <c r="I19" s="2">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="J19" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
-        <v>44162</v>
+        <v>44166</v>
       </c>
       <c r="B20" s="2">
-        <v>3473</v>
+        <v>3639</v>
       </c>
       <c r="C20" s="2">
-        <v>263</v>
+        <v>170</v>
       </c>
       <c r="D20" s="2">
-        <v>628</v>
+        <v>685</v>
       </c>
       <c r="E20" s="2">
-        <v>4364</v>
+        <v>4494</v>
       </c>
       <c r="F20" s="2">
-        <v>504</v>
+        <v>569</v>
       </c>
       <c r="G20" s="2">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H20" s="2">
         <v>6</v>
       </c>
       <c r="I20" s="2">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="J20" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
-        <v>44161</v>
+        <v>44165</v>
       </c>
       <c r="B21" s="2">
-        <v>3446</v>
+        <v>3601</v>
       </c>
       <c r="C21" s="2">
-        <v>263</v>
+        <v>173</v>
       </c>
       <c r="D21" s="2">
-        <v>616</v>
+        <v>675</v>
       </c>
       <c r="E21" s="2">
-        <v>4325</v>
+        <v>4449</v>
       </c>
       <c r="F21" s="2">
-        <v>490</v>
+        <v>542</v>
       </c>
       <c r="G21" s="2">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H21" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I21" s="2">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J21" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
-        <v>44160</v>
+        <v>44164</v>
       </c>
       <c r="B22" s="2">
-        <v>3399</v>
+        <v>3529</v>
       </c>
       <c r="C22" s="2">
-        <v>267</v>
+        <v>192</v>
       </c>
       <c r="D22" s="2">
-        <v>606</v>
+        <v>651</v>
       </c>
       <c r="E22" s="2">
-        <v>4272</v>
+        <v>4372</v>
       </c>
       <c r="F22" s="2">
-        <v>477</v>
+        <v>530</v>
       </c>
       <c r="G22" s="2">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H22" s="2">
         <v>7</v>
       </c>
       <c r="I22" s="2">
+        <v>100</v>
+      </c>
+      <c r="J22" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3502</v>
+      </c>
+      <c r="C23" s="2">
+        <v>219</v>
+      </c>
+      <c r="D23" s="2">
+        <v>645</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4366</v>
+      </c>
+      <c r="F23" s="2">
+        <v>521</v>
+      </c>
+      <c r="G23" s="2">
+        <v>111</v>
+      </c>
+      <c r="H23" s="2">
+        <v>6</v>
+      </c>
+      <c r="I23" s="2">
+        <v>105</v>
+      </c>
+      <c r="J23" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3473</v>
+      </c>
+      <c r="C24" s="2">
+        <v>263</v>
+      </c>
+      <c r="D24" s="2">
+        <v>628</v>
+      </c>
+      <c r="E24" s="2">
+        <v>4364</v>
+      </c>
+      <c r="F24" s="2">
+        <v>504</v>
+      </c>
+      <c r="G24" s="2">
+        <v>112</v>
+      </c>
+      <c r="H24" s="2">
+        <v>6</v>
+      </c>
+      <c r="I24" s="2">
+        <v>106</v>
+      </c>
+      <c r="J24" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3446</v>
+      </c>
+      <c r="C25" s="2">
+        <v>263</v>
+      </c>
+      <c r="D25" s="2">
+        <v>616</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4325</v>
+      </c>
+      <c r="F25" s="2">
+        <v>490</v>
+      </c>
+      <c r="G25" s="2">
+        <v>114</v>
+      </c>
+      <c r="H25" s="2">
+        <v>6</v>
+      </c>
+      <c r="I25" s="2">
+        <v>108</v>
+      </c>
+      <c r="J25" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1">
+        <v>44160</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3399</v>
+      </c>
+      <c r="C26" s="2">
+        <v>267</v>
+      </c>
+      <c r="D26" s="2">
+        <v>606</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4272</v>
+      </c>
+      <c r="F26" s="2">
+        <v>477</v>
+      </c>
+      <c r="G26" s="2">
+        <v>117</v>
+      </c>
+      <c r="H26" s="2">
+        <v>7</v>
+      </c>
+      <c r="I26" s="2">
         <v>110</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J26" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="27" spans="1:10">
+      <c r="A27" s="1">
         <v>44159</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B27" s="2">
         <v>3336</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C27" s="2">
         <v>282</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D27" s="2">
         <v>582</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E27" s="2">
         <v>4200</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F27" s="2">
         <v>464</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G27" s="2">
         <v>107</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H27" s="2">
         <v>7</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I27" s="2">
         <v>100</v>
-      </c>
-      <c r="J23" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>44158</v>
-      </c>
-      <c r="B24" s="2">
-        <v>3283</v>
-      </c>
-      <c r="C24" s="2">
-        <v>273</v>
-      </c>
-      <c r="D24" s="2">
-        <v>568</v>
-      </c>
-      <c r="E24" s="2">
-        <v>4124</v>
-      </c>
-      <c r="F24" s="2">
-        <v>442</v>
-      </c>
-      <c r="G24" s="2">
-        <v>115</v>
-      </c>
-      <c r="H24" s="2">
-        <v>7</v>
-      </c>
-      <c r="I24" s="2">
-        <v>108</v>
-      </c>
-      <c r="J24" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>44157</v>
-      </c>
-      <c r="B25" s="2">
-        <v>3279</v>
-      </c>
-      <c r="C25" s="2">
-        <v>177</v>
-      </c>
-      <c r="D25" s="2">
-        <v>562</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4018</v>
-      </c>
-      <c r="F25" s="2">
-        <v>430</v>
-      </c>
-      <c r="G25" s="2">
-        <v>121</v>
-      </c>
-      <c r="H25" s="2">
-        <v>7</v>
-      </c>
-      <c r="I25" s="2">
-        <v>114</v>
-      </c>
-      <c r="J25" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>44156</v>
-      </c>
-      <c r="B26" s="2">
-        <v>3235</v>
-      </c>
-      <c r="C26" s="2">
-        <v>242</v>
-      </c>
-      <c r="D26" s="2">
-        <v>539</v>
-      </c>
-      <c r="E26" s="2">
-        <v>4016</v>
-      </c>
-      <c r="F26" s="2">
-        <v>424</v>
-      </c>
-      <c r="G26" s="2">
-        <v>104</v>
-      </c>
-      <c r="H26" s="2">
-        <v>6</v>
-      </c>
-      <c r="I26" s="2">
-        <v>98</v>
-      </c>
-      <c r="J26" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>44155</v>
-      </c>
-      <c r="B27" s="2">
-        <v>3200</v>
-      </c>
-      <c r="C27" s="2">
-        <v>245</v>
-      </c>
-      <c r="D27" s="2">
-        <v>535</v>
-      </c>
-      <c r="E27" s="2">
-        <v>3980</v>
-      </c>
-      <c r="F27" s="2">
-        <v>413</v>
-      </c>
-      <c r="G27" s="2">
-        <v>111</v>
-      </c>
-      <c r="H27" s="2">
-        <v>6</v>
-      </c>
-      <c r="I27" s="2">
-        <v>105</v>
       </c>
       <c r="J27" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
-        <v>44154</v>
+        <v>44158</v>
       </c>
       <c r="B28" s="2">
-        <v>3071</v>
+        <v>3283</v>
       </c>
       <c r="C28" s="2">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="D28" s="2">
-        <v>525</v>
+        <v>568</v>
       </c>
       <c r="E28" s="2">
-        <v>3908</v>
+        <v>4124</v>
       </c>
       <c r="F28" s="2">
-        <v>406</v>
+        <v>442</v>
       </c>
       <c r="G28" s="2">
+        <v>115</v>
+      </c>
+      <c r="H28" s="2">
+        <v>7</v>
+      </c>
+      <c r="I28" s="2">
         <v>108</v>
-      </c>
-      <c r="H28" s="2">
-        <v>3</v>
-      </c>
-      <c r="I28" s="2">
-        <v>105</v>
       </c>
       <c r="J28" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
-        <v>44153</v>
+        <v>44157</v>
       </c>
       <c r="B29" s="2">
-        <v>3039</v>
+        <v>3279</v>
       </c>
       <c r="C29" s="2">
-        <v>294</v>
+        <v>177</v>
       </c>
       <c r="D29" s="2">
-        <v>516</v>
+        <v>562</v>
       </c>
       <c r="E29" s="2">
-        <v>3849</v>
+        <v>4018</v>
       </c>
       <c r="F29" s="2">
-        <v>399</v>
+        <v>430</v>
       </c>
       <c r="G29" s="2">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="H29" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I29" s="2">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="J29" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
+        <v>44156</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3235</v>
+      </c>
+      <c r="C30" s="2">
+        <v>242</v>
+      </c>
+      <c r="D30" s="2">
+        <v>539</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4016</v>
+      </c>
+      <c r="F30" s="2">
+        <v>424</v>
+      </c>
+      <c r="G30" s="2">
+        <v>104</v>
+      </c>
+      <c r="H30" s="2">
+        <v>6</v>
+      </c>
+      <c r="I30" s="2">
+        <v>98</v>
+      </c>
+      <c r="J30" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1">
+        <v>44155</v>
+      </c>
+      <c r="B31" s="2">
+        <v>3200</v>
+      </c>
+      <c r="C31" s="2">
+        <v>245</v>
+      </c>
+      <c r="D31" s="2">
+        <v>535</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3980</v>
+      </c>
+      <c r="F31" s="2">
+        <v>413</v>
+      </c>
+      <c r="G31" s="2">
+        <v>111</v>
+      </c>
+      <c r="H31" s="2">
+        <v>6</v>
+      </c>
+      <c r="I31" s="2">
+        <v>105</v>
+      </c>
+      <c r="J31" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1">
+        <v>44154</v>
+      </c>
+      <c r="B32" s="2">
+        <v>3071</v>
+      </c>
+      <c r="C32" s="2">
+        <v>312</v>
+      </c>
+      <c r="D32" s="2">
+        <v>525</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3908</v>
+      </c>
+      <c r="F32" s="2">
+        <v>406</v>
+      </c>
+      <c r="G32" s="2">
+        <v>108</v>
+      </c>
+      <c r="H32" s="2">
+        <v>3</v>
+      </c>
+      <c r="I32" s="2">
+        <v>105</v>
+      </c>
+      <c r="J32" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1">
+        <v>44153</v>
+      </c>
+      <c r="B33" s="2">
+        <v>3039</v>
+      </c>
+      <c r="C33" s="2">
+        <v>294</v>
+      </c>
+      <c r="D33" s="2">
+        <v>516</v>
+      </c>
+      <c r="E33" s="2">
+        <v>3849</v>
+      </c>
+      <c r="F33" s="2">
+        <v>399</v>
+      </c>
+      <c r="G33" s="2">
+        <v>106</v>
+      </c>
+      <c r="H33" s="2">
+        <v>3</v>
+      </c>
+      <c r="I33" s="2">
+        <v>103</v>
+      </c>
+      <c r="J33" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="1">
         <v>44152</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B34" s="2">
         <v>3004</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C34" s="2">
         <v>238</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D34" s="2">
         <v>499</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E34" s="2">
         <v>3741</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F34" s="2">
         <v>394</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G34" s="2">
         <v>95</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1</v>
-      </c>
-      <c r="I30" s="2">
-        <v>94</v>
-      </c>
-      <c r="J30" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>44151</v>
-      </c>
-      <c r="B31" s="2">
-        <v>3000</v>
-      </c>
-      <c r="C31" s="2">
-        <v>204</v>
-      </c>
-      <c r="D31" s="2">
-        <v>490</v>
-      </c>
-      <c r="E31" s="2">
-        <v>3694</v>
-      </c>
-      <c r="F31" s="2">
-        <v>388</v>
-      </c>
-      <c r="G31" s="2">
-        <v>92</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
-        <v>91</v>
-      </c>
-      <c r="J31" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>44150</v>
-      </c>
-      <c r="B32" s="2">
-        <v>2982</v>
-      </c>
-      <c r="C32" s="2">
-        <v>201</v>
-      </c>
-      <c r="D32" s="2">
-        <v>471</v>
-      </c>
-      <c r="E32" s="2">
-        <v>3654</v>
-      </c>
-      <c r="F32" s="2">
-        <v>384</v>
-      </c>
-      <c r="G32" s="2">
-        <v>77</v>
-      </c>
-      <c r="H32" s="2">
-        <v>1</v>
-      </c>
-      <c r="I32" s="2">
-        <v>76</v>
-      </c>
-      <c r="J32" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>44149</v>
-      </c>
-      <c r="B33" s="2">
-        <v>2970</v>
-      </c>
-      <c r="C33" s="2">
-        <v>214</v>
-      </c>
-      <c r="D33" s="2">
-        <v>465</v>
-      </c>
-      <c r="E33" s="2">
-        <v>3649</v>
-      </c>
-      <c r="F33" s="2">
-        <v>378</v>
-      </c>
-      <c r="G33" s="2">
-        <v>77</v>
-      </c>
-      <c r="H33" s="2">
-        <v>1</v>
-      </c>
-      <c r="I33" s="2">
-        <v>76</v>
-      </c>
-      <c r="J33" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>44148</v>
-      </c>
-      <c r="B34" s="2">
-        <v>2954</v>
-      </c>
-      <c r="C34" s="2">
-        <v>185</v>
-      </c>
-      <c r="D34" s="2">
-        <v>453</v>
-      </c>
-      <c r="E34" s="2">
-        <v>3592</v>
-      </c>
-      <c r="F34" s="2">
-        <v>372</v>
-      </c>
-      <c r="G34" s="2">
-        <v>71</v>
       </c>
       <c r="H34" s="2">
         <v>1</v>
       </c>
       <c r="I34" s="2">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="J34" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
-        <v>44147</v>
+        <v>44151</v>
       </c>
       <c r="B35" s="2">
-        <v>2943</v>
+        <v>3000</v>
       </c>
       <c r="C35" s="2">
-        <v>151</v>
+        <v>204</v>
       </c>
       <c r="D35" s="2">
-        <v>441</v>
+        <v>490</v>
       </c>
       <c r="E35" s="2">
-        <v>3535</v>
+        <v>3694</v>
       </c>
       <c r="F35" s="2">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="G35" s="2">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="H35" s="2">
         <v>1</v>
       </c>
       <c r="I35" s="2">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="J35" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
-        <v>44146</v>
+        <v>44150</v>
       </c>
       <c r="B36" s="2">
-        <v>2927</v>
+        <v>2982</v>
       </c>
       <c r="C36" s="2">
-        <v>137</v>
+        <v>201</v>
       </c>
       <c r="D36" s="2">
-        <v>419</v>
+        <v>471</v>
       </c>
       <c r="E36" s="2">
-        <v>3483</v>
+        <v>3654</v>
       </c>
       <c r="F36" s="2">
-        <v>367</v>
+        <v>384</v>
       </c>
       <c r="G36" s="2">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="H36" s="2">
         <v>1</v>
       </c>
       <c r="I36" s="2">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="J36" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
-        <v>44145</v>
+        <v>44149</v>
       </c>
       <c r="B37" s="2">
-        <v>2922</v>
+        <v>2970</v>
       </c>
       <c r="C37" s="2">
-        <v>110</v>
+        <v>214</v>
       </c>
       <c r="D37" s="2">
-        <v>414</v>
+        <v>465</v>
       </c>
       <c r="E37" s="2">
-        <v>3446</v>
+        <v>3649</v>
       </c>
       <c r="F37" s="2">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="G37" s="2">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="H37" s="2">
         <v>1</v>
       </c>
       <c r="I37" s="2">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="J37" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
-        <v>44144</v>
+        <v>44148</v>
       </c>
       <c r="B38" s="2">
-        <v>2912</v>
+        <v>2954</v>
       </c>
       <c r="C38" s="2">
-        <v>78</v>
+        <v>185</v>
       </c>
       <c r="D38" s="2">
-        <v>403</v>
+        <v>453</v>
       </c>
       <c r="E38" s="2">
-        <v>3393</v>
+        <v>3592</v>
       </c>
       <c r="F38" s="2">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="G38" s="2">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="H38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="2">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="J38" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
-        <v>44143</v>
+        <v>44147</v>
       </c>
       <c r="B39" s="2">
-        <v>2909</v>
+        <v>2943</v>
       </c>
       <c r="C39" s="2">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="D39" s="2">
-        <v>401</v>
+        <v>441</v>
       </c>
       <c r="E39" s="2">
-        <v>3345</v>
+        <v>3535</v>
       </c>
       <c r="F39" s="2">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="G39" s="2">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="H39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="2">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="J39" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
-        <v>44142</v>
+        <v>44146</v>
       </c>
       <c r="B40" s="2">
-        <v>2879</v>
+        <v>2927</v>
       </c>
       <c r="C40" s="2">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="D40" s="2">
-        <v>396</v>
+        <v>419</v>
       </c>
       <c r="E40" s="2">
-        <v>3324</v>
+        <v>3483</v>
       </c>
       <c r="F40" s="2">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="G40" s="2">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="H40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="2">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="J40" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
-        <v>44141</v>
+        <v>44145</v>
       </c>
       <c r="B41" s="2">
-        <v>2859</v>
+        <v>2922</v>
       </c>
       <c r="C41" s="2">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="D41" s="2">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="E41" s="2">
-        <v>3317</v>
+        <v>3446</v>
       </c>
       <c r="F41" s="2">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="G41" s="2">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="H41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="2">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="J41" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
-        <v>44140</v>
+        <v>44144</v>
       </c>
       <c r="B42" s="2">
-        <v>2812</v>
+        <v>2912</v>
       </c>
       <c r="C42" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D42" s="2">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="E42" s="2">
-        <v>3278</v>
+        <v>3393</v>
       </c>
       <c r="F42" s="2">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="G42" s="2">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
       </c>
       <c r="I42" s="2">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J42" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
-        <v>44139</v>
+        <v>44143</v>
       </c>
       <c r="B43" s="2">
-        <v>2803</v>
+        <v>2909</v>
       </c>
       <c r="C43" s="2">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="D43" s="2">
-        <v>379</v>
+        <v>401</v>
       </c>
       <c r="E43" s="2">
-        <v>3252</v>
+        <v>3345</v>
       </c>
       <c r="F43" s="2">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="G43" s="2">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
       </c>
       <c r="I43" s="2">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="J43" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
-        <v>44138</v>
+        <v>44142</v>
       </c>
       <c r="B44" s="2">
-        <v>2785</v>
+        <v>2879</v>
       </c>
       <c r="C44" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D44" s="2">
-        <v>377</v>
+        <v>396</v>
       </c>
       <c r="E44" s="2">
-        <v>3204</v>
+        <v>3324</v>
       </c>
       <c r="F44" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G44" s="2">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H44" s="2">
         <v>0</v>
       </c>
       <c r="I44" s="2">
+        <v>29</v>
+      </c>
+      <c r="J44" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="1">
+        <v>44141</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2859</v>
+      </c>
+      <c r="C45" s="2">
+        <v>70</v>
+      </c>
+      <c r="D45" s="2">
+        <v>388</v>
+      </c>
+      <c r="E45" s="2">
+        <v>3317</v>
+      </c>
+      <c r="F45" s="2">
+        <v>356</v>
+      </c>
+      <c r="G45" s="2">
+        <v>22</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2">
+        <v>22</v>
+      </c>
+      <c r="J45" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2812</v>
+      </c>
+      <c r="C46" s="2">
+        <v>86</v>
+      </c>
+      <c r="D46" s="2">
+        <v>380</v>
+      </c>
+      <c r="E46" s="2">
+        <v>3278</v>
+      </c>
+      <c r="F46" s="2">
+        <v>355</v>
+      </c>
+      <c r="G46" s="2">
+        <v>16</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2">
+        <v>16</v>
+      </c>
+      <c r="J46" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="1">
+        <v>44139</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2803</v>
+      </c>
+      <c r="C47" s="2">
+        <v>70</v>
+      </c>
+      <c r="D47" s="2">
+        <v>379</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3252</v>
+      </c>
+      <c r="F47" s="2">
+        <v>355</v>
+      </c>
+      <c r="G47" s="2">
+        <v>15</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2">
+        <v>15</v>
+      </c>
+      <c r="J47" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1">
+        <v>44138</v>
+      </c>
+      <c r="B48" s="2">
+        <v>2785</v>
+      </c>
+      <c r="C48" s="2">
+        <v>42</v>
+      </c>
+      <c r="D48" s="2">
+        <v>377</v>
+      </c>
+      <c r="E48" s="2">
+        <v>3204</v>
+      </c>
+      <c r="F48" s="2">
+        <v>355</v>
+      </c>
+      <c r="G48" s="2">
         <v>13</v>
       </c>
-      <c r="J44" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <v>13</v>
+      </c>
+      <c r="J48" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1">
         <v>44137</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B49" s="2">
         <v>2776</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C49" s="2">
         <v>35</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D49" s="2">
         <v>376</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E49" s="2">
         <v>3187</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F49" s="2">
         <v>354</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G49" s="2">
         <v>13</v>
-      </c>
-      <c r="H45" s="2">
-        <v>1</v>
-      </c>
-      <c r="I45" s="2">
-        <v>12</v>
-      </c>
-      <c r="J45" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>44136</v>
-      </c>
-      <c r="B46" s="2">
-        <v>2763</v>
-      </c>
-      <c r="C46" s="2">
-        <v>39</v>
-      </c>
-      <c r="D46" s="2">
-        <v>376</v>
-      </c>
-      <c r="E46" s="2">
-        <v>3178</v>
-      </c>
-      <c r="F46" s="2">
-        <v>354</v>
-      </c>
-      <c r="G46" s="2">
-        <v>13</v>
-      </c>
-      <c r="H46" s="2">
-        <v>1</v>
-      </c>
-      <c r="I46" s="2">
-        <v>12</v>
-      </c>
-      <c r="J46" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>44135</v>
-      </c>
-      <c r="B47" s="2">
-        <v>2762</v>
-      </c>
-      <c r="C47" s="2">
-        <v>41</v>
-      </c>
-      <c r="D47" s="2">
-        <v>375</v>
-      </c>
-      <c r="E47" s="2">
-        <v>3178</v>
-      </c>
-      <c r="F47" s="2">
-        <v>354</v>
-      </c>
-      <c r="G47" s="2">
-        <v>12</v>
-      </c>
-      <c r="H47" s="2">
-        <v>1</v>
-      </c>
-      <c r="I47" s="2">
-        <v>11</v>
-      </c>
-      <c r="J47" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>44134</v>
-      </c>
-      <c r="B48" s="2">
-        <v>2736</v>
-      </c>
-      <c r="C48" s="2">
-        <v>59</v>
-      </c>
-      <c r="D48" s="2">
-        <v>370</v>
-      </c>
-      <c r="E48" s="2">
-        <v>3165</v>
-      </c>
-      <c r="F48" s="2">
-        <v>354</v>
-      </c>
-      <c r="G48" s="2">
-        <v>7</v>
-      </c>
-      <c r="H48" s="2">
-        <v>1</v>
-      </c>
-      <c r="I48" s="2">
-        <v>6</v>
-      </c>
-      <c r="J48" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>44133</v>
-      </c>
-      <c r="B49" s="2">
-        <v>2720</v>
-      </c>
-      <c r="C49" s="2">
-        <v>59</v>
-      </c>
-      <c r="D49" s="2">
-        <v>366</v>
-      </c>
-      <c r="E49" s="2">
-        <v>3145</v>
-      </c>
-      <c r="F49" s="2">
-        <v>353</v>
-      </c>
-      <c r="G49" s="2">
-        <v>4</v>
       </c>
       <c r="H49" s="2">
         <v>1</v>
       </c>
       <c r="I49" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J49" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
-        <v>44132</v>
+        <v>44136</v>
       </c>
       <c r="B50" s="2">
-        <v>2713</v>
+        <v>2763</v>
       </c>
       <c r="C50" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D50" s="2">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="E50" s="2">
-        <v>3114</v>
+        <v>3178</v>
       </c>
       <c r="F50" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G50" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H50" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J50" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
-        <v>44131</v>
+        <v>44135</v>
       </c>
       <c r="B51" s="2">
-        <v>2702</v>
+        <v>2762</v>
       </c>
       <c r="C51" s="2">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D51" s="2">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="E51" s="2">
-        <v>3098</v>
+        <v>3178</v>
       </c>
       <c r="F51" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G51" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H51" s="2">
         <v>1</v>
       </c>
       <c r="I51" s="2">
+        <v>11</v>
+      </c>
+      <c r="J51" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
+        <v>44134</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2736</v>
+      </c>
+      <c r="C52" s="2">
+        <v>59</v>
+      </c>
+      <c r="D52" s="2">
+        <v>370</v>
+      </c>
+      <c r="E52" s="2">
+        <v>3165</v>
+      </c>
+      <c r="F52" s="2">
+        <v>354</v>
+      </c>
+      <c r="G52" s="2">
+        <v>7</v>
+      </c>
+      <c r="H52" s="2">
         <v>1</v>
       </c>
-      <c r="J51" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>44130</v>
-      </c>
-      <c r="B52" s="2">
-        <v>2698</v>
-      </c>
-      <c r="C52" s="2">
-        <v>17</v>
-      </c>
-      <c r="D52" s="2">
-        <v>364</v>
-      </c>
-      <c r="E52" s="2">
-        <v>3079</v>
-      </c>
-      <c r="F52" s="2">
+      <c r="I52" s="2">
+        <v>6</v>
+      </c>
+      <c r="J52" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
+        <v>44133</v>
+      </c>
+      <c r="B53" s="2">
+        <v>2720</v>
+      </c>
+      <c r="C53" s="2">
+        <v>59</v>
+      </c>
+      <c r="D53" s="2">
+        <v>366</v>
+      </c>
+      <c r="E53" s="2">
+        <v>3145</v>
+      </c>
+      <c r="F53" s="2">
         <v>353</v>
       </c>
-      <c r="G52" s="2">
-        <v>2</v>
-      </c>
-      <c r="H52" s="2">
-        <v>0</v>
-      </c>
-      <c r="I52" s="2">
-        <v>2</v>
-      </c>
-      <c r="J52" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>44129</v>
-      </c>
-      <c r="B53" s="2">
-        <v>2690</v>
-      </c>
-      <c r="C53" s="2">
-        <v>21</v>
-      </c>
-      <c r="D53" s="2">
-        <v>364</v>
-      </c>
-      <c r="E53" s="2">
-        <v>3073</v>
-      </c>
-      <c r="F53" s="2">
-        <v>352</v>
-      </c>
       <c r="G53" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="2">
         <v>3</v>
@@ -2095,1173 +2090,1301 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
-        <v>44128</v>
+        <v>44132</v>
       </c>
       <c r="B54" s="2">
-        <v>2676</v>
+        <v>2713</v>
       </c>
       <c r="C54" s="2">
         <v>36</v>
       </c>
       <c r="D54" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E54" s="2">
-        <v>3075</v>
+        <v>3114</v>
       </c>
       <c r="F54" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G54" s="2">
         <v>3</v>
       </c>
       <c r="H54" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I54" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J54" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
-        <v>44127</v>
+        <v>44131</v>
       </c>
       <c r="B55" s="2">
-        <v>2670</v>
+        <v>2702</v>
       </c>
       <c r="C55" s="2">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D55" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E55" s="2">
-        <v>3061</v>
+        <v>3098</v>
       </c>
       <c r="F55" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G55" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J55" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
-        <v>44126</v>
+        <v>44130</v>
       </c>
       <c r="B56" s="2">
-        <v>2656</v>
+        <v>2698</v>
       </c>
       <c r="C56" s="2">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D56" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E56" s="2">
-        <v>3052</v>
+        <v>3079</v>
       </c>
       <c r="F56" s="2">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="G56" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
       </c>
       <c r="I56" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J56" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
-        <v>44125</v>
+        <v>44129</v>
       </c>
       <c r="B57" s="2">
-        <v>2648</v>
+        <v>2690</v>
       </c>
       <c r="C57" s="2">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D57" s="2">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="E57" s="2">
-        <v>3042</v>
+        <v>3073</v>
       </c>
       <c r="F57" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="G57" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H57" s="2">
         <v>0</v>
       </c>
       <c r="I57" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J57" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
-        <v>44124</v>
+        <v>44128</v>
       </c>
       <c r="B58" s="2">
-        <v>2631</v>
+        <v>2676</v>
       </c>
       <c r="C58" s="2">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D58" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E58" s="2">
-        <v>3033</v>
+        <v>3075</v>
       </c>
       <c r="F58" s="2">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="G58" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H58" s="2">
         <v>0</v>
       </c>
       <c r="I58" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J58" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
-        <v>44123</v>
+        <v>44127</v>
       </c>
       <c r="B59" s="2">
-        <v>2631</v>
+        <v>2670</v>
       </c>
       <c r="C59" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D59" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E59" s="2">
-        <v>3018</v>
+        <v>3061</v>
       </c>
       <c r="F59" s="2">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="G59" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H59" s="2">
         <v>0</v>
       </c>
       <c r="I59" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J59" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
-        <v>44122</v>
+        <v>44126</v>
       </c>
       <c r="B60" s="2">
-        <v>2615</v>
+        <v>2656</v>
       </c>
       <c r="C60" s="2">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D60" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E60" s="2">
-        <v>3005</v>
+        <v>3052</v>
       </c>
       <c r="F60" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="G60" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H60" s="2">
         <v>0</v>
       </c>
       <c r="I60" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J60" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
-        <v>44121</v>
+        <v>44125</v>
       </c>
       <c r="B61" s="2">
-        <v>2613</v>
+        <v>2648</v>
       </c>
       <c r="C61" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D61" s="2">
         <v>362</v>
       </c>
       <c r="E61" s="2">
-        <v>3005</v>
+        <v>3042</v>
       </c>
       <c r="F61" s="2">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G61" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H61" s="2">
         <v>0</v>
       </c>
       <c r="I61" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J61" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
-        <v>44120</v>
+        <v>44124</v>
       </c>
       <c r="B62" s="2">
-        <v>2611</v>
+        <v>2631</v>
       </c>
       <c r="C62" s="2">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D62" s="2">
         <v>362</v>
       </c>
       <c r="E62" s="2">
-        <v>2999</v>
+        <v>3033</v>
       </c>
       <c r="F62" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="G62" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H62" s="2">
         <v>0</v>
       </c>
       <c r="I62" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J62" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
-        <v>44119</v>
+        <v>44123</v>
       </c>
       <c r="B63" s="2">
-        <v>2595</v>
+        <v>2631</v>
       </c>
       <c r="C63" s="2">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D63" s="2">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="E63" s="2">
-        <v>2989</v>
+        <v>3018</v>
       </c>
       <c r="F63" s="2">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="G63" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H63" s="2">
         <v>0</v>
       </c>
       <c r="I63" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J63" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
-        <v>44118</v>
+        <v>44122</v>
       </c>
       <c r="B64" s="2">
-        <v>2586</v>
+        <v>2615</v>
       </c>
       <c r="C64" s="2">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D64" s="2">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="E64" s="2">
-        <v>2976</v>
+        <v>3005</v>
       </c>
       <c r="F64" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="G64" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H64" s="2">
         <v>0</v>
       </c>
       <c r="I64" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J64" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
-        <v>44117</v>
+        <v>44121</v>
       </c>
       <c r="B65" s="2">
-        <v>2585</v>
+        <v>2613</v>
       </c>
       <c r="C65" s="2">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D65" s="2">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="E65" s="2">
-        <v>2959</v>
+        <v>3005</v>
       </c>
       <c r="F65" s="2">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="G65" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H65" s="2">
         <v>0</v>
       </c>
       <c r="I65" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J65" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
-        <v>44116</v>
+        <v>44120</v>
       </c>
       <c r="B66" s="2">
-        <v>2584</v>
+        <v>2611</v>
       </c>
       <c r="C66" s="2">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D66" s="2">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="E66" s="2">
-        <v>2954</v>
+        <v>2999</v>
       </c>
       <c r="F66" s="2">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="G66" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H66" s="2">
         <v>0</v>
       </c>
       <c r="I66" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J66" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
-        <v>44115</v>
+        <v>44119</v>
       </c>
       <c r="B67" s="2">
-        <v>2584</v>
+        <v>2595</v>
       </c>
       <c r="C67" s="2">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D67" s="2">
         <v>358</v>
       </c>
       <c r="E67" s="2">
-        <v>2953</v>
+        <v>2989</v>
       </c>
       <c r="F67" s="2">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="G67" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H67" s="2">
         <v>0</v>
       </c>
       <c r="I67" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J67" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
-        <v>44114</v>
+        <v>44118</v>
       </c>
       <c r="B68" s="2">
-        <v>2577</v>
+        <v>2586</v>
       </c>
       <c r="C68" s="2">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D68" s="2">
         <v>358</v>
       </c>
       <c r="E68" s="2">
-        <v>2953</v>
+        <v>2976</v>
       </c>
       <c r="F68" s="2">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="G68" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H68" s="2">
         <v>0</v>
       </c>
       <c r="I68" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J68" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <v>44113</v>
+        <v>44117</v>
       </c>
       <c r="B69" s="2">
-        <v>2572</v>
+        <v>2585</v>
       </c>
       <c r="C69" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D69" s="2">
         <v>358</v>
       </c>
       <c r="E69" s="2">
-        <v>2945</v>
+        <v>2959</v>
       </c>
       <c r="F69" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="G69" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H69" s="2">
         <v>0</v>
       </c>
       <c r="I69" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J69" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
-        <v>44112</v>
+        <v>44116</v>
       </c>
       <c r="B70" s="2">
-        <v>2561</v>
+        <v>2584</v>
       </c>
       <c r="C70" s="2">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D70" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E70" s="2">
-        <v>2944</v>
+        <v>2954</v>
       </c>
       <c r="F70" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="G70" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H70" s="2">
         <v>0</v>
       </c>
       <c r="I70" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J70" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
-        <v>44111</v>
+        <v>44115</v>
       </c>
       <c r="B71" s="2">
-        <v>2554</v>
+        <v>2584</v>
       </c>
       <c r="C71" s="2">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D71" s="2">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="E71" s="2">
-        <v>2926</v>
+        <v>2953</v>
       </c>
       <c r="F71" s="2">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="G71" s="2">
         <v>9</v>
       </c>
       <c r="H71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J71" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
-        <v>44110</v>
+        <v>44114</v>
       </c>
       <c r="B72" s="2">
-        <v>2546</v>
+        <v>2577</v>
       </c>
       <c r="C72" s="2">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D72" s="2">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="E72" s="2">
-        <v>2920</v>
+        <v>2953</v>
       </c>
       <c r="F72" s="2">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="G72" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J72" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
-        <v>44109</v>
+        <v>44113</v>
       </c>
       <c r="B73" s="2">
-        <v>2540</v>
+        <v>2572</v>
       </c>
       <c r="C73" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D73" s="2">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="E73" s="2">
-        <v>2910</v>
+        <v>2945</v>
       </c>
       <c r="F73" s="2">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="G73" s="2">
         <v>10</v>
       </c>
       <c r="H73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J73" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
-        <v>44108</v>
+        <v>44112</v>
       </c>
       <c r="B74" s="2">
-        <v>2537</v>
+        <v>2561</v>
       </c>
       <c r="C74" s="2">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D74" s="2">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="E74" s="2">
-        <v>2901</v>
+        <v>2944</v>
       </c>
       <c r="F74" s="2">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="G74" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" s="2">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J74" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
-        <v>44107</v>
+        <v>44111</v>
       </c>
       <c r="B75" s="2">
-        <v>2522</v>
+        <v>2554</v>
       </c>
       <c r="C75" s="2">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D75" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E75" s="2">
-        <v>2898</v>
+        <v>2926</v>
       </c>
       <c r="F75" s="2">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="G75" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H75" s="2">
         <v>1</v>
       </c>
       <c r="I75" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J75" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
-        <v>44106</v>
+        <v>44110</v>
       </c>
       <c r="B76" s="2">
-        <v>2520</v>
+        <v>2546</v>
       </c>
       <c r="C76" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D76" s="2">
         <v>353</v>
       </c>
       <c r="E76" s="2">
-        <v>2895</v>
+        <v>2920</v>
       </c>
       <c r="F76" s="2">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="G76" s="2">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H76" s="2">
         <v>1</v>
       </c>
       <c r="I76" s="2">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J76" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
-        <v>44105</v>
+        <v>44109</v>
       </c>
       <c r="B77" s="2">
-        <v>2516</v>
+        <v>2540</v>
       </c>
       <c r="C77" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D77" s="2">
         <v>353</v>
       </c>
       <c r="E77" s="2">
-        <v>2885</v>
+        <v>2910</v>
       </c>
       <c r="F77" s="2">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="G77" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H77" s="2">
         <v>1</v>
       </c>
       <c r="I77" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J77" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
-        <v>44104</v>
+        <v>44108</v>
       </c>
       <c r="B78" s="2">
-        <v>2479</v>
+        <v>2537</v>
       </c>
       <c r="C78" s="2">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D78" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E78" s="2">
-        <v>2873</v>
+        <v>2901</v>
       </c>
       <c r="F78" s="2">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="G78" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H78" s="2">
         <v>1</v>
       </c>
       <c r="I78" s="2">
+        <v>11</v>
+      </c>
+      <c r="J78" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1">
+        <v>44107</v>
+      </c>
+      <c r="B79" s="2">
+        <v>2522</v>
+      </c>
+      <c r="C79" s="2">
+        <v>23</v>
+      </c>
+      <c r="D79" s="2">
+        <v>353</v>
+      </c>
+      <c r="E79" s="2">
+        <v>2898</v>
+      </c>
+      <c r="F79" s="2">
+        <v>331</v>
+      </c>
+      <c r="G79" s="2">
         <v>13</v>
       </c>
-      <c r="J78" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>44103</v>
-      </c>
-      <c r="B79" s="2">
-        <v>2483</v>
-      </c>
-      <c r="C79" s="2">
-        <v>31</v>
-      </c>
-      <c r="D79" s="2">
-        <v>351</v>
-      </c>
-      <c r="E79" s="2">
-        <v>2865</v>
-      </c>
-      <c r="F79" s="2">
-        <v>329</v>
-      </c>
-      <c r="G79" s="2">
-        <v>14</v>
-      </c>
       <c r="H79" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I79" s="2">
         <v>12</v>
       </c>
       <c r="J79" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
-        <v>44102</v>
+        <v>44106</v>
       </c>
       <c r="B80" s="2">
-        <v>2466</v>
+        <v>2520</v>
       </c>
       <c r="C80" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D80" s="2">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="E80" s="2">
-        <v>2841</v>
+        <v>2895</v>
       </c>
       <c r="F80" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="G80" s="2">
+        <v>14</v>
+      </c>
+      <c r="H80" s="2">
+        <v>1</v>
+      </c>
+      <c r="I80" s="2">
         <v>13</v>
       </c>
-      <c r="H80" s="2">
-        <v>2</v>
-      </c>
-      <c r="I80" s="2">
-        <v>11</v>
-      </c>
       <c r="J80" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
-        <v>44101</v>
+        <v>44105</v>
       </c>
       <c r="B81" s="2">
-        <v>2468</v>
+        <v>2516</v>
       </c>
       <c r="C81" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D81" s="2">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="E81" s="2">
-        <v>2830</v>
+        <v>2885</v>
       </c>
       <c r="F81" s="2">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="G81" s="2">
         <v>14</v>
       </c>
       <c r="H81" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I81" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J81" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
-        <v>44100</v>
+        <v>44104</v>
       </c>
       <c r="B82" s="2">
-        <v>2424</v>
+        <v>2479</v>
       </c>
       <c r="C82" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D82" s="2">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="E82" s="2">
-        <v>2791</v>
+        <v>2873</v>
       </c>
       <c r="F82" s="2">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="G82" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H82" s="2">
         <v>1</v>
       </c>
       <c r="I82" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J82" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
-        <v>44099</v>
+        <v>44103</v>
       </c>
       <c r="B83" s="2">
-        <v>2424</v>
+        <v>2483</v>
       </c>
       <c r="C83" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D83" s="2">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="E83" s="2">
-        <v>2791</v>
+        <v>2865</v>
       </c>
       <c r="F83" s="2">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="G83" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H83" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I83" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J83" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
-        <v>44098</v>
+        <v>44102</v>
       </c>
       <c r="B84" s="2">
-        <v>2420</v>
+        <v>2466</v>
       </c>
       <c r="C84" s="2">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D84" s="2">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="E84" s="2">
-        <v>2791</v>
+        <v>2841</v>
       </c>
       <c r="F84" s="2">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G84" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H84" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I84" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J84" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
-        <v>44097</v>
+        <v>44101</v>
       </c>
       <c r="B85" s="2">
-        <v>2406</v>
+        <v>2468</v>
       </c>
       <c r="C85" s="2">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D85" s="2">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="E85" s="2">
-        <v>2769</v>
+        <v>2830</v>
       </c>
       <c r="F85" s="2">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="G85" s="2">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H85" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I85" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J85" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
-        <v>44096</v>
+        <v>44100</v>
       </c>
       <c r="B86" s="2">
-        <v>2400</v>
+        <v>2424</v>
       </c>
       <c r="C86" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D86" s="2">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="E86" s="2">
-        <v>2762</v>
+        <v>2791</v>
       </c>
       <c r="F86" s="2">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="G86" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H86" s="2">
         <v>1</v>
       </c>
       <c r="I86" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J86" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
-        <v>44095</v>
+        <v>44099</v>
       </c>
       <c r="B87" s="2">
-        <v>2399</v>
+        <v>2424</v>
       </c>
       <c r="C87" s="2">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D87" s="2">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="E87" s="2">
-        <v>2748</v>
+        <v>2791</v>
       </c>
       <c r="F87" s="2">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G87" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H87" s="2">
         <v>1</v>
       </c>
       <c r="I87" s="2">
+        <v>7</v>
+      </c>
+      <c r="J87" s="2">
         <v>8</v>
       </c>
-      <c r="J87" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
-        <v>44094</v>
+        <v>44098</v>
       </c>
       <c r="B88" s="2">
-        <v>2385</v>
+        <v>2420</v>
       </c>
       <c r="C88" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D88" s="2">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E88" s="2">
-        <v>2742</v>
+        <v>2791</v>
       </c>
       <c r="F88" s="2">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G88" s="2">
         <v>8</v>
       </c>
       <c r="H88" s="2">
+        <v>0</v>
+      </c>
+      <c r="I88" s="2">
+        <v>8</v>
+      </c>
+      <c r="J88" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="1">
+        <v>44097</v>
+      </c>
+      <c r="B89" s="2">
+        <v>2406</v>
+      </c>
+      <c r="C89" s="2">
+        <v>25</v>
+      </c>
+      <c r="D89" s="2">
+        <v>338</v>
+      </c>
+      <c r="E89" s="2">
+        <v>2769</v>
+      </c>
+      <c r="F89" s="2">
+        <v>323</v>
+      </c>
+      <c r="G89" s="2">
+        <v>7</v>
+      </c>
+      <c r="H89" s="2">
+        <v>0</v>
+      </c>
+      <c r="I89" s="2">
+        <v>7</v>
+      </c>
+      <c r="J89" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="1">
+        <v>44096</v>
+      </c>
+      <c r="B90" s="2">
+        <v>2400</v>
+      </c>
+      <c r="C90" s="2">
+        <v>24</v>
+      </c>
+      <c r="D90" s="2">
+        <v>338</v>
+      </c>
+      <c r="E90" s="2">
+        <v>2762</v>
+      </c>
+      <c r="F90" s="2">
+        <v>338</v>
+      </c>
+      <c r="G90" s="2">
+        <v>8</v>
+      </c>
+      <c r="H90" s="2">
         <v>1</v>
       </c>
-      <c r="I88" s="2">
+      <c r="I90" s="2">
         <v>7</v>
       </c>
-      <c r="J88" s="2">
+      <c r="J90" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+    <row r="91" spans="1:10">
+      <c r="A91" s="1">
+        <v>44095</v>
+      </c>
+      <c r="B91" s="2">
+        <v>2399</v>
+      </c>
+      <c r="C91" s="2">
+        <v>11</v>
+      </c>
+      <c r="D91" s="2">
+        <v>338</v>
+      </c>
+      <c r="E91" s="2">
+        <v>2748</v>
+      </c>
+      <c r="F91" s="2">
+        <v>322</v>
+      </c>
+      <c r="G91" s="2">
+        <v>9</v>
+      </c>
+      <c r="H91" s="2">
+        <v>1</v>
+      </c>
+      <c r="I91" s="2">
+        <v>8</v>
+      </c>
+      <c r="J91" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="1">
+        <v>44094</v>
+      </c>
+      <c r="B92" s="2">
+        <v>2385</v>
+      </c>
+      <c r="C92" s="2">
+        <v>20</v>
+      </c>
+      <c r="D92" s="2">
+        <v>337</v>
+      </c>
+      <c r="E92" s="2">
+        <v>2742</v>
+      </c>
+      <c r="F92" s="2">
+        <v>322</v>
+      </c>
+      <c r="G92" s="2">
+        <v>8</v>
+      </c>
+      <c r="H92" s="2">
+        <v>1</v>
+      </c>
+      <c r="I92" s="2">
+        <v>7</v>
+      </c>
+      <c r="J92" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="1">
         <v>44093</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+    <row r="94" spans="1:10">
+      <c r="A94" s="1">
         <v>44092</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+    <row r="95" spans="1:10">
+      <c r="A95" s="1">
         <v>44091</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+    <row r="96" spans="1:10">
+      <c r="A96" s="1">
         <v>44090</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+    <row r="97" spans="1:1">
+      <c r="A97" s="1">
         <v>44089</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+    <row r="98" spans="1:1">
+      <c r="A98" s="1">
         <v>44088</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+    <row r="99" spans="1:1">
+      <c r="A99" s="1">
         <v>44087</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+    <row r="100" spans="1:1">
+      <c r="A100" s="1">
         <v>44086</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+    <row r="101" spans="1:1">
+      <c r="A101" s="1">
         <v>44085</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+    <row r="102" spans="1:1">
+      <c r="A102" s="1">
         <v>44084</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Análise dos dados de 2020
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>DATA</t>
   </si>
@@ -101,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -118,6 +118,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +391,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -400,9 +401,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A184" sqref="A184"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -6289,8 +6290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6980,12 +6981,269 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="6">
+        <v>43983</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="6">
+        <v>43982</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="6">
+        <v>43981</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="6">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="6">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="6">
+        <v>43978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="6">
+        <v>43977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="6">
+        <v>43976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="6">
+        <v>43975</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="6">
+        <v>43974</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="6">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="6">
+        <v>43972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="6">
+        <v>43971</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="6">
+        <v>43970</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="6">
+        <v>43969</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="6">
+        <v>43968</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="6">
+        <v>43967</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="6">
+        <v>43966</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="6">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="6">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="6">
+        <v>43963</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="6">
+        <v>43962</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="6">
+        <v>43961</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="6">
+        <v>43960</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="6">
+        <v>43959</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="6">
+        <v>43958</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="6">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="6">
+        <v>43956</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="6">
+        <v>43955</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="6">
+        <v>43954</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="6">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="6">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="6">
+        <v>43951</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="6">
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="6">
+        <v>43949</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="6">
+        <v>43948</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="6">
+        <v>43947</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="6">
+        <v>43946</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="6">
+        <v>43945</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="6">
+        <v>43944</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="6">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="6">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="6">
+        <v>43941</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="6">
+        <v>43940</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="6">
+        <v>43939</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="6">
+        <v>43938</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="6">
+        <v>43937</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="6">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="6"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add data until January 25th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -214,7 +219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -391,37 +396,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J183"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -485,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -517,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -549,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -581,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -613,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -645,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -677,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -709,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -741,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -773,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -805,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -837,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -869,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -901,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -933,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -965,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -997,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1029,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1093,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1125,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1157,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1221,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1253,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1285,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1317,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1349,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1413,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1445,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1477,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1509,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1541,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1573,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1605,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1637,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1669,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1701,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1733,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1765,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1829,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1861,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1893,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1925,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1957,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1989,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2021,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2053,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2085,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2117,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2149,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2181,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2213,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2245,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2277,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2309,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2341,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2373,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2405,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2437,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2469,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2501,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2533,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2565,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2597,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2629,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2661,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2693,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2725,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2757,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2789,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2821,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2853,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2885,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2917,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2949,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2981,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3013,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3045,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3077,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3109,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3141,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3173,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3205,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3237,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3269,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3301,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3333,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3365,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3397,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3429,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3461,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3493,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3525,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3557,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3589,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3621,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3653,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3685,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3717,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3749,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3781,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3813,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3845,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3877,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3909,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3941,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3973,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4005,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4037,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4069,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4101,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4133,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4165,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4197,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4229,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4261,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4293,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4325,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4357,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4389,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4421,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4453,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4485,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4517,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4549,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4581,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4613,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4645,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4709,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4741,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4773,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4805,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4837,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4869,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4901,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4933,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4965,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -4997,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5029,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5061,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5093,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5125,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5157,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5189,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5221,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5253,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5285,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5317,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5349,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5381,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5413,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5445,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5477,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5509,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5541,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5573,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5605,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5637,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5669,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5701,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5733,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5765,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5797,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5829,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5861,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5893,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5925,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5957,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5989,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6021,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6053,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6085,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6117,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6149,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6181,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6213,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6245,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6275,6 +6280,806 @@
       </c>
       <c r="J183" s="2">
         <v>19</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B184" s="2">
+        <v>4445</v>
+      </c>
+      <c r="C184" s="2">
+        <v>47</v>
+      </c>
+      <c r="D184" s="2">
+        <v>874</v>
+      </c>
+      <c r="E184" s="2">
+        <v>5366</v>
+      </c>
+      <c r="F184" s="2">
+        <v>807</v>
+      </c>
+      <c r="G184" s="2">
+        <v>48</v>
+      </c>
+      <c r="H184" s="2">
+        <v>2</v>
+      </c>
+      <c r="I184" s="2">
+        <v>46</v>
+      </c>
+      <c r="J184" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>44198</v>
+      </c>
+      <c r="B185" s="2">
+        <v>4466</v>
+      </c>
+      <c r="C185" s="2">
+        <v>32</v>
+      </c>
+      <c r="D185" s="2">
+        <v>877</v>
+      </c>
+      <c r="E185" s="2">
+        <v>5375</v>
+      </c>
+      <c r="F185" s="2">
+        <v>811</v>
+      </c>
+      <c r="G185" s="2">
+        <v>47</v>
+      </c>
+      <c r="H185" s="2">
+        <v>2</v>
+      </c>
+      <c r="I185" s="2">
+        <v>45</v>
+      </c>
+      <c r="J185" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>44199</v>
+      </c>
+      <c r="B186" s="2">
+        <v>4467</v>
+      </c>
+      <c r="C186" s="2">
+        <v>31</v>
+      </c>
+      <c r="D186" s="2">
+        <v>878</v>
+      </c>
+      <c r="E186" s="2">
+        <v>5376</v>
+      </c>
+      <c r="F186" s="2">
+        <v>814</v>
+      </c>
+      <c r="G186" s="2">
+        <v>45</v>
+      </c>
+      <c r="H186" s="2">
+        <v>2</v>
+      </c>
+      <c r="I186" s="2">
+        <v>43</v>
+      </c>
+      <c r="J186" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B187" s="2">
+        <v>4467</v>
+      </c>
+      <c r="C187" s="2">
+        <v>43</v>
+      </c>
+      <c r="D187" s="2">
+        <v>878</v>
+      </c>
+      <c r="E187" s="2">
+        <v>5388</v>
+      </c>
+      <c r="F187" s="2">
+        <v>816</v>
+      </c>
+      <c r="G187" s="2">
+        <v>41</v>
+      </c>
+      <c r="H187" s="2">
+        <v>2</v>
+      </c>
+      <c r="I187" s="2">
+        <v>39</v>
+      </c>
+      <c r="J187" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>44201</v>
+      </c>
+      <c r="B188" s="2">
+        <v>4471</v>
+      </c>
+      <c r="C188" s="2">
+        <v>113</v>
+      </c>
+      <c r="D188" s="2">
+        <v>879</v>
+      </c>
+      <c r="E188" s="2">
+        <v>5463</v>
+      </c>
+      <c r="F188" s="2">
+        <v>818</v>
+      </c>
+      <c r="G188" s="2">
+        <v>40</v>
+      </c>
+      <c r="H188" s="2">
+        <v>2</v>
+      </c>
+      <c r="I188" s="2">
+        <v>38</v>
+      </c>
+      <c r="J188" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>44202</v>
+      </c>
+      <c r="B189" s="2">
+        <v>4471</v>
+      </c>
+      <c r="C189" s="2">
+        <v>134</v>
+      </c>
+      <c r="D189" s="2">
+        <v>882</v>
+      </c>
+      <c r="E189" s="2">
+        <v>5487</v>
+      </c>
+      <c r="F189" s="2">
+        <v>822</v>
+      </c>
+      <c r="G189" s="2">
+        <v>39</v>
+      </c>
+      <c r="H189" s="2">
+        <v>2</v>
+      </c>
+      <c r="I189" s="2">
+        <v>37</v>
+      </c>
+      <c r="J189" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>44203</v>
+      </c>
+      <c r="B190" s="2">
+        <v>4527</v>
+      </c>
+      <c r="C190" s="2">
+        <v>103</v>
+      </c>
+      <c r="D190" s="2">
+        <v>902</v>
+      </c>
+      <c r="E190" s="2">
+        <v>5532</v>
+      </c>
+      <c r="F190" s="2">
+        <v>828</v>
+      </c>
+      <c r="G190" s="2">
+        <v>52</v>
+      </c>
+      <c r="H190" s="2">
+        <v>2</v>
+      </c>
+      <c r="I190" s="2">
+        <v>50</v>
+      </c>
+      <c r="J190" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>44204</v>
+      </c>
+      <c r="B191" s="2">
+        <v>4537</v>
+      </c>
+      <c r="C191" s="2">
+        <v>138</v>
+      </c>
+      <c r="D191" s="2">
+        <v>905</v>
+      </c>
+      <c r="E191" s="2">
+        <v>5580</v>
+      </c>
+      <c r="F191" s="2">
+        <v>831</v>
+      </c>
+      <c r="G191" s="2">
+        <v>52</v>
+      </c>
+      <c r="H191" s="2">
+        <v>2</v>
+      </c>
+      <c r="I191" s="2">
+        <v>50</v>
+      </c>
+      <c r="J191" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>44205</v>
+      </c>
+      <c r="B192" s="2">
+        <v>4591</v>
+      </c>
+      <c r="C192" s="2">
+        <v>115</v>
+      </c>
+      <c r="D192" s="2">
+        <v>932</v>
+      </c>
+      <c r="E192" s="2">
+        <v>5638</v>
+      </c>
+      <c r="F192" s="2">
+        <v>838</v>
+      </c>
+      <c r="G192" s="2">
+        <v>72</v>
+      </c>
+      <c r="H192" s="2">
+        <v>3</v>
+      </c>
+      <c r="I192" s="2">
+        <v>69</v>
+      </c>
+      <c r="J192" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>44206</v>
+      </c>
+      <c r="B193" s="2">
+        <v>4591</v>
+      </c>
+      <c r="C193" s="2">
+        <v>120</v>
+      </c>
+      <c r="D193" s="2">
+        <v>932</v>
+      </c>
+      <c r="E193" s="2">
+        <v>5643</v>
+      </c>
+      <c r="F193" s="2">
+        <v>843</v>
+      </c>
+      <c r="G193" s="2">
+        <v>67</v>
+      </c>
+      <c r="H193" s="2">
+        <v>4</v>
+      </c>
+      <c r="I193" s="2">
+        <v>63</v>
+      </c>
+      <c r="J193" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>44207</v>
+      </c>
+      <c r="B194" s="2">
+        <v>4608</v>
+      </c>
+      <c r="C194" s="2">
+        <v>137</v>
+      </c>
+      <c r="D194" s="2">
+        <v>938</v>
+      </c>
+      <c r="E194" s="2">
+        <v>5683</v>
+      </c>
+      <c r="F194" s="2">
+        <v>860</v>
+      </c>
+      <c r="G194" s="2">
+        <v>56</v>
+      </c>
+      <c r="H194" s="2">
+        <v>5</v>
+      </c>
+      <c r="I194" s="2">
+        <v>51</v>
+      </c>
+      <c r="J194" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>44208</v>
+      </c>
+      <c r="B195" s="2">
+        <v>4616</v>
+      </c>
+      <c r="C195" s="2">
+        <v>172</v>
+      </c>
+      <c r="D195" s="2">
+        <v>941</v>
+      </c>
+      <c r="E195" s="2">
+        <v>5729</v>
+      </c>
+      <c r="F195" s="2">
+        <v>865</v>
+      </c>
+      <c r="G195" s="2">
+        <v>54</v>
+      </c>
+      <c r="H195" s="2">
+        <v>5</v>
+      </c>
+      <c r="I195" s="2">
+        <v>49</v>
+      </c>
+      <c r="J195" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>44209</v>
+      </c>
+      <c r="B196" s="2">
+        <v>4660</v>
+      </c>
+      <c r="C196" s="2">
+        <v>160</v>
+      </c>
+      <c r="D196" s="2">
+        <v>961</v>
+      </c>
+      <c r="E196" s="2">
+        <v>5781</v>
+      </c>
+      <c r="F196" s="2">
+        <v>870</v>
+      </c>
+      <c r="G196" s="2">
+        <v>69</v>
+      </c>
+      <c r="H196" s="2">
+        <v>5</v>
+      </c>
+      <c r="I196" s="2">
+        <v>64</v>
+      </c>
+      <c r="J196" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>44210</v>
+      </c>
+      <c r="B197" s="2">
+        <v>4733</v>
+      </c>
+      <c r="C197" s="2">
+        <v>120</v>
+      </c>
+      <c r="D197" s="2">
+        <v>973</v>
+      </c>
+      <c r="E197" s="2">
+        <v>5826</v>
+      </c>
+      <c r="F197" s="2">
+        <v>876</v>
+      </c>
+      <c r="G197" s="2">
+        <v>75</v>
+      </c>
+      <c r="H197" s="2">
+        <v>5</v>
+      </c>
+      <c r="I197" s="2">
+        <v>70</v>
+      </c>
+      <c r="J197" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>44211</v>
+      </c>
+      <c r="B198" s="2">
+        <v>4768</v>
+      </c>
+      <c r="C198" s="2">
+        <v>88</v>
+      </c>
+      <c r="D198" s="2">
+        <v>993</v>
+      </c>
+      <c r="E198" s="2">
+        <v>5849</v>
+      </c>
+      <c r="F198" s="2">
+        <v>884</v>
+      </c>
+      <c r="G198" s="2">
+        <v>86</v>
+      </c>
+      <c r="H198" s="2">
+        <v>5</v>
+      </c>
+      <c r="I198" s="2">
+        <v>81</v>
+      </c>
+      <c r="J198" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>44212</v>
+      </c>
+      <c r="B199" s="2">
+        <v>4789</v>
+      </c>
+      <c r="C199" s="2">
+        <v>92</v>
+      </c>
+      <c r="D199" s="2">
+        <v>1002</v>
+      </c>
+      <c r="E199" s="2">
+        <v>5883</v>
+      </c>
+      <c r="F199" s="2">
+        <v>886</v>
+      </c>
+      <c r="G199" s="2">
+        <v>93</v>
+      </c>
+      <c r="H199" s="2">
+        <v>5</v>
+      </c>
+      <c r="I199" s="2">
+        <v>88</v>
+      </c>
+      <c r="J199" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>44213</v>
+      </c>
+      <c r="B200" s="2">
+        <v>4792</v>
+      </c>
+      <c r="C200" s="2">
+        <v>98</v>
+      </c>
+      <c r="D200" s="2">
+        <v>1002</v>
+      </c>
+      <c r="E200" s="2">
+        <v>5892</v>
+      </c>
+      <c r="F200" s="2">
+        <v>889</v>
+      </c>
+      <c r="G200" s="2">
+        <v>90</v>
+      </c>
+      <c r="H200" s="2">
+        <v>5</v>
+      </c>
+      <c r="I200" s="2">
+        <v>85</v>
+      </c>
+      <c r="J200" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B201" s="2">
+        <v>4824</v>
+      </c>
+      <c r="C201" s="2">
+        <v>81</v>
+      </c>
+      <c r="D201" s="2">
+        <v>1011</v>
+      </c>
+      <c r="E201" s="2">
+        <v>5916</v>
+      </c>
+      <c r="F201" s="2">
+        <v>900</v>
+      </c>
+      <c r="G201" s="2">
+        <v>88</v>
+      </c>
+      <c r="H201" s="2">
+        <v>3</v>
+      </c>
+      <c r="I201" s="2">
+        <v>85</v>
+      </c>
+      <c r="J201" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>44215</v>
+      </c>
+      <c r="B202" s="2">
+        <v>4837</v>
+      </c>
+      <c r="C202" s="2">
+        <v>120</v>
+      </c>
+      <c r="D202" s="2">
+        <v>1022</v>
+      </c>
+      <c r="E202" s="2">
+        <v>5979</v>
+      </c>
+      <c r="F202" s="2">
+        <v>912</v>
+      </c>
+      <c r="G202" s="2">
+        <v>87</v>
+      </c>
+      <c r="H202" s="2">
+        <v>3</v>
+      </c>
+      <c r="I202" s="2">
+        <v>84</v>
+      </c>
+      <c r="J202" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>44216</v>
+      </c>
+      <c r="B203" s="2">
+        <v>4868</v>
+      </c>
+      <c r="C203" s="2">
+        <v>120</v>
+      </c>
+      <c r="D203" s="2">
+        <v>1034</v>
+      </c>
+      <c r="E203" s="2">
+        <v>6022</v>
+      </c>
+      <c r="F203" s="2">
+        <v>925</v>
+      </c>
+      <c r="G203" s="2">
+        <v>86</v>
+      </c>
+      <c r="H203" s="2">
+        <v>4</v>
+      </c>
+      <c r="I203" s="2">
+        <v>82</v>
+      </c>
+      <c r="J203" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>44217</v>
+      </c>
+      <c r="B204" s="2">
+        <v>4903</v>
+      </c>
+      <c r="C204" s="2">
+        <v>112</v>
+      </c>
+      <c r="D204" s="2">
+        <v>1050</v>
+      </c>
+      <c r="E204" s="2">
+        <v>6065</v>
+      </c>
+      <c r="F204" s="2">
+        <v>932</v>
+      </c>
+      <c r="G204" s="2">
+        <v>95</v>
+      </c>
+      <c r="H204" s="2">
+        <v>4</v>
+      </c>
+      <c r="I204" s="2">
+        <v>91</v>
+      </c>
+      <c r="J204" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>44218</v>
+      </c>
+      <c r="B205" s="2">
+        <v>4937</v>
+      </c>
+      <c r="C205" s="2">
+        <v>104</v>
+      </c>
+      <c r="D205" s="2">
+        <v>1068</v>
+      </c>
+      <c r="E205" s="2">
+        <v>6109</v>
+      </c>
+      <c r="F205" s="2">
+        <v>946</v>
+      </c>
+      <c r="G205" s="2">
+        <v>99</v>
+      </c>
+      <c r="H205" s="2">
+        <v>4</v>
+      </c>
+      <c r="I205" s="2">
+        <v>95</v>
+      </c>
+      <c r="J205" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>44219</v>
+      </c>
+      <c r="B206" s="2">
+        <v>4991</v>
+      </c>
+      <c r="C206" s="2">
+        <v>93</v>
+      </c>
+      <c r="D206" s="2">
+        <v>1080</v>
+      </c>
+      <c r="E206" s="2">
+        <v>6164</v>
+      </c>
+      <c r="F206" s="2">
+        <v>952</v>
+      </c>
+      <c r="G206" s="2">
+        <v>105</v>
+      </c>
+      <c r="H206" s="2">
+        <v>5</v>
+      </c>
+      <c r="I206" s="2">
+        <v>100</v>
+      </c>
+      <c r="J206" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>44220</v>
+      </c>
+      <c r="B207" s="2">
+        <v>5014</v>
+      </c>
+      <c r="C207" s="2">
+        <v>62</v>
+      </c>
+      <c r="D207" s="2">
+        <v>1090</v>
+      </c>
+      <c r="E207" s="2">
+        <v>6166</v>
+      </c>
+      <c r="F207" s="2">
+        <v>957</v>
+      </c>
+      <c r="G207" s="2">
+        <v>110</v>
+      </c>
+      <c r="H207" s="2">
+        <v>5</v>
+      </c>
+      <c r="I207" s="2">
+        <v>105</v>
+      </c>
+      <c r="J207" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>44221</v>
+      </c>
+      <c r="B208" s="2">
+        <v>5017</v>
+      </c>
+      <c r="C208" s="2">
+        <v>93</v>
+      </c>
+      <c r="D208" s="2">
+        <v>1091</v>
+      </c>
+      <c r="E208" s="2">
+        <v>6201</v>
+      </c>
+      <c r="F208" s="2">
+        <v>968</v>
+      </c>
+      <c r="G208" s="2">
+        <v>100</v>
+      </c>
+      <c r="H208" s="2">
+        <v>5</v>
+      </c>
+      <c r="I208" s="2">
+        <v>95</v>
+      </c>
+      <c r="J208" s="2">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -6287,29 +7092,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6344,7 +7149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -6367,7 +7172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -6390,7 +7195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -6413,7 +7218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -6436,7 +7241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -6459,7 +7264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -6482,7 +7287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -6502,7 +7307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -6522,7 +7327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -6542,7 +7347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -6562,7 +7367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -6582,12 +7387,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -6607,7 +7412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -6627,7 +7432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -6647,7 +7452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -6667,7 +7472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -6687,7 +7492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -6707,7 +7512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -6727,7 +7532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -6747,7 +7552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -6767,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -6775,7 +7580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -6798,7 +7603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -6818,7 +7623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -6838,7 +7643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -6858,17 +7663,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -6888,7 +7693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -6911,7 +7716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -6934,7 +7739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -6954,7 +7759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -6980,267 +7785,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until March 2nd
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -219,7 +214,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -396,37 +391,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J208"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B245" sqref="B245"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1957,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +4997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6245,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6277,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6309,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6373,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6469,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7080,6 +7075,1158 @@
       </c>
       <c r="J208" s="2">
         <v>23</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10">
+      <c r="A209" s="1">
+        <v>44222</v>
+      </c>
+      <c r="B209" s="2">
+        <v>5029</v>
+      </c>
+      <c r="C209" s="2">
+        <v>119</v>
+      </c>
+      <c r="D209" s="2">
+        <v>1096</v>
+      </c>
+      <c r="E209" s="2">
+        <v>6244</v>
+      </c>
+      <c r="F209" s="2">
+        <v>984</v>
+      </c>
+      <c r="G209" s="2">
+        <v>89</v>
+      </c>
+      <c r="H209" s="2">
+        <v>5</v>
+      </c>
+      <c r="I209" s="2">
+        <v>84</v>
+      </c>
+      <c r="J209" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10">
+      <c r="A210" s="1">
+        <v>44223</v>
+      </c>
+      <c r="B210" s="2">
+        <v>5039</v>
+      </c>
+      <c r="C210" s="2">
+        <v>130</v>
+      </c>
+      <c r="D210" s="2">
+        <v>1103</v>
+      </c>
+      <c r="E210" s="2">
+        <v>6272</v>
+      </c>
+      <c r="F210" s="2">
+        <v>994</v>
+      </c>
+      <c r="G210" s="2">
+        <v>86</v>
+      </c>
+      <c r="H210" s="2">
+        <v>5</v>
+      </c>
+      <c r="I210" s="2">
+        <v>81</v>
+      </c>
+      <c r="J210" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10">
+      <c r="A211" s="1">
+        <v>44224</v>
+      </c>
+      <c r="B211" s="2">
+        <v>5097</v>
+      </c>
+      <c r="C211" s="2">
+        <v>141</v>
+      </c>
+      <c r="D211" s="2">
+        <v>1130</v>
+      </c>
+      <c r="E211" s="2">
+        <v>6368</v>
+      </c>
+      <c r="F211" s="2">
+        <v>1004</v>
+      </c>
+      <c r="G211" s="2">
+        <v>103</v>
+      </c>
+      <c r="H211" s="2">
+        <v>5</v>
+      </c>
+      <c r="I211" s="2">
+        <v>98</v>
+      </c>
+      <c r="J211" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10">
+      <c r="A212" s="1">
+        <v>44225</v>
+      </c>
+      <c r="B212" s="2">
+        <v>5145</v>
+      </c>
+      <c r="C212" s="2">
+        <v>112</v>
+      </c>
+      <c r="D212" s="2">
+        <v>1142</v>
+      </c>
+      <c r="E212" s="2">
+        <v>6399</v>
+      </c>
+      <c r="F212" s="2">
+        <v>1012</v>
+      </c>
+      <c r="G212" s="2">
+        <v>107</v>
+      </c>
+      <c r="H212" s="2">
+        <v>5</v>
+      </c>
+      <c r="I212" s="2">
+        <v>102</v>
+      </c>
+      <c r="J212" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10">
+      <c r="A213" s="1">
+        <v>44226</v>
+      </c>
+      <c r="B213" s="2">
+        <v>5172</v>
+      </c>
+      <c r="C213" s="2">
+        <v>95</v>
+      </c>
+      <c r="D213" s="2">
+        <v>1146</v>
+      </c>
+      <c r="E213" s="2">
+        <v>6413</v>
+      </c>
+      <c r="F213" s="2">
+        <v>1019</v>
+      </c>
+      <c r="G213" s="2">
+        <v>103</v>
+      </c>
+      <c r="H213" s="2">
+        <v>6</v>
+      </c>
+      <c r="I213" s="2">
+        <v>97</v>
+      </c>
+      <c r="J213" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10">
+      <c r="A214" s="1">
+        <v>44227</v>
+      </c>
+      <c r="B214" s="2">
+        <v>5189</v>
+      </c>
+      <c r="C214" s="2">
+        <v>83</v>
+      </c>
+      <c r="D214" s="2">
+        <v>1147</v>
+      </c>
+      <c r="E214" s="2">
+        <v>6419</v>
+      </c>
+      <c r="F214" s="2">
+        <v>1030</v>
+      </c>
+      <c r="G214" s="2">
+        <v>92</v>
+      </c>
+      <c r="H214" s="2">
+        <v>6</v>
+      </c>
+      <c r="I214" s="2">
+        <v>86</v>
+      </c>
+      <c r="J214" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10">
+      <c r="A215" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B215" s="2">
+        <v>5203</v>
+      </c>
+      <c r="C215" s="2">
+        <v>109</v>
+      </c>
+      <c r="D215" s="2">
+        <v>1149</v>
+      </c>
+      <c r="E215" s="2">
+        <v>6461</v>
+      </c>
+      <c r="F215" s="2">
+        <v>1044</v>
+      </c>
+      <c r="G215" s="2">
+        <v>79</v>
+      </c>
+      <c r="H215" s="2">
+        <v>7</v>
+      </c>
+      <c r="I215" s="2">
+        <v>72</v>
+      </c>
+      <c r="J215" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10">
+      <c r="A216" s="1">
+        <v>44229</v>
+      </c>
+      <c r="B216" s="2">
+        <v>5212</v>
+      </c>
+      <c r="C216" s="2">
+        <v>144</v>
+      </c>
+      <c r="D216" s="2">
+        <v>1154</v>
+      </c>
+      <c r="E216" s="2">
+        <v>6510</v>
+      </c>
+      <c r="F216" s="2">
+        <v>1053</v>
+      </c>
+      <c r="G216" s="2">
+        <v>75</v>
+      </c>
+      <c r="H216" s="2">
+        <v>7</v>
+      </c>
+      <c r="I216" s="2">
+        <v>68</v>
+      </c>
+      <c r="J216" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10">
+      <c r="A217" s="1">
+        <v>44230</v>
+      </c>
+      <c r="B217" s="2">
+        <v>5219</v>
+      </c>
+      <c r="C217" s="2">
+        <v>200</v>
+      </c>
+      <c r="D217" s="2">
+        <v>1160</v>
+      </c>
+      <c r="E217" s="2">
+        <v>6579</v>
+      </c>
+      <c r="F217" s="2">
+        <v>1066</v>
+      </c>
+      <c r="G217" s="2">
+        <v>68</v>
+      </c>
+      <c r="H217" s="2">
+        <v>8</v>
+      </c>
+      <c r="I217" s="2">
+        <v>60</v>
+      </c>
+      <c r="J217" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10">
+      <c r="A218" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B218" s="2">
+        <v>5235</v>
+      </c>
+      <c r="C218" s="2">
+        <v>206</v>
+      </c>
+      <c r="D218" s="2">
+        <v>1163</v>
+      </c>
+      <c r="E218" s="2">
+        <v>6604</v>
+      </c>
+      <c r="F218" s="2">
+        <v>1076</v>
+      </c>
+      <c r="G218" s="2">
+        <v>60</v>
+      </c>
+      <c r="H218" s="2">
+        <v>9</v>
+      </c>
+      <c r="I218" s="2">
+        <v>51</v>
+      </c>
+      <c r="J218" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10">
+      <c r="A219" s="1">
+        <v>44232</v>
+      </c>
+      <c r="B219" s="2">
+        <v>5313</v>
+      </c>
+      <c r="C219" s="2">
+        <v>130</v>
+      </c>
+      <c r="D219" s="2">
+        <v>1196</v>
+      </c>
+      <c r="E219" s="2">
+        <v>6639</v>
+      </c>
+      <c r="F219" s="2">
+        <v>1090</v>
+      </c>
+      <c r="G219" s="2">
+        <v>79</v>
+      </c>
+      <c r="H219" s="2">
+        <v>12</v>
+      </c>
+      <c r="I219" s="2">
+        <v>67</v>
+      </c>
+      <c r="J219" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10">
+      <c r="A220" s="1">
+        <v>44233</v>
+      </c>
+      <c r="B220" s="2">
+        <v>5322</v>
+      </c>
+      <c r="C220" s="2">
+        <v>118</v>
+      </c>
+      <c r="D220" s="2">
+        <v>1200</v>
+      </c>
+      <c r="E220" s="2">
+        <v>6640</v>
+      </c>
+      <c r="F220" s="2">
+        <v>1096</v>
+      </c>
+      <c r="G220" s="2">
+        <v>77</v>
+      </c>
+      <c r="H220" s="2">
+        <v>12</v>
+      </c>
+      <c r="I220" s="2">
+        <v>65</v>
+      </c>
+      <c r="J220" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10">
+      <c r="A221" s="1">
+        <v>44234</v>
+      </c>
+      <c r="B221" s="2">
+        <v>5325</v>
+      </c>
+      <c r="C221" s="2">
+        <v>120</v>
+      </c>
+      <c r="D221" s="2">
+        <v>1204</v>
+      </c>
+      <c r="E221" s="2">
+        <v>6649</v>
+      </c>
+      <c r="F221" s="2">
+        <v>1099</v>
+      </c>
+      <c r="G221" s="2">
+        <v>77</v>
+      </c>
+      <c r="H221" s="2">
+        <v>11</v>
+      </c>
+      <c r="I221" s="2">
+        <v>66</v>
+      </c>
+      <c r="J221" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10">
+      <c r="A222" s="1">
+        <v>44235</v>
+      </c>
+      <c r="B222" s="2">
+        <v>5380</v>
+      </c>
+      <c r="C222" s="2">
+        <v>98</v>
+      </c>
+      <c r="D222" s="2">
+        <v>1209</v>
+      </c>
+      <c r="E222" s="2">
+        <v>6687</v>
+      </c>
+      <c r="F222" s="2">
+        <v>1112</v>
+      </c>
+      <c r="G222" s="2">
+        <v>69</v>
+      </c>
+      <c r="H222" s="2">
+        <v>11</v>
+      </c>
+      <c r="I222" s="2">
+        <v>58</v>
+      </c>
+      <c r="J222" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10">
+      <c r="A223" s="1">
+        <v>44236</v>
+      </c>
+      <c r="B223" s="2">
+        <v>5397</v>
+      </c>
+      <c r="C223" s="2">
+        <v>116</v>
+      </c>
+      <c r="D223" s="2">
+        <v>1210</v>
+      </c>
+      <c r="E223" s="2">
+        <v>6723</v>
+      </c>
+      <c r="F223" s="2">
+        <v>1118</v>
+      </c>
+      <c r="G223" s="2">
+        <v>64</v>
+      </c>
+      <c r="H223" s="2">
+        <v>12</v>
+      </c>
+      <c r="I223" s="2">
+        <v>52</v>
+      </c>
+      <c r="J223" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10">
+      <c r="A224" s="1">
+        <v>44237</v>
+      </c>
+      <c r="B224" s="2">
+        <v>5438</v>
+      </c>
+      <c r="C224" s="2">
+        <v>104</v>
+      </c>
+      <c r="D224" s="2">
+        <v>1213</v>
+      </c>
+      <c r="E224" s="2">
+        <v>6755</v>
+      </c>
+      <c r="F224" s="2">
+        <v>1126</v>
+      </c>
+      <c r="G224" s="2">
+        <v>59</v>
+      </c>
+      <c r="H224" s="2">
+        <v>11</v>
+      </c>
+      <c r="I224" s="2">
+        <v>48</v>
+      </c>
+      <c r="J224" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10">
+      <c r="A225" s="1">
+        <v>44238</v>
+      </c>
+      <c r="B225" s="2">
+        <v>5482</v>
+      </c>
+      <c r="C225" s="2">
+        <v>114</v>
+      </c>
+      <c r="D225" s="2">
+        <v>1225</v>
+      </c>
+      <c r="E225" s="2">
+        <v>6821</v>
+      </c>
+      <c r="F225" s="2">
+        <v>1128</v>
+      </c>
+      <c r="G225" s="2">
+        <v>68</v>
+      </c>
+      <c r="H225" s="2">
+        <v>10</v>
+      </c>
+      <c r="I225" s="2">
+        <v>58</v>
+      </c>
+      <c r="J225" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10">
+      <c r="A226" s="1">
+        <v>44239</v>
+      </c>
+      <c r="B226" s="2">
+        <v>5501</v>
+      </c>
+      <c r="C226" s="2">
+        <v>126</v>
+      </c>
+      <c r="D226" s="2">
+        <v>1227</v>
+      </c>
+      <c r="E226" s="2">
+        <v>6854</v>
+      </c>
+      <c r="F226" s="2">
+        <v>1135</v>
+      </c>
+      <c r="G226" s="2">
+        <v>63</v>
+      </c>
+      <c r="H226" s="2">
+        <v>10</v>
+      </c>
+      <c r="I226" s="2">
+        <v>53</v>
+      </c>
+      <c r="J226" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10">
+      <c r="A227" s="1">
+        <v>44240</v>
+      </c>
+      <c r="B227" s="2">
+        <v>5529</v>
+      </c>
+      <c r="C227" s="2">
+        <v>113</v>
+      </c>
+      <c r="D227" s="2">
+        <v>1237</v>
+      </c>
+      <c r="E227" s="2">
+        <v>6879</v>
+      </c>
+      <c r="F227" s="2">
+        <v>1148</v>
+      </c>
+      <c r="G227" s="2">
+        <v>59</v>
+      </c>
+      <c r="H227" s="2">
+        <v>11</v>
+      </c>
+      <c r="I227" s="2">
+        <v>48</v>
+      </c>
+      <c r="J227" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10">
+      <c r="A228" s="1">
+        <v>44241</v>
+      </c>
+      <c r="B228" s="2">
+        <v>5531</v>
+      </c>
+      <c r="C228" s="2">
+        <v>117</v>
+      </c>
+      <c r="D228" s="2">
+        <v>1237</v>
+      </c>
+      <c r="E228" s="2">
+        <v>6885</v>
+      </c>
+      <c r="F228" s="2">
+        <v>1151</v>
+      </c>
+      <c r="G228" s="2">
+        <v>55</v>
+      </c>
+      <c r="H228" s="2">
+        <v>10</v>
+      </c>
+      <c r="I228" s="2">
+        <v>45</v>
+      </c>
+      <c r="J228" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10">
+      <c r="A229" s="1">
+        <v>44242</v>
+      </c>
+      <c r="B229" s="2">
+        <v>5555</v>
+      </c>
+      <c r="C229" s="2">
+        <v>88</v>
+      </c>
+      <c r="D229" s="2">
+        <v>1245</v>
+      </c>
+      <c r="E229" s="2">
+        <v>6888</v>
+      </c>
+      <c r="F229" s="2">
+        <v>1157</v>
+      </c>
+      <c r="G229" s="2">
+        <v>57</v>
+      </c>
+      <c r="H229" s="2">
+        <v>8</v>
+      </c>
+      <c r="I229" s="2">
+        <v>49</v>
+      </c>
+      <c r="J229" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10">
+      <c r="A230" s="1">
+        <v>44243</v>
+      </c>
+      <c r="B230" s="2">
+        <v>5557</v>
+      </c>
+      <c r="C230" s="2">
+        <v>108</v>
+      </c>
+      <c r="D230" s="2">
+        <v>1247</v>
+      </c>
+      <c r="E230" s="2">
+        <v>6912</v>
+      </c>
+      <c r="F230" s="2">
+        <v>1160</v>
+      </c>
+      <c r="G230" s="2">
+        <v>56</v>
+      </c>
+      <c r="H230" s="2">
+        <v>7</v>
+      </c>
+      <c r="I230" s="2">
+        <v>49</v>
+      </c>
+      <c r="J230" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10">
+      <c r="A231" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B231" s="2">
+        <v>5575</v>
+      </c>
+      <c r="C231" s="2">
+        <v>110</v>
+      </c>
+      <c r="D231" s="2">
+        <v>1255</v>
+      </c>
+      <c r="E231" s="2">
+        <v>6940</v>
+      </c>
+      <c r="F231" s="2">
+        <v>1166</v>
+      </c>
+      <c r="G231" s="2">
+        <v>58</v>
+      </c>
+      <c r="H231" s="2">
+        <v>8</v>
+      </c>
+      <c r="I231" s="2">
+        <v>50</v>
+      </c>
+      <c r="J231" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10">
+      <c r="A232" s="1">
+        <v>44245</v>
+      </c>
+      <c r="B232" s="2">
+        <v>5592</v>
+      </c>
+      <c r="C232" s="2">
+        <v>120</v>
+      </c>
+      <c r="D232" s="2">
+        <v>1262</v>
+      </c>
+      <c r="E232" s="2">
+        <v>6974</v>
+      </c>
+      <c r="F232" s="2">
+        <v>1167</v>
+      </c>
+      <c r="G232" s="2">
+        <v>64</v>
+      </c>
+      <c r="H232" s="2">
+        <v>8</v>
+      </c>
+      <c r="I232" s="2">
+        <v>56</v>
+      </c>
+      <c r="J232" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10">
+      <c r="A233" s="1">
+        <v>44246</v>
+      </c>
+      <c r="B233" s="2">
+        <v>5608</v>
+      </c>
+      <c r="C233" s="2">
+        <v>146</v>
+      </c>
+      <c r="D233" s="2">
+        <v>1267</v>
+      </c>
+      <c r="E233" s="2">
+        <v>7021</v>
+      </c>
+      <c r="F233" s="2">
+        <v>1176</v>
+      </c>
+      <c r="G233" s="2">
+        <v>60</v>
+      </c>
+      <c r="H233" s="2">
+        <v>8</v>
+      </c>
+      <c r="I233" s="2">
+        <v>52</v>
+      </c>
+      <c r="J233" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10">
+      <c r="A234" s="1">
+        <v>44247</v>
+      </c>
+      <c r="B234" s="2">
+        <v>5633</v>
+      </c>
+      <c r="C234" s="2">
+        <v>158</v>
+      </c>
+      <c r="D234" s="2">
+        <v>1281</v>
+      </c>
+      <c r="E234" s="2">
+        <v>7072</v>
+      </c>
+      <c r="F234" s="2">
+        <v>1178</v>
+      </c>
+      <c r="G234" s="2">
+        <v>72</v>
+      </c>
+      <c r="H234" s="2">
+        <v>8</v>
+      </c>
+      <c r="I234" s="2">
+        <v>64</v>
+      </c>
+      <c r="J234" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10">
+      <c r="A235" s="1">
+        <v>44248</v>
+      </c>
+      <c r="B235" s="2">
+        <v>5682</v>
+      </c>
+      <c r="C235" s="2">
+        <v>88</v>
+      </c>
+      <c r="D235" s="2">
+        <v>1303</v>
+      </c>
+      <c r="E235" s="2">
+        <v>7073</v>
+      </c>
+      <c r="F235" s="2">
+        <v>1180</v>
+      </c>
+      <c r="G235" s="2">
+        <v>92</v>
+      </c>
+      <c r="H235" s="2">
+        <v>8</v>
+      </c>
+      <c r="I235" s="2">
+        <v>84</v>
+      </c>
+      <c r="J235" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10">
+      <c r="A236" s="1">
+        <v>44249</v>
+      </c>
+      <c r="B236" s="2">
+        <v>5695</v>
+      </c>
+      <c r="C236" s="2">
+        <v>88</v>
+      </c>
+      <c r="D236" s="2">
+        <v>1304</v>
+      </c>
+      <c r="E236" s="2">
+        <v>7087</v>
+      </c>
+      <c r="F236" s="2">
+        <v>1183</v>
+      </c>
+      <c r="G236" s="2">
+        <v>90</v>
+      </c>
+      <c r="H236" s="2">
+        <v>7</v>
+      </c>
+      <c r="I236" s="2">
+        <v>83</v>
+      </c>
+      <c r="J236" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10">
+      <c r="A237" s="1">
+        <v>44250</v>
+      </c>
+      <c r="B237" s="2">
+        <v>5704</v>
+      </c>
+      <c r="C237" s="2">
+        <v>127</v>
+      </c>
+      <c r="D237" s="2">
+        <v>1325</v>
+      </c>
+      <c r="E237" s="2">
+        <v>7156</v>
+      </c>
+      <c r="F237" s="2">
+        <v>1183</v>
+      </c>
+      <c r="G237" s="2">
+        <v>110</v>
+      </c>
+      <c r="H237" s="2">
+        <v>8</v>
+      </c>
+      <c r="I237" s="2">
+        <v>102</v>
+      </c>
+      <c r="J237" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10">
+      <c r="A238" s="1">
+        <v>44251</v>
+      </c>
+      <c r="B238" s="2">
+        <v>5736</v>
+      </c>
+      <c r="C238" s="2">
+        <v>226</v>
+      </c>
+      <c r="D238" s="2">
+        <v>1333</v>
+      </c>
+      <c r="E238" s="2">
+        <v>7295</v>
+      </c>
+      <c r="F238" s="2">
+        <v>1197</v>
+      </c>
+      <c r="G238" s="2">
+        <v>103</v>
+      </c>
+      <c r="H238" s="2">
+        <v>7</v>
+      </c>
+      <c r="I238" s="2">
+        <v>96</v>
+      </c>
+      <c r="J238" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10">
+      <c r="A239" s="1">
+        <v>44252</v>
+      </c>
+      <c r="B239" s="2">
+        <v>5760</v>
+      </c>
+      <c r="C239" s="2">
+        <v>207</v>
+      </c>
+      <c r="D239" s="2">
+        <v>1362</v>
+      </c>
+      <c r="E239" s="2">
+        <v>7329</v>
+      </c>
+      <c r="F239" s="2">
+        <v>1203</v>
+      </c>
+      <c r="G239" s="2">
+        <v>126</v>
+      </c>
+      <c r="H239" s="2">
+        <v>7</v>
+      </c>
+      <c r="I239" s="2">
+        <v>119</v>
+      </c>
+      <c r="J239" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10">
+      <c r="A240" s="1">
+        <v>44253</v>
+      </c>
+      <c r="B240" s="2">
+        <v>5808</v>
+      </c>
+      <c r="C240" s="2">
+        <v>249</v>
+      </c>
+      <c r="D240" s="2">
+        <v>1372</v>
+      </c>
+      <c r="E240" s="2">
+        <v>7429</v>
+      </c>
+      <c r="F240" s="2">
+        <v>1219</v>
+      </c>
+      <c r="G240" s="2">
+        <v>120</v>
+      </c>
+      <c r="H240" s="2">
+        <v>9</v>
+      </c>
+      <c r="I240" s="2">
+        <v>111</v>
+      </c>
+      <c r="J240" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10">
+      <c r="A241" s="1">
+        <v>44254</v>
+      </c>
+      <c r="B241" s="2">
+        <v>5841</v>
+      </c>
+      <c r="C241" s="2">
+        <v>294</v>
+      </c>
+      <c r="D241" s="2">
+        <v>1388</v>
+      </c>
+      <c r="E241" s="2">
+        <v>7523</v>
+      </c>
+      <c r="F241" s="2">
+        <v>1228</v>
+      </c>
+      <c r="G241" s="2">
+        <v>127</v>
+      </c>
+      <c r="H241" s="2">
+        <v>7</v>
+      </c>
+      <c r="I241" s="2">
+        <v>120</v>
+      </c>
+      <c r="J241" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10">
+      <c r="A242" s="1">
+        <v>44255</v>
+      </c>
+      <c r="B242" s="2">
+        <v>5847</v>
+      </c>
+      <c r="C242" s="2">
+        <v>302</v>
+      </c>
+      <c r="D242" s="2">
+        <v>1389</v>
+      </c>
+      <c r="E242" s="2">
+        <v>7538</v>
+      </c>
+      <c r="F242" s="2">
+        <v>1228</v>
+      </c>
+      <c r="G242" s="2">
+        <v>128</v>
+      </c>
+      <c r="H242" s="2">
+        <v>8</v>
+      </c>
+      <c r="I242" s="2">
+        <v>120</v>
+      </c>
+      <c r="J242" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10">
+      <c r="A243" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B243" s="2">
+        <v>5972</v>
+      </c>
+      <c r="C243" s="2">
+        <v>186</v>
+      </c>
+      <c r="D243" s="2">
+        <v>1428</v>
+      </c>
+      <c r="E243" s="2">
+        <v>7586</v>
+      </c>
+      <c r="F243" s="2">
+        <v>1233</v>
+      </c>
+      <c r="G243" s="2">
+        <v>162</v>
+      </c>
+      <c r="H243" s="2">
+        <v>8</v>
+      </c>
+      <c r="I243" s="2">
+        <v>154</v>
+      </c>
+      <c r="J243" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10">
+      <c r="A244" s="1">
+        <v>44257</v>
+      </c>
+      <c r="B244" s="2">
+        <v>6012</v>
+      </c>
+      <c r="C244" s="2">
+        <v>218</v>
+      </c>
+      <c r="D244" s="2">
+        <v>1433</v>
+      </c>
+      <c r="E244" s="2">
+        <v>7663</v>
+      </c>
+      <c r="F244" s="2">
+        <v>1233</v>
+      </c>
+      <c r="G244" s="2">
+        <v>167</v>
+      </c>
+      <c r="H244" s="2">
+        <v>7</v>
+      </c>
+      <c r="I244" s="2">
+        <v>160</v>
+      </c>
+      <c r="J244" s="2">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -7092,29 +8239,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7149,7 +8296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -7172,7 +8319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -7195,7 +8342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -7218,7 +8365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -7241,7 +8388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -7264,7 +8411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -7287,7 +8434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -7307,7 +8454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -7327,7 +8474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -7347,7 +8494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -7367,7 +8514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -7387,12 +8534,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -7412,7 +8559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -7432,7 +8579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -7452,7 +8599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -7472,7 +8619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -7492,7 +8639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -7512,7 +8659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -7532,7 +8679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -7552,7 +8699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -7572,7 +8719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -7580,7 +8727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -7603,7 +8750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -7623,7 +8770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -7643,7 +8790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -7663,17 +8810,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -7693,7 +8840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -7716,7 +8863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -7739,7 +8886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -7759,7 +8906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -7785,267 +8932,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until March 8th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,37 +396,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J244"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B245" sqref="B245"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B250" sqref="B250"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -485,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -517,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -549,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -581,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -613,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -645,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -677,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -709,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -741,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -773,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -805,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -837,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -869,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -901,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -933,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -965,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -997,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1029,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1093,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1125,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1157,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1221,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1253,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1285,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1317,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1349,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1413,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1445,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1477,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1509,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1541,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1573,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1605,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1637,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1669,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1701,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1733,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1765,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1829,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1861,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1893,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1925,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1957,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1989,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2021,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2053,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2085,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2117,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2149,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2181,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2213,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2245,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2277,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2309,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2341,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2373,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2405,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2437,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2469,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2501,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2533,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2565,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2597,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2629,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2661,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2693,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2725,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2757,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2789,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2821,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2853,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2885,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2917,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2949,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2981,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3013,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3045,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3077,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3109,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3141,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3173,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3205,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3237,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3269,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3301,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3333,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3365,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3397,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3429,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3461,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3493,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3525,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3557,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3589,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3621,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3653,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3685,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3717,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3749,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3781,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3813,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3845,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3877,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3909,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3941,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3973,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4005,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4037,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4069,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4101,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4133,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4165,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4197,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4229,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4261,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4293,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4325,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4357,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4389,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4421,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4453,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4485,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4517,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4549,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4581,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4613,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4645,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4709,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4741,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4773,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4805,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4837,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4869,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4901,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4933,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4965,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -4997,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5029,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5061,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5093,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5125,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5157,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5189,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5221,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5253,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5285,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5317,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5349,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5381,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5413,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5445,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5477,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5509,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5541,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5573,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5605,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5637,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5669,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5701,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5733,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5765,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5797,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5829,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5861,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5893,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5925,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5957,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5989,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6021,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6053,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6085,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6117,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6149,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6181,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6213,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6245,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6277,7 +6282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6309,7 +6314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6341,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6373,7 +6378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6405,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6437,7 +6442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6469,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6501,7 +6506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6533,7 +6538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6565,7 +6570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6597,7 +6602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6629,7 +6634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6661,7 +6666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6693,7 +6698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6725,7 +6730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6757,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6789,7 +6794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6821,7 +6826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6853,7 +6858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6885,7 +6890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6917,7 +6922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6949,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6981,7 +6986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7013,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7045,7 +7050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7077,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7109,7 +7114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7141,7 +7146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7173,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7205,7 +7210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7237,7 +7242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7269,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7301,7 +7306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7333,7 +7338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7365,7 +7370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7397,7 +7402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7429,7 +7434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7461,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7493,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7525,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7557,7 +7562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7589,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7621,7 +7626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7653,7 +7658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7685,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7717,7 +7722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7749,7 +7754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7781,7 +7786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7813,7 +7818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7845,7 +7850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7877,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7909,7 +7914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7941,7 +7946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7973,7 +7978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8005,7 +8010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8037,7 +8042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8069,7 +8074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8101,7 +8106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8133,7 +8138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8165,7 +8170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8197,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8227,6 +8232,166 @@
       </c>
       <c r="J244" s="2">
         <v>33</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>44258</v>
+      </c>
+      <c r="B245" s="2">
+        <v>6063</v>
+      </c>
+      <c r="C245" s="2">
+        <v>255</v>
+      </c>
+      <c r="D245" s="2">
+        <v>1471</v>
+      </c>
+      <c r="E245" s="2">
+        <v>7759</v>
+      </c>
+      <c r="F245" s="2">
+        <v>1247</v>
+      </c>
+      <c r="G245" s="2">
+        <v>191</v>
+      </c>
+      <c r="H245" s="2">
+        <v>8</v>
+      </c>
+      <c r="I245" s="2">
+        <v>183</v>
+      </c>
+      <c r="J245" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>44259</v>
+      </c>
+      <c r="B246" s="2">
+        <v>6075</v>
+      </c>
+      <c r="C246" s="2">
+        <v>286</v>
+      </c>
+      <c r="D246" s="2">
+        <v>1489</v>
+      </c>
+      <c r="E246" s="2">
+        <v>7850</v>
+      </c>
+      <c r="F246" s="2">
+        <v>1258</v>
+      </c>
+      <c r="G246" s="2">
+        <v>198</v>
+      </c>
+      <c r="H246" s="2">
+        <v>7</v>
+      </c>
+      <c r="I246" s="2">
+        <v>191</v>
+      </c>
+      <c r="J246" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>44260</v>
+      </c>
+      <c r="B247" s="2">
+        <v>6132</v>
+      </c>
+      <c r="C247" s="2">
+        <v>267</v>
+      </c>
+      <c r="D247" s="2">
+        <v>1510</v>
+      </c>
+      <c r="E247" s="2">
+        <v>7909</v>
+      </c>
+      <c r="F247" s="2">
+        <v>1278</v>
+      </c>
+      <c r="G247" s="2">
+        <v>197</v>
+      </c>
+      <c r="H247" s="2">
+        <v>10</v>
+      </c>
+      <c r="I247" s="2">
+        <v>187</v>
+      </c>
+      <c r="J247" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>44261</v>
+      </c>
+      <c r="B248" s="2">
+        <v>6174</v>
+      </c>
+      <c r="C248" s="2">
+        <v>215</v>
+      </c>
+      <c r="D248" s="2">
+        <v>1528</v>
+      </c>
+      <c r="E248" s="2">
+        <v>7917</v>
+      </c>
+      <c r="F248" s="2">
+        <v>1278</v>
+      </c>
+      <c r="G248" s="2">
+        <v>214</v>
+      </c>
+      <c r="H248" s="2">
+        <v>10</v>
+      </c>
+      <c r="I248" s="2">
+        <v>204</v>
+      </c>
+      <c r="J248" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>44262</v>
+      </c>
+      <c r="B249" s="2">
+        <v>6223</v>
+      </c>
+      <c r="C249" s="2">
+        <v>162</v>
+      </c>
+      <c r="D249" s="2">
+        <v>1555</v>
+      </c>
+      <c r="E249" s="2">
+        <v>7940</v>
+      </c>
+      <c r="F249" s="2">
+        <v>1282</v>
+      </c>
+      <c r="G249" s="2">
+        <v>237</v>
+      </c>
+      <c r="H249" s="2">
+        <v>11</v>
+      </c>
+      <c r="I249" s="2">
+        <v>226</v>
+      </c>
+      <c r="J249" s="2">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -8239,29 +8404,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8296,7 +8461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -8319,7 +8484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -8342,7 +8507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -8365,7 +8530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -8388,7 +8553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -8411,7 +8576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -8434,7 +8599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -8454,7 +8619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -8474,7 +8639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -8494,7 +8659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -8514,7 +8679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -8534,12 +8699,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -8559,7 +8724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -8579,7 +8744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -8599,7 +8764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -8619,7 +8784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -8639,7 +8804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -8659,7 +8824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -8679,7 +8844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -8699,7 +8864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -8719,7 +8884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -8727,7 +8892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -8750,7 +8915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -8770,7 +8935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -8790,7 +8955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -8810,17 +8975,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -8840,7 +9005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -8863,7 +9028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -8886,7 +9051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -8906,7 +9071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -8932,267 +9097,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until March 12th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,37 +391,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J249"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J254"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B250" sqref="B250"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A255" sqref="A255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1957,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +4997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6245,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6277,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6309,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6373,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6469,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7082,7 +7077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7114,7 +7109,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7146,7 +7141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7178,7 +7173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7210,7 +7205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7242,7 +7237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7274,7 +7269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7306,7 +7301,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7338,7 +7333,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7370,7 +7365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7402,7 +7397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7434,7 +7429,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7466,7 +7461,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7498,7 +7493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7530,7 +7525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7562,7 +7557,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7594,7 +7589,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7626,7 +7621,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7658,7 +7653,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7690,7 +7685,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7722,7 +7717,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7754,7 +7749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7786,7 +7781,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7818,7 +7813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7850,7 +7845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7882,7 +7877,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7914,7 +7909,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7946,7 +7941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7978,7 +7973,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8010,7 +8005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8042,7 +8037,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8074,7 +8069,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8106,7 +8101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8138,7 +8133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8170,7 +8165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8202,7 +8197,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8234,7 +8229,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8266,7 +8261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8298,7 +8293,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8330,7 +8325,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8362,7 +8357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8392,6 +8387,166 @@
       </c>
       <c r="J249" s="2">
         <v>36</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10">
+      <c r="A250" s="1">
+        <v>44263</v>
+      </c>
+      <c r="B250" s="2">
+        <v>6268</v>
+      </c>
+      <c r="C250" s="2">
+        <v>169</v>
+      </c>
+      <c r="D250" s="2">
+        <v>1574</v>
+      </c>
+      <c r="E250" s="2">
+        <v>8011</v>
+      </c>
+      <c r="F250" s="2">
+        <v>1310</v>
+      </c>
+      <c r="G250" s="2">
+        <v>227</v>
+      </c>
+      <c r="H250" s="2">
+        <v>11</v>
+      </c>
+      <c r="I250" s="2">
+        <v>216</v>
+      </c>
+      <c r="J250" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10">
+      <c r="A251" s="1">
+        <v>44264</v>
+      </c>
+      <c r="B251" s="2">
+        <v>6306</v>
+      </c>
+      <c r="C251" s="2">
+        <v>186</v>
+      </c>
+      <c r="D251" s="2">
+        <v>1602</v>
+      </c>
+      <c r="E251" s="2">
+        <v>8094</v>
+      </c>
+      <c r="F251" s="2">
+        <v>1329</v>
+      </c>
+      <c r="G251" s="2">
+        <v>236</v>
+      </c>
+      <c r="H251" s="2">
+        <v>12</v>
+      </c>
+      <c r="I251" s="2">
+        <v>224</v>
+      </c>
+      <c r="J251" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10">
+      <c r="A252" s="1">
+        <v>44265</v>
+      </c>
+      <c r="B252" s="2">
+        <v>6358</v>
+      </c>
+      <c r="C252" s="2">
+        <v>288</v>
+      </c>
+      <c r="D252" s="2">
+        <v>1629</v>
+      </c>
+      <c r="E252" s="2">
+        <v>8275</v>
+      </c>
+      <c r="F252" s="2">
+        <v>1347</v>
+      </c>
+      <c r="G252" s="2">
+        <v>245</v>
+      </c>
+      <c r="H252" s="2">
+        <v>12</v>
+      </c>
+      <c r="I252" s="2">
+        <v>233</v>
+      </c>
+      <c r="J252" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10">
+      <c r="A253" s="1">
+        <v>44266</v>
+      </c>
+      <c r="B253" s="2">
+        <v>6403</v>
+      </c>
+      <c r="C253" s="2">
+        <v>301</v>
+      </c>
+      <c r="D253" s="2">
+        <v>1651</v>
+      </c>
+      <c r="E253" s="2">
+        <v>8355</v>
+      </c>
+      <c r="F253" s="2">
+        <v>1356</v>
+      </c>
+      <c r="G253" s="2">
+        <v>258</v>
+      </c>
+      <c r="H253" s="2">
+        <v>12</v>
+      </c>
+      <c r="I253" s="2">
+        <v>246</v>
+      </c>
+      <c r="J253" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10">
+      <c r="A254" s="1">
+        <v>44267</v>
+      </c>
+      <c r="B254" s="2">
+        <v>6467</v>
+      </c>
+      <c r="C254" s="2">
+        <v>276</v>
+      </c>
+      <c r="D254" s="2">
+        <v>1698</v>
+      </c>
+      <c r="E254" s="2">
+        <v>8441</v>
+      </c>
+      <c r="F254" s="2">
+        <v>1377</v>
+      </c>
+      <c r="G254" s="2">
+        <v>284</v>
+      </c>
+      <c r="H254" s="2">
+        <v>14</v>
+      </c>
+      <c r="I254" s="2">
+        <v>270</v>
+      </c>
+      <c r="J254" s="2">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -8404,29 +8559,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8461,7 +8616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -8484,7 +8639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -8507,7 +8662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -8530,7 +8685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -8553,7 +8708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -8576,7 +8731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -8599,7 +8754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -8619,7 +8774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -8639,7 +8794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -8659,7 +8814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -8679,7 +8834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -8699,12 +8854,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -8724,7 +8879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -8744,7 +8899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -8764,7 +8919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -8784,7 +8939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -8804,7 +8959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -8824,7 +8979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -8844,7 +8999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -8864,7 +9019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -8884,7 +9039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -8892,7 +9047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -8915,7 +9070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -8935,7 +9090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -8955,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -8975,17 +9130,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -9005,7 +9160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -9028,7 +9183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -9051,7 +9206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -9071,7 +9226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -9097,267 +9252,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data untin March 14th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,37 +396,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J254"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A255" sqref="A255"/>
+      <selection pane="bottomLeft" activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -485,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -517,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -549,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -581,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -613,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -645,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -677,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -709,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -741,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -773,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -805,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -837,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -869,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -901,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -933,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -965,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -997,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1029,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1093,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1125,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1157,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1221,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1253,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1285,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1317,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1349,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1413,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1445,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1477,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1509,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1541,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1573,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1605,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1637,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1669,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1701,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1733,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1765,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1829,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1861,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1893,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1925,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1957,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1989,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2021,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2053,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2085,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2117,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2149,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2181,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2213,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2245,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2277,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2309,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2341,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2373,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2405,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2437,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2469,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2501,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2533,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2565,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2597,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2629,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2661,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2693,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2725,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2757,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2789,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2821,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2853,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2885,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2917,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2949,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2981,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3013,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3045,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3077,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3109,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3141,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3173,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3205,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3237,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3269,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3301,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3333,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3365,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3397,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3429,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3461,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3493,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3525,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3557,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3589,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3621,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3653,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3685,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3717,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3749,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3781,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3813,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3845,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3877,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3909,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3941,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3973,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4005,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4037,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4069,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4101,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4133,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4165,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4197,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4229,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4261,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4293,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4325,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4357,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4389,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4421,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4453,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4485,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4517,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4549,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4581,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4613,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4645,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4709,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4741,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4773,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4805,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4837,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4869,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4901,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4933,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4965,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -4997,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5029,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5061,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5093,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5125,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5157,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5189,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5221,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5253,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5285,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5317,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5349,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5381,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5413,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5445,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5477,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5509,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5541,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5573,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5605,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5637,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5669,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5701,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5733,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5765,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5797,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5829,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5861,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5893,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5925,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5957,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5989,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6021,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6053,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6085,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6117,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6149,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6181,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6213,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6245,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6277,7 +6282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6309,7 +6314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6341,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6373,7 +6378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6405,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6437,7 +6442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6469,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6501,7 +6506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6533,7 +6538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6565,7 +6570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6597,7 +6602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6629,7 +6634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6661,7 +6666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6693,7 +6698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6725,7 +6730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6757,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6789,7 +6794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6821,7 +6826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6853,7 +6858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6885,7 +6890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6917,7 +6922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6949,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6981,7 +6986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7013,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7045,7 +7050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7077,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7109,7 +7114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7141,7 +7146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7173,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7205,7 +7210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7237,7 +7242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7269,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7301,7 +7306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7333,7 +7338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7365,7 +7370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7397,7 +7402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7429,7 +7434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7461,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7493,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7525,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7557,7 +7562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7589,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7621,7 +7626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7653,7 +7658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7685,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7717,7 +7722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7749,7 +7754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7781,7 +7786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7813,7 +7818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7845,7 +7850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7877,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7909,7 +7914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7941,7 +7946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7973,7 +7978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8005,7 +8010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8037,7 +8042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8069,7 +8074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8101,7 +8106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8133,7 +8138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8165,7 +8170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8197,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8229,7 +8234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8261,7 +8266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8293,7 +8298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8325,7 +8330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8357,7 +8362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8389,7 +8394,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8421,7 +8426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8453,7 +8458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8485,7 +8490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8517,7 +8522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8547,6 +8552,70 @@
       </c>
       <c r="J254" s="2">
         <v>37</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>44268</v>
+      </c>
+      <c r="B255" s="2">
+        <v>6501</v>
+      </c>
+      <c r="C255" s="2">
+        <v>297</v>
+      </c>
+      <c r="D255" s="2">
+        <v>1732</v>
+      </c>
+      <c r="E255" s="2">
+        <v>8530</v>
+      </c>
+      <c r="F255" s="2">
+        <v>1404</v>
+      </c>
+      <c r="G255" s="2">
+        <v>291</v>
+      </c>
+      <c r="H255" s="2">
+        <v>14</v>
+      </c>
+      <c r="I255" s="2">
+        <v>277</v>
+      </c>
+      <c r="J255" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>44269</v>
+      </c>
+      <c r="B256" s="2">
+        <v>6507</v>
+      </c>
+      <c r="C256" s="2">
+        <v>306</v>
+      </c>
+      <c r="D256" s="2">
+        <v>1732</v>
+      </c>
+      <c r="E256" s="2">
+        <v>8545</v>
+      </c>
+      <c r="F256" s="2">
+        <v>1405</v>
+      </c>
+      <c r="G256" s="2">
+        <v>288</v>
+      </c>
+      <c r="H256" s="2">
+        <v>13</v>
+      </c>
+      <c r="I256" s="2">
+        <v>275</v>
+      </c>
+      <c r="J256" s="2">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -8559,29 +8628,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8616,7 +8685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -8639,7 +8708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -8662,7 +8731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -8685,7 +8754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -8708,7 +8777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -8731,7 +8800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -8754,7 +8823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -8774,7 +8843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -8794,7 +8863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -8814,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -8834,7 +8903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -8854,12 +8923,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -8879,7 +8948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -8899,7 +8968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -8919,7 +8988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -8939,7 +9008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -8959,7 +9028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -8979,7 +9048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -8999,7 +9068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -9019,7 +9088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -9039,7 +9108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -9047,7 +9116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -9070,7 +9139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -9090,7 +9159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -9110,7 +9179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -9130,17 +9199,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -9160,7 +9229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -9183,7 +9252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -9206,7 +9275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -9226,7 +9295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -9252,267 +9321,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data until March 16th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,37 +391,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J256"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B256" sqref="B256"/>
+      <selection pane="bottomLeft" activeCell="F257" sqref="F257"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1957,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2341,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +4997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6245,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6277,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6309,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6373,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6469,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7082,7 +7077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7114,7 +7109,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7146,7 +7141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7178,7 +7173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7210,7 +7205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7242,7 +7237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7274,7 +7269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7306,7 +7301,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7338,7 +7333,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7370,7 +7365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7402,7 +7397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7434,7 +7429,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7466,7 +7461,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7498,7 +7493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7530,7 +7525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7562,7 +7557,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7594,7 +7589,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7626,7 +7621,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7658,7 +7653,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7690,7 +7685,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7722,7 +7717,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7754,7 +7749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7786,7 +7781,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7818,7 +7813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7850,7 +7845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7882,7 +7877,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7914,7 +7909,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7946,7 +7941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7978,7 +7973,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8010,7 +8005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8042,7 +8037,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8074,7 +8069,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8106,7 +8101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8138,7 +8133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8170,7 +8165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8202,7 +8197,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8234,7 +8229,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8266,7 +8261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8298,7 +8293,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8330,7 +8325,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8362,7 +8357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8394,7 +8389,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8426,7 +8421,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8458,7 +8453,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8490,7 +8485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8522,7 +8517,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8554,7 +8549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8586,7 +8581,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8616,6 +8611,70 @@
       </c>
       <c r="J256" s="2">
         <v>39</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10">
+      <c r="A257" s="1">
+        <v>44270</v>
+      </c>
+      <c r="B257" s="2">
+        <v>6555</v>
+      </c>
+      <c r="C257" s="2">
+        <v>300</v>
+      </c>
+      <c r="D257" s="2">
+        <v>1766</v>
+      </c>
+      <c r="E257" s="2">
+        <v>8621</v>
+      </c>
+      <c r="F257" s="2">
+        <v>1422</v>
+      </c>
+      <c r="G257" s="2">
+        <v>305</v>
+      </c>
+      <c r="H257" s="2">
+        <v>15</v>
+      </c>
+      <c r="I257" s="2">
+        <v>290</v>
+      </c>
+      <c r="J257" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10">
+      <c r="A258" s="1">
+        <v>44271</v>
+      </c>
+      <c r="B258" s="2">
+        <v>6643</v>
+      </c>
+      <c r="C258" s="2">
+        <v>313</v>
+      </c>
+      <c r="D258" s="2">
+        <v>1815</v>
+      </c>
+      <c r="E258" s="2">
+        <v>8771</v>
+      </c>
+      <c r="F258" s="2">
+        <v>1462</v>
+      </c>
+      <c r="G258" s="2">
+        <v>311</v>
+      </c>
+      <c r="H258" s="2">
+        <v>14</v>
+      </c>
+      <c r="I258" s="2">
+        <v>297</v>
+      </c>
+      <c r="J258" s="2">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -8628,29 +8687,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8685,7 +8744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -8708,7 +8767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -8731,7 +8790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -8754,7 +8813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -8777,7 +8836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -8800,7 +8859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -8823,7 +8882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -8843,7 +8902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -8863,7 +8922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -8883,7 +8942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -8903,7 +8962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -8923,12 +8982,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -8948,7 +9007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -8968,7 +9027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -8988,7 +9047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -9008,7 +9067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -9028,7 +9087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -9048,7 +9107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -9068,7 +9127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -9088,7 +9147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -9108,7 +9167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -9116,7 +9175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -9139,7 +9198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -9159,7 +9218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -9179,7 +9238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -9199,17 +9258,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -9229,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -9252,7 +9311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -9275,7 +9334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -9295,7 +9354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -9321,267 +9380,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data until March 17th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -391,7 +391,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -399,11 +399,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J258"/>
+  <dimension ref="A1:J259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F257" sqref="F257"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J260" sqref="J260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -8675,6 +8675,38 @@
       </c>
       <c r="J258" s="2">
         <v>42</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10">
+      <c r="A259" s="1">
+        <v>44272</v>
+      </c>
+      <c r="B259" s="2">
+        <v>6666</v>
+      </c>
+      <c r="C259" s="2">
+        <v>357</v>
+      </c>
+      <c r="D259" s="2">
+        <v>1840</v>
+      </c>
+      <c r="E259" s="2">
+        <v>8863</v>
+      </c>
+      <c r="F259" s="2">
+        <v>1486</v>
+      </c>
+      <c r="G259" s="2">
+        <v>311</v>
+      </c>
+      <c r="H259" s="2">
+        <v>15</v>
+      </c>
+      <c r="I259" s="2">
+        <v>296</v>
+      </c>
+      <c r="J259" s="2">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until March 20th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -72,16 +72,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,7 +119,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -402,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,11 +402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J261"/>
+  <dimension ref="A1:J262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I261" sqref="I261"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A263" sqref="A263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -8753,7 +8745,68 @@
       </c>
     </row>
     <row r="261" spans="1:10">
-      <c r="I261" s="7"/>
+      <c r="A261" s="1">
+        <v>44274</v>
+      </c>
+      <c r="B261" s="2">
+        <v>6838</v>
+      </c>
+      <c r="C261" s="2">
+        <v>349</v>
+      </c>
+      <c r="D261" s="2">
+        <v>1965</v>
+      </c>
+      <c r="E261" s="2">
+        <v>9152</v>
+      </c>
+      <c r="F261" s="2">
+        <v>1527</v>
+      </c>
+      <c r="G261" s="2">
+        <v>395</v>
+      </c>
+      <c r="H261" s="2">
+        <v>16</v>
+      </c>
+      <c r="I261" s="7">
+        <v>379</v>
+      </c>
+      <c r="J261" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10">
+      <c r="A262" s="1">
+        <v>44275</v>
+      </c>
+      <c r="B262" s="2">
+        <v>6934</v>
+      </c>
+      <c r="C262" s="2">
+        <v>325</v>
+      </c>
+      <c r="D262" s="2">
+        <v>2011</v>
+      </c>
+      <c r="E262" s="2">
+        <v>9270</v>
+      </c>
+      <c r="F262" s="2">
+        <v>1530</v>
+      </c>
+      <c r="G262" s="2">
+        <v>437</v>
+      </c>
+      <c r="H262" s="2">
+        <v>16</v>
+      </c>
+      <c r="I262" s="2">
+        <v>421</v>
+      </c>
+      <c r="J262" s="2">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:J173">

</xml_diff>

<commit_message>
add data until March 21th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,37 +399,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J262"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A263" sqref="A263"/>
+      <selection pane="bottomLeft" activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -488,7 +493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -520,7 +525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -552,7 +557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -584,7 +589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -616,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -648,7 +653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -680,7 +685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -712,7 +717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -744,7 +749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -776,7 +781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -808,7 +813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -840,7 +845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -872,7 +877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -904,7 +909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -936,7 +941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -968,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1000,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1032,7 +1037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1064,7 +1069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1096,7 +1101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1128,7 +1133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1160,7 +1165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1192,7 +1197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1224,7 +1229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1256,7 +1261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1288,7 +1293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1320,7 +1325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1352,7 +1357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1384,7 +1389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1416,7 +1421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1448,7 +1453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1480,7 +1485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1512,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1544,7 +1549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1576,7 +1581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1608,7 +1613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1640,7 +1645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1672,7 +1677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1704,7 +1709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1736,7 +1741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1768,7 +1773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1800,7 +1805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1832,7 +1837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1864,7 +1869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1896,7 +1901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1928,7 +1933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1960,7 +1965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1992,7 +1997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2024,7 +2029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2056,7 +2061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2088,7 +2093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2120,7 +2125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2152,7 +2157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2184,7 +2189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2216,7 +2221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2248,7 +2253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2280,7 +2285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2312,7 +2317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2344,7 +2349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2376,7 +2381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2408,7 +2413,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2440,7 +2445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2472,7 +2477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2504,7 +2509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2536,7 +2541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2568,7 +2573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2600,7 +2605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2632,7 +2637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2664,7 +2669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2696,7 +2701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2728,7 +2733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2760,7 +2765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2792,7 +2797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2824,7 +2829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2856,7 +2861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2888,7 +2893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2920,7 +2925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2952,7 +2957,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2984,7 +2989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3016,7 +3021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3048,7 +3053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3080,7 +3085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3112,7 +3117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3144,7 +3149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3176,7 +3181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3208,7 +3213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3240,7 +3245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3272,7 +3277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3304,7 +3309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3336,7 +3341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3368,7 +3373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3432,7 +3437,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3464,7 +3469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3496,7 +3501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3528,7 +3533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3560,7 +3565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3592,7 +3597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3624,7 +3629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3656,7 +3661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3688,7 +3693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3720,7 +3725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3752,7 +3757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3784,7 +3789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3816,7 +3821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3848,7 +3853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3880,7 +3885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3912,7 +3917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3944,7 +3949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3976,7 +3981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4008,7 +4013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4040,7 +4045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4072,7 +4077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4104,7 +4109,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4136,7 +4141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4168,7 +4173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4200,7 +4205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4232,7 +4237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4264,7 +4269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4296,7 +4301,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4328,7 +4333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4360,7 +4365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4392,7 +4397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4424,7 +4429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4456,7 +4461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4488,7 +4493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4520,7 +4525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4552,7 +4557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4584,7 +4589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4616,7 +4621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4648,7 +4653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4680,7 +4685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4712,7 +4717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4744,7 +4749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4776,7 +4781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4808,7 +4813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4840,7 +4845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4872,7 +4877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4904,7 +4909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4936,7 +4941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4968,7 +4973,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5000,7 +5005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5032,7 +5037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5064,7 +5069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5096,7 +5101,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5128,7 +5133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5160,7 +5165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5192,7 +5197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5224,7 +5229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5256,7 +5261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5288,7 +5293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5320,7 +5325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5352,7 +5357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5384,7 +5389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5416,7 +5421,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5448,7 +5453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5480,7 +5485,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5512,7 +5517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5544,7 +5549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5576,7 +5581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5608,7 +5613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5640,7 +5645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5672,7 +5677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5704,7 +5709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5736,7 +5741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5768,7 +5773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5800,7 +5805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5832,7 +5837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5864,7 +5869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5896,7 +5901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5928,7 +5933,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5960,7 +5965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5992,7 +5997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6024,7 +6029,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6056,7 +6061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6088,7 +6093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6120,7 +6125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6152,7 +6157,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6184,7 +6189,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6216,7 +6221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6248,7 +6253,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6280,7 +6285,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6312,7 +6317,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6344,7 +6349,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6376,7 +6381,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6408,7 +6413,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6440,7 +6445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6472,7 +6477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6504,7 +6509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6536,7 +6541,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6568,7 +6573,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6600,7 +6605,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6632,7 +6637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6664,7 +6669,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6696,7 +6701,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6728,7 +6733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6760,7 +6765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6792,7 +6797,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6824,7 +6829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6856,7 +6861,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6888,7 +6893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6920,7 +6925,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6952,7 +6957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6984,7 +6989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7016,7 +7021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7048,7 +7053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7080,7 +7085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7112,7 +7117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7144,7 +7149,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7176,7 +7181,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7208,7 +7213,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7240,7 +7245,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7272,7 +7277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7304,7 +7309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7336,7 +7341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7368,7 +7373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7400,7 +7405,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7432,7 +7437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7464,7 +7469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7496,7 +7501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7528,7 +7533,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7560,7 +7565,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7592,7 +7597,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7624,7 +7629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7656,7 +7661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7688,7 +7693,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7720,7 +7725,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7752,7 +7757,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7784,7 +7789,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7816,7 +7821,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7848,7 +7853,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7880,7 +7885,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7912,7 +7917,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7944,7 +7949,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7976,7 +7981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8008,7 +8013,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8040,7 +8045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8072,7 +8077,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8104,7 +8109,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8136,7 +8141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8168,7 +8173,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8200,7 +8205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8232,7 +8237,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8264,7 +8269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8296,7 +8301,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8328,7 +8333,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8360,7 +8365,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8392,7 +8397,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8424,7 +8429,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8456,7 +8461,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8488,7 +8493,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8520,7 +8525,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8552,7 +8557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8584,7 +8589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8616,7 +8621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8648,7 +8653,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8680,7 +8685,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8712,7 +8717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8744,7 +8749,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8776,7 +8781,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8806,6 +8811,38 @@
       </c>
       <c r="J262" s="2">
         <v>44</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
+        <v>44276</v>
+      </c>
+      <c r="B263" s="2">
+        <v>6968</v>
+      </c>
+      <c r="C263" s="2">
+        <v>287</v>
+      </c>
+      <c r="D263" s="2">
+        <v>2039</v>
+      </c>
+      <c r="E263" s="2">
+        <v>9294</v>
+      </c>
+      <c r="F263" s="2">
+        <v>1530</v>
+      </c>
+      <c r="G263" s="2">
+        <v>464</v>
+      </c>
+      <c r="H263" s="2">
+        <v>16</v>
+      </c>
+      <c r="I263" s="2">
+        <v>448</v>
+      </c>
+      <c r="J263" s="2">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -8818,29 +8855,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8875,7 +8912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -8898,7 +8935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -8921,7 +8958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -8944,7 +8981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -8967,7 +9004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -8990,7 +9027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9013,7 +9050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9033,7 +9070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9053,7 +9090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9073,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9093,7 +9130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9113,12 +9150,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -9138,7 +9175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -9158,7 +9195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -9178,7 +9215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -9198,7 +9235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -9218,7 +9255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -9238,7 +9275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -9258,7 +9295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -9278,7 +9315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -9298,7 +9335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -9306,7 +9343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -9329,7 +9366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -9349,7 +9386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -9369,7 +9406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -9389,17 +9426,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -9419,7 +9456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -9442,7 +9479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -9465,7 +9502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -9485,7 +9522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -9511,267 +9548,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until March 22th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,37 +394,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J263"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A264" sqref="A264"/>
+      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -493,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -525,7 +520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -557,7 +552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -589,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -621,7 +616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -653,7 +648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -685,7 +680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -717,7 +712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -749,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -781,7 +776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -813,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -845,7 +840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -877,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -909,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -941,7 +936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -973,7 +968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1005,7 +1000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1037,7 +1032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1069,7 +1064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1101,7 +1096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1133,7 +1128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1165,7 +1160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1197,7 +1192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1229,7 +1224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1261,7 +1256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1293,7 +1288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1325,7 +1320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1357,7 +1352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1389,7 +1384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1421,7 +1416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1453,7 +1448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1485,7 +1480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1517,7 +1512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1549,7 +1544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1581,7 +1576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1613,7 +1608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1645,7 +1640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1677,7 +1672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1709,7 +1704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1741,7 +1736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1773,7 +1768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1805,7 +1800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1837,7 +1832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1869,7 +1864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1901,7 +1896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1933,7 +1928,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1965,7 +1960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1997,7 +1992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2029,7 +2024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2061,7 +2056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2093,7 +2088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2125,7 +2120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2157,7 +2152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2189,7 +2184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2221,7 +2216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2253,7 +2248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2285,7 +2280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2317,7 +2312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2349,7 +2344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2381,7 +2376,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2413,7 +2408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2445,7 +2440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2477,7 +2472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2509,7 +2504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2541,7 +2536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2573,7 +2568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2605,7 +2600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2637,7 +2632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2669,7 +2664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2701,7 +2696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2733,7 +2728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2765,7 +2760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2797,7 +2792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2829,7 +2824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2861,7 +2856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2893,7 +2888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2925,7 +2920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2957,7 +2952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2989,7 +2984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3021,7 +3016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3053,7 +3048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3085,7 +3080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3117,7 +3112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3149,7 +3144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3181,7 +3176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3213,7 +3208,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3245,7 +3240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3277,7 +3272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3309,7 +3304,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3341,7 +3336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3373,7 +3368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3405,7 +3400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3437,7 +3432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3469,7 +3464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3501,7 +3496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3533,7 +3528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3565,7 +3560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3597,7 +3592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3629,7 +3624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3661,7 +3656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3693,7 +3688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3725,7 +3720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3757,7 +3752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3789,7 +3784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3821,7 +3816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3853,7 +3848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3885,7 +3880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3917,7 +3912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3949,7 +3944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3981,7 +3976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4013,7 +4008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4045,7 +4040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4077,7 +4072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4109,7 +4104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4141,7 +4136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4173,7 +4168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4205,7 +4200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4237,7 +4232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4269,7 +4264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4301,7 +4296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4333,7 +4328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4365,7 +4360,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4397,7 +4392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4429,7 +4424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4461,7 +4456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4493,7 +4488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4525,7 +4520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4557,7 +4552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4589,7 +4584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4621,7 +4616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4653,7 +4648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4685,7 +4680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4717,7 +4712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4749,7 +4744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4781,7 +4776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4813,7 +4808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4845,7 +4840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4877,7 +4872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4909,7 +4904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4941,7 +4936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4973,7 +4968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5005,7 +5000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5037,7 +5032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5069,7 +5064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5101,7 +5096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5133,7 +5128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5165,7 +5160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5197,7 +5192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5229,7 +5224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5261,7 +5256,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5293,7 +5288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5325,7 +5320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5357,7 +5352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5389,7 +5384,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5421,7 +5416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5453,7 +5448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5485,7 +5480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5517,7 +5512,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5549,7 +5544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5581,7 +5576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5613,7 +5608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5645,7 +5640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5677,7 +5672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5709,7 +5704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5741,7 +5736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5773,7 +5768,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5805,7 +5800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5837,7 +5832,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5869,7 +5864,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5901,7 +5896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5933,7 +5928,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5965,7 +5960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5997,7 +5992,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6029,7 +6024,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6061,7 +6056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6093,7 +6088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6125,7 +6120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6157,7 +6152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6189,7 +6184,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6221,7 +6216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6253,7 +6248,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6285,7 +6280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6317,7 +6312,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6349,7 +6344,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6381,7 +6376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6413,7 +6408,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6445,7 +6440,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6477,7 +6472,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6509,7 +6504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6541,7 +6536,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6573,7 +6568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6605,7 +6600,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6637,7 +6632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6669,7 +6664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6701,7 +6696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6733,7 +6728,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6765,7 +6760,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6797,7 +6792,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6829,7 +6824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6861,7 +6856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6893,7 +6888,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6925,7 +6920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6957,7 +6952,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6989,7 +6984,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7021,7 +7016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7053,7 +7048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7085,7 +7080,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7117,7 +7112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7149,7 +7144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7181,7 +7176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7213,7 +7208,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7245,7 +7240,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7277,7 +7272,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7309,7 +7304,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7341,7 +7336,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7373,7 +7368,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7405,7 +7400,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7437,7 +7432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7469,7 +7464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7501,7 +7496,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7533,7 +7528,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7565,7 +7560,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7597,7 +7592,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7629,7 +7624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7661,7 +7656,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7693,7 +7688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7725,7 +7720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7757,7 +7752,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7789,7 +7784,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7821,7 +7816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7853,7 +7848,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7885,7 +7880,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7917,7 +7912,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7949,7 +7944,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7981,7 +7976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8013,7 +8008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8045,7 +8040,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8077,7 +8072,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8109,7 +8104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8141,7 +8136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8173,7 +8168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8205,7 +8200,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8237,7 +8232,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8269,7 +8264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8301,7 +8296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8333,7 +8328,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8365,7 +8360,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8397,7 +8392,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8429,7 +8424,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8461,7 +8456,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8493,7 +8488,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8525,7 +8520,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8557,7 +8552,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8589,7 +8584,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8621,7 +8616,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8653,7 +8648,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8685,7 +8680,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8717,7 +8712,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8749,7 +8744,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8781,7 +8776,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8813,7 +8808,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8843,6 +8838,38 @@
       </c>
       <c r="J263" s="2">
         <v>45</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10">
+      <c r="A264" s="1">
+        <v>44277</v>
+      </c>
+      <c r="B264" s="2">
+        <v>7008</v>
+      </c>
+      <c r="C264" s="2">
+        <v>346</v>
+      </c>
+      <c r="D264" s="2">
+        <v>2053</v>
+      </c>
+      <c r="E264" s="2">
+        <v>9407</v>
+      </c>
+      <c r="F264" s="2">
+        <v>1588</v>
+      </c>
+      <c r="G264" s="2">
+        <v>417</v>
+      </c>
+      <c r="H264" s="2">
+        <v>17</v>
+      </c>
+      <c r="I264" s="2">
+        <v>400</v>
+      </c>
+      <c r="J264" s="2">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -8855,29 +8882,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8912,7 +8939,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -8935,7 +8962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -8958,7 +8985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -8981,7 +9008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9004,7 +9031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9027,7 +9054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9050,7 +9077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9070,7 +9097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9090,7 +9117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9110,7 +9137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9130,7 +9157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9150,12 +9177,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -9175,7 +9202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -9195,7 +9222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -9215,7 +9242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -9235,7 +9262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -9255,7 +9282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -9275,7 +9302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -9295,7 +9322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -9315,7 +9342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -9335,7 +9362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -9343,7 +9370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -9366,7 +9393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -9386,7 +9413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -9406,7 +9433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -9426,17 +9453,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -9456,7 +9483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -9479,7 +9506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -9502,7 +9529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -9522,7 +9549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -9548,267 +9575,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until March 23th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,11 +402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J264"/>
+  <dimension ref="A1:J265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D264" sqref="D264"/>
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A266" sqref="A266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -8870,6 +8870,38 @@
       </c>
       <c r="J264" s="2">
         <v>48</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10">
+      <c r="A265" s="1">
+        <v>44278</v>
+      </c>
+      <c r="B265" s="2">
+        <v>7063</v>
+      </c>
+      <c r="C265" s="2">
+        <v>399</v>
+      </c>
+      <c r="D265" s="2">
+        <v>2134</v>
+      </c>
+      <c r="E265" s="2">
+        <v>9596</v>
+      </c>
+      <c r="F265" s="2">
+        <v>1610</v>
+      </c>
+      <c r="G265" s="2">
+        <v>475</v>
+      </c>
+      <c r="H265" s="2">
+        <v>17</v>
+      </c>
+      <c r="I265" s="2">
+        <v>458</v>
+      </c>
+      <c r="J265" s="2">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until March 24th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,11 +402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J265"/>
+  <dimension ref="A1:J266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A266" sqref="A266"/>
+      <selection pane="bottomLeft" activeCell="A267" sqref="A267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -8902,6 +8902,38 @@
       </c>
       <c r="J265" s="2">
         <v>49</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10">
+      <c r="A266" s="1">
+        <v>44279</v>
+      </c>
+      <c r="B266" s="2">
+        <v>7164</v>
+      </c>
+      <c r="C266" s="2">
+        <v>461</v>
+      </c>
+      <c r="D266" s="2">
+        <v>2221</v>
+      </c>
+      <c r="E266" s="2">
+        <v>9846</v>
+      </c>
+      <c r="F266" s="2">
+        <v>1654</v>
+      </c>
+      <c r="G266" s="2">
+        <v>516</v>
+      </c>
+      <c r="H266" s="2">
+        <v>20</v>
+      </c>
+      <c r="I266" s="2">
+        <v>496</v>
+      </c>
+      <c r="J266" s="2">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data until March 25th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -72,8 +72,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -120,6 +128,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -394,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,11 +413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J266"/>
+  <dimension ref="A1:J268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A267" sqref="A267"/>
+      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A268" sqref="A268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -8935,6 +8946,41 @@
       <c r="J266" s="2">
         <v>51</v>
       </c>
+    </row>
+    <row r="267" spans="1:10">
+      <c r="A267" s="1">
+        <v>44280</v>
+      </c>
+      <c r="B267" s="2">
+        <v>7201</v>
+      </c>
+      <c r="C267" s="2">
+        <v>561</v>
+      </c>
+      <c r="D267" s="2">
+        <v>2265</v>
+      </c>
+      <c r="E267" s="2">
+        <v>10027</v>
+      </c>
+      <c r="F267" s="2">
+        <v>1687</v>
+      </c>
+      <c r="G267" s="2">
+        <v>525</v>
+      </c>
+      <c r="H267" s="2">
+        <v>19</v>
+      </c>
+      <c r="I267" s="2">
+        <v>508</v>
+      </c>
+      <c r="J267" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10">
+      <c r="B268" s="8"/>
     </row>
   </sheetData>
   <sortState ref="A2:J173">

</xml_diff>

<commit_message>
add data until March 26th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -72,16 +72,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,9 +120,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -405,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,9 +404,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A268" sqref="A268"/>
+      <selection pane="bottomLeft" activeCell="C270" sqref="C270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -8980,7 +8969,36 @@
       </c>
     </row>
     <row r="268" spans="1:10">
-      <c r="B268" s="8"/>
+      <c r="A268" s="1">
+        <v>44281</v>
+      </c>
+      <c r="B268" s="7">
+        <v>7296</v>
+      </c>
+      <c r="C268" s="2">
+        <v>513</v>
+      </c>
+      <c r="D268" s="2">
+        <v>2315</v>
+      </c>
+      <c r="E268" s="2">
+        <v>10124</v>
+      </c>
+      <c r="F268" s="2">
+        <v>1721</v>
+      </c>
+      <c r="G268" s="2">
+        <v>539</v>
+      </c>
+      <c r="H268" s="2">
+        <v>19</v>
+      </c>
+      <c r="I268" s="2">
+        <v>520</v>
+      </c>
+      <c r="J268" s="2">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:J173">

</xml_diff>

<commit_message>
add data until March 29th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,11 +402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J268"/>
+  <dimension ref="A1:J271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C270" sqref="C270"/>
+      <selection pane="bottomLeft" activeCell="A272" sqref="A272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -8998,6 +8998,102 @@
       </c>
       <c r="J268" s="2">
         <v>55</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10">
+      <c r="A269" s="1">
+        <v>44282</v>
+      </c>
+      <c r="B269" s="2">
+        <v>7475</v>
+      </c>
+      <c r="C269" s="2">
+        <v>406</v>
+      </c>
+      <c r="D269" s="2">
+        <v>2366</v>
+      </c>
+      <c r="E269" s="2">
+        <v>10247</v>
+      </c>
+      <c r="F269" s="2">
+        <v>1763</v>
+      </c>
+      <c r="G269" s="2">
+        <v>548</v>
+      </c>
+      <c r="H269" s="2">
+        <v>22</v>
+      </c>
+      <c r="I269" s="2">
+        <v>526</v>
+      </c>
+      <c r="J269" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10">
+      <c r="A270" s="1">
+        <v>44283</v>
+      </c>
+      <c r="B270" s="2">
+        <v>7547</v>
+      </c>
+      <c r="C270" s="2">
+        <v>421</v>
+      </c>
+      <c r="D270" s="2">
+        <v>2465</v>
+      </c>
+      <c r="E270" s="2">
+        <v>10433</v>
+      </c>
+      <c r="F270" s="2">
+        <v>1770</v>
+      </c>
+      <c r="G270" s="2">
+        <v>640</v>
+      </c>
+      <c r="H270" s="2">
+        <v>21</v>
+      </c>
+      <c r="I270" s="2">
+        <v>619</v>
+      </c>
+      <c r="J270" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10">
+      <c r="A271" s="1">
+        <v>44284</v>
+      </c>
+      <c r="B271" s="2">
+        <v>7757</v>
+      </c>
+      <c r="C271" s="2">
+        <v>270</v>
+      </c>
+      <c r="D271" s="2">
+        <v>2494</v>
+      </c>
+      <c r="E271" s="2">
+        <v>10521</v>
+      </c>
+      <c r="F271" s="2">
+        <v>1825</v>
+      </c>
+      <c r="G271" s="2">
+        <v>611</v>
+      </c>
+      <c r="H271" s="2">
+        <v>21</v>
+      </c>
+      <c r="I271" s="2">
+        <v>590</v>
+      </c>
+      <c r="J271" s="2">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until March 30
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,11 +402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J271"/>
+  <dimension ref="A1:J272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A272" sqref="A272"/>
+      <selection pane="bottomLeft" activeCell="E273" sqref="E273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -9093,6 +9093,38 @@
         <v>590</v>
       </c>
       <c r="J271" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10">
+      <c r="A272" s="1">
+        <v>44285</v>
+      </c>
+      <c r="B272" s="2">
+        <v>7768</v>
+      </c>
+      <c r="C272" s="2">
+        <v>367</v>
+      </c>
+      <c r="D272" s="2">
+        <v>2507</v>
+      </c>
+      <c r="E272" s="2">
+        <v>10642</v>
+      </c>
+      <c r="F272" s="2">
+        <v>1876</v>
+      </c>
+      <c r="G272" s="2">
+        <v>573</v>
+      </c>
+      <c r="H272" s="2">
+        <v>25</v>
+      </c>
+      <c r="I272" s="2">
+        <v>548</v>
+      </c>
+      <c r="J272" s="2">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add data until April 2nd
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,11 +402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J272"/>
+  <dimension ref="A1:J275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E273" sqref="E273"/>
+      <selection pane="bottomLeft" activeCell="A276" sqref="A276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -9126,6 +9126,102 @@
       </c>
       <c r="J272" s="2">
         <v>58</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10">
+      <c r="A273" s="1">
+        <v>44286</v>
+      </c>
+      <c r="B273" s="2">
+        <v>7819</v>
+      </c>
+      <c r="C273" s="2">
+        <v>469</v>
+      </c>
+      <c r="D273" s="2">
+        <v>2549</v>
+      </c>
+      <c r="E273" s="2">
+        <v>10837</v>
+      </c>
+      <c r="F273" s="2">
+        <v>1918</v>
+      </c>
+      <c r="G273" s="2">
+        <v>573</v>
+      </c>
+      <c r="H273" s="2">
+        <v>25</v>
+      </c>
+      <c r="I273" s="2">
+        <v>548</v>
+      </c>
+      <c r="J273" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10">
+      <c r="A274" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B274" s="2">
+        <v>7935</v>
+      </c>
+      <c r="C274" s="2">
+        <v>374</v>
+      </c>
+      <c r="D274" s="2">
+        <v>2615</v>
+      </c>
+      <c r="E274" s="2">
+        <v>10924</v>
+      </c>
+      <c r="F274" s="2">
+        <v>1977</v>
+      </c>
+      <c r="G274" s="2">
+        <v>578</v>
+      </c>
+      <c r="H274" s="2">
+        <v>25</v>
+      </c>
+      <c r="I274" s="2">
+        <v>553</v>
+      </c>
+      <c r="J274" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10">
+      <c r="A275" s="1">
+        <v>44288</v>
+      </c>
+      <c r="B275" s="2">
+        <v>7982</v>
+      </c>
+      <c r="C275" s="2">
+        <v>350</v>
+      </c>
+      <c r="D275" s="2">
+        <v>2660</v>
+      </c>
+      <c r="E275" s="2">
+        <v>10992</v>
+      </c>
+      <c r="F275" s="2">
+        <v>2036</v>
+      </c>
+      <c r="G275" s="2">
+        <v>564</v>
+      </c>
+      <c r="H275" s="2">
+        <v>25</v>
+      </c>
+      <c r="I275" s="2">
+        <v>539</v>
+      </c>
+      <c r="J275" s="2">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 3th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -394,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,25 +402,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J275"/>
+  <dimension ref="A1:J277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A276" sqref="A276"/>
+      <selection pane="bottomLeft" activeCell="J276" sqref="J276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
@@ -9223,6 +9222,41 @@
       <c r="J275" s="2">
         <v>60</v>
       </c>
+    </row>
+    <row r="276" spans="1:10">
+      <c r="A276" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B276" s="2">
+        <v>7999</v>
+      </c>
+      <c r="C276" s="2">
+        <v>370</v>
+      </c>
+      <c r="D276" s="2">
+        <v>2694</v>
+      </c>
+      <c r="E276" s="2">
+        <v>11063</v>
+      </c>
+      <c r="F276" s="2">
+        <v>2069</v>
+      </c>
+      <c r="G276" s="2">
+        <v>563</v>
+      </c>
+      <c r="H276" s="2">
+        <v>24</v>
+      </c>
+      <c r="I276" s="2">
+        <v>539</v>
+      </c>
+      <c r="J276" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10">
+      <c r="D277" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A2:J173">

</xml_diff>

<commit_message>
add data until April 6th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,7 +187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -217,7 +222,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -394,36 +399,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J277"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J279"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J276" sqref="J276"/>
+      <selection pane="bottomLeft" activeCell="A280" sqref="A280"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -487,7 +492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -519,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -551,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -583,7 +588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -615,7 +620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -647,7 +652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -679,7 +684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -711,7 +716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -743,7 +748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -775,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -807,7 +812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -839,7 +844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -871,7 +876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -903,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -935,7 +940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -967,7 +972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -999,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1063,7 +1068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1095,7 +1100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1127,7 +1132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1159,7 +1164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1191,7 +1196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1223,7 +1228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1255,7 +1260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1287,7 +1292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1319,7 +1324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1351,7 +1356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1383,7 +1388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1415,7 +1420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1447,7 +1452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1479,7 +1484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1511,7 +1516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1543,7 +1548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1575,7 +1580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1607,7 +1612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1639,7 +1644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1671,7 +1676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1703,7 +1708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1735,7 +1740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1767,7 +1772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1799,7 +1804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1831,7 +1836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1863,7 +1868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1895,7 +1900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1927,7 +1932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1959,7 +1964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1991,7 +1996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2023,7 +2028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2055,7 +2060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2087,7 +2092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2119,7 +2124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2151,7 +2156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2183,7 +2188,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2215,7 +2220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2247,7 +2252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2279,7 +2284,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2311,7 +2316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2343,7 +2348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2375,7 +2380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2407,7 +2412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2439,7 +2444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2471,7 +2476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2503,7 +2508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2535,7 +2540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2567,7 +2572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2599,7 +2604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2631,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2663,7 +2668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2695,7 +2700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2727,7 +2732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2759,7 +2764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2791,7 +2796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2823,7 +2828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2855,7 +2860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2887,7 +2892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2919,7 +2924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2951,7 +2956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2983,7 +2988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3015,7 +3020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3047,7 +3052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3079,7 +3084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3111,7 +3116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3143,7 +3148,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3175,7 +3180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3207,7 +3212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3239,7 +3244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3271,7 +3276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3303,7 +3308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3335,7 +3340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3367,7 +3372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3399,7 +3404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3431,7 +3436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3463,7 +3468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3495,7 +3500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3527,7 +3532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3559,7 +3564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3591,7 +3596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3623,7 +3628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3655,7 +3660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3687,7 +3692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3719,7 +3724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3751,7 +3756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3783,7 +3788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3815,7 +3820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3847,7 +3852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3879,7 +3884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3911,7 +3916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3943,7 +3948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3975,7 +3980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4007,7 +4012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4039,7 +4044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4071,7 +4076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4103,7 +4108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4135,7 +4140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4167,7 +4172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4199,7 +4204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4231,7 +4236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4263,7 +4268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4295,7 +4300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4327,7 +4332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4359,7 +4364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4391,7 +4396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4423,7 +4428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4455,7 +4460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4487,7 +4492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4519,7 +4524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4551,7 +4556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4583,7 +4588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4615,7 +4620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4647,7 +4652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4679,7 +4684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4711,7 +4716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4743,7 +4748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4775,7 +4780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4807,7 +4812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4839,7 +4844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4871,7 +4876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4903,7 +4908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4935,7 +4940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4967,7 +4972,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -4999,7 +5004,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5031,7 +5036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5063,7 +5068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5095,7 +5100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5127,7 +5132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5159,7 +5164,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5191,7 +5196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5223,7 +5228,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5255,7 +5260,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5287,7 +5292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5319,7 +5324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5351,7 +5356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5383,7 +5388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5415,7 +5420,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5447,7 +5452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5479,7 +5484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5511,7 +5516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5543,7 +5548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5575,7 +5580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5607,7 +5612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5639,7 +5644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5671,7 +5676,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5703,7 +5708,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5735,7 +5740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5767,7 +5772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5799,7 +5804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5831,7 +5836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5863,7 +5868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5895,7 +5900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5927,7 +5932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5959,7 +5964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5991,7 +5996,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6023,7 +6028,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6055,7 +6060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6087,7 +6092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6119,7 +6124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6151,7 +6156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6183,7 +6188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6215,7 +6220,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6247,7 +6252,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6279,7 +6284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6311,7 +6316,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6343,7 +6348,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6375,7 +6380,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6407,7 +6412,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6439,7 +6444,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6471,7 +6476,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6503,7 +6508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6535,7 +6540,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6567,7 +6572,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6599,7 +6604,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6631,7 +6636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6663,7 +6668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6695,7 +6700,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6727,7 +6732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6759,7 +6764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6791,7 +6796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6823,7 +6828,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6855,7 +6860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6887,7 +6892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6919,7 +6924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6951,7 +6956,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6983,7 +6988,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7015,7 +7020,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7047,7 +7052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7079,7 +7084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7111,7 +7116,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7143,7 +7148,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7175,7 +7180,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7207,7 +7212,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7239,7 +7244,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7271,7 +7276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7303,7 +7308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7335,7 +7340,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7367,7 +7372,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7399,7 +7404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7431,7 +7436,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7463,7 +7468,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7495,7 +7500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7527,7 +7532,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7559,7 +7564,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7591,7 +7596,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7623,7 +7628,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7655,7 +7660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7687,7 +7692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7719,7 +7724,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7751,7 +7756,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7783,7 +7788,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7815,7 +7820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7847,7 +7852,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7879,7 +7884,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7911,7 +7916,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7943,7 +7948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7975,7 +7980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8007,7 +8012,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8039,7 +8044,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8071,7 +8076,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8103,7 +8108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8135,7 +8140,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8167,7 +8172,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8199,7 +8204,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8231,7 +8236,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8263,7 +8268,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8295,7 +8300,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8327,7 +8332,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8359,7 +8364,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8391,7 +8396,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8423,7 +8428,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8455,7 +8460,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8487,7 +8492,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8519,7 +8524,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8551,7 +8556,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8583,7 +8588,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8615,7 +8620,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8647,7 +8652,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8679,7 +8684,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8711,7 +8716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8743,7 +8748,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8775,7 +8780,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8807,7 +8812,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8839,7 +8844,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8871,7 +8876,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8903,7 +8908,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8935,7 +8940,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8967,7 +8972,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -8999,7 +9004,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9031,7 +9036,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9063,7 +9068,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9095,7 +9100,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9127,7 +9132,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9159,7 +9164,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9191,7 +9196,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9223,7 +9228,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9255,8 +9260,101 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
-      <c r="D277" s="7"/>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B277" s="2">
+        <v>8139</v>
+      </c>
+      <c r="C277" s="2">
+        <v>289</v>
+      </c>
+      <c r="D277" s="7">
+        <v>2711</v>
+      </c>
+      <c r="E277" s="2">
+        <v>11139</v>
+      </c>
+      <c r="F277" s="2">
+        <v>2082</v>
+      </c>
+      <c r="G277" s="2">
+        <v>565</v>
+      </c>
+      <c r="H277" s="2">
+        <v>23</v>
+      </c>
+      <c r="I277" s="2">
+        <v>542</v>
+      </c>
+      <c r="J277" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>44291</v>
+      </c>
+      <c r="B278" s="2">
+        <v>8139</v>
+      </c>
+      <c r="C278" s="2">
+        <v>350</v>
+      </c>
+      <c r="D278" s="2">
+        <v>2721</v>
+      </c>
+      <c r="E278" s="2">
+        <v>11210</v>
+      </c>
+      <c r="F278" s="2">
+        <v>2158</v>
+      </c>
+      <c r="G278" s="2">
+        <v>499</v>
+      </c>
+      <c r="H278" s="2">
+        <v>23</v>
+      </c>
+      <c r="I278" s="2">
+        <v>476</v>
+      </c>
+      <c r="J278" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B279" s="2">
+        <v>8140</v>
+      </c>
+      <c r="C279" s="2">
+        <v>362</v>
+      </c>
+      <c r="D279" s="2">
+        <v>2737</v>
+      </c>
+      <c r="E279" s="2">
+        <v>11239</v>
+      </c>
+      <c r="F279" s="2">
+        <v>2232</v>
+      </c>
+      <c r="G279" s="2">
+        <v>440</v>
+      </c>
+      <c r="H279" s="2">
+        <v>23</v>
+      </c>
+      <c r="I279" s="2">
+        <v>417</v>
+      </c>
+      <c r="J279" s="2">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:J173">
@@ -9268,29 +9366,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9325,7 +9423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9348,7 +9446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9371,7 +9469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9394,7 +9492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9417,7 +9515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9440,7 +9538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9463,7 +9561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9483,7 +9581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9503,7 +9601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9523,7 +9621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9543,7 +9641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9563,12 +9661,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -9588,7 +9686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -9608,7 +9706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -9628,7 +9726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -9648,7 +9746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -9668,7 +9766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -9688,7 +9786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -9708,7 +9806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -9728,7 +9826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -9748,7 +9846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -9756,7 +9854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -9779,7 +9877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -9799,7 +9897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -9819,7 +9917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -9839,17 +9937,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -9869,7 +9967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -9892,7 +9990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -9915,7 +10013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -9935,7 +10033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -9961,267 +10059,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 8th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,9 +71,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -106,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -125,6 +128,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -187,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -222,7 +228,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -399,36 +405,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J279"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A280" sqref="A280"/>
+      <selection pane="bottomLeft" activeCell="A282" sqref="A282"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -492,7 +498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -524,7 +530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -556,7 +562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -588,7 +594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -620,7 +626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -652,7 +658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -684,7 +690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -716,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -748,7 +754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -780,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -812,7 +818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -844,7 +850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -876,7 +882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -908,7 +914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -940,7 +946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -972,7 +978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1036,7 +1042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1420,7 +1426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1452,7 +1458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1612,7 +1618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1644,7 +1650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1676,7 +1682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1708,7 +1714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1772,7 +1778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1836,7 +1842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1868,7 +1874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1900,7 +1906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1932,7 +1938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1964,7 +1970,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2028,7 +2034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2060,7 +2066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2124,7 +2130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2156,7 +2162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2188,7 +2194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2220,7 +2226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2252,7 +2258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2284,7 +2290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2316,7 +2322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2348,7 +2354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2380,7 +2386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2476,7 +2482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2508,7 +2514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2540,7 +2546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2572,7 +2578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2604,7 +2610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2668,7 +2674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2700,7 +2706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2732,7 +2738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2764,7 +2770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2796,7 +2802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2828,7 +2834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2860,7 +2866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2892,7 +2898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2956,7 +2962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2988,7 +2994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3020,7 +3026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3052,7 +3058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3084,7 +3090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3148,7 +3154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3180,7 +3186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3212,7 +3218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3244,7 +3250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3308,7 +3314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3340,7 +3346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3404,7 +3410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3436,7 +3442,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3468,7 +3474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3500,7 +3506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3532,7 +3538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3564,7 +3570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3596,7 +3602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3628,7 +3634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3660,7 +3666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3692,7 +3698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3756,7 +3762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3788,7 +3794,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3852,7 +3858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3884,7 +3890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3916,7 +3922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3948,7 +3954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3980,7 +3986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4012,7 +4018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4044,7 +4050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4076,7 +4082,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4108,7 +4114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4140,7 +4146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4172,7 +4178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4204,7 +4210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4300,7 +4306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4332,7 +4338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4364,7 +4370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4396,7 +4402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4428,7 +4434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4460,7 +4466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4492,7 +4498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4524,7 +4530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4556,7 +4562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4588,7 +4594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4620,7 +4626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4652,7 +4658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4684,7 +4690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4716,7 +4722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4748,7 +4754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4780,7 +4786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4812,7 +4818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4844,7 +4850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4876,7 +4882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4908,7 +4914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4940,7 +4946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4972,7 +4978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5004,7 +5010,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5036,7 +5042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5068,7 +5074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5100,7 +5106,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5132,7 +5138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5164,7 +5170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5196,7 +5202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5228,7 +5234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5260,7 +5266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5292,7 +5298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5324,7 +5330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5356,7 +5362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5388,7 +5394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5420,7 +5426,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5452,7 +5458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5484,7 +5490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5516,7 +5522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5548,7 +5554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5580,7 +5586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5612,7 +5618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5644,7 +5650,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5676,7 +5682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5708,7 +5714,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5740,7 +5746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5772,7 +5778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5804,7 +5810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5836,7 +5842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5868,7 +5874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5900,7 +5906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5932,7 +5938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5964,7 +5970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5996,7 +6002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6028,7 +6034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6060,7 +6066,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6092,7 +6098,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6124,7 +6130,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6156,7 +6162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6188,7 +6194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6220,7 +6226,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6252,7 +6258,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6284,7 +6290,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6316,7 +6322,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6348,7 +6354,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6380,7 +6386,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6412,7 +6418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6444,7 +6450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6476,7 +6482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6508,7 +6514,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6540,7 +6546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6572,7 +6578,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6604,7 +6610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6636,7 +6642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6668,7 +6674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6700,7 +6706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6732,7 +6738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6764,7 +6770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6796,7 +6802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6828,7 +6834,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6860,7 +6866,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6892,7 +6898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6924,7 +6930,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6956,7 +6962,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6988,7 +6994,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7020,7 +7026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7052,7 +7058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7084,7 +7090,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7116,7 +7122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7148,7 +7154,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7180,7 +7186,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7212,7 +7218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7244,7 +7250,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7276,7 +7282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7308,7 +7314,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7340,7 +7346,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7372,7 +7378,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7404,7 +7410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7436,7 +7442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7468,7 +7474,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7500,7 +7506,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7532,7 +7538,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7564,7 +7570,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7596,7 +7602,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7628,7 +7634,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7660,7 +7666,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7692,7 +7698,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7724,7 +7730,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7756,7 +7762,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7788,7 +7794,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7820,7 +7826,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7852,7 +7858,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7884,7 +7890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7916,7 +7922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7948,7 +7954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7980,7 +7986,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8012,7 +8018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8044,7 +8050,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8076,7 +8082,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8108,7 +8114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8140,7 +8146,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8172,7 +8178,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8204,7 +8210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8236,7 +8242,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8268,7 +8274,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8300,7 +8306,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8332,7 +8338,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8364,7 +8370,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8396,7 +8402,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8428,7 +8434,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8460,7 +8466,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8492,7 +8498,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8524,7 +8530,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8556,7 +8562,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8588,7 +8594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8620,7 +8626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8652,7 +8658,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8684,7 +8690,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8716,7 +8722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8748,7 +8754,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8780,7 +8786,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8812,7 +8818,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8844,7 +8850,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8876,7 +8882,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8908,7 +8914,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8940,7 +8946,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8972,7 +8978,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9004,7 +9010,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9036,7 +9042,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9068,7 +9074,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9100,7 +9106,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9132,7 +9138,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9164,7 +9170,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9196,7 +9202,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9228,7 +9234,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9260,7 +9266,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9292,7 +9298,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9324,7 +9330,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9355,6 +9361,73 @@
       <c r="J279" s="2">
         <v>65</v>
       </c>
+    </row>
+    <row r="280" spans="1:10">
+      <c r="A280" s="1">
+        <v>44293</v>
+      </c>
+      <c r="B280" s="2">
+        <v>8193</v>
+      </c>
+      <c r="C280" s="2">
+        <v>375</v>
+      </c>
+      <c r="D280" s="2">
+        <v>2772</v>
+      </c>
+      <c r="E280" s="2">
+        <v>11340</v>
+      </c>
+      <c r="F280" s="2">
+        <v>2302</v>
+      </c>
+      <c r="G280" s="2">
+        <v>403</v>
+      </c>
+      <c r="H280" s="2">
+        <v>23</v>
+      </c>
+      <c r="I280" s="2">
+        <v>380</v>
+      </c>
+      <c r="J280" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10">
+      <c r="A281" s="1">
+        <v>44294</v>
+      </c>
+      <c r="B281" s="2">
+        <v>8239</v>
+      </c>
+      <c r="C281" s="2">
+        <v>345</v>
+      </c>
+      <c r="D281" s="2">
+        <v>2821</v>
+      </c>
+      <c r="E281" s="2">
+        <v>11405</v>
+      </c>
+      <c r="F281" s="2">
+        <v>2361</v>
+      </c>
+      <c r="G281" s="2">
+        <v>392</v>
+      </c>
+      <c r="H281" s="2">
+        <v>25</v>
+      </c>
+      <c r="I281" s="2">
+        <v>367</v>
+      </c>
+      <c r="J281" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10">
+      <c r="A282" s="8"/>
     </row>
   </sheetData>
   <sortState ref="A2:J173">
@@ -9366,29 +9439,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9423,7 +9496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9446,7 +9519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9469,7 +9542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9492,7 +9565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9515,7 +9588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9538,7 +9611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9561,7 +9634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9581,7 +9654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9601,7 +9674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9621,7 +9694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9641,7 +9714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9661,12 +9734,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -9686,7 +9759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -9706,7 +9779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -9726,7 +9799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -9746,7 +9819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -9766,7 +9839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -9786,7 +9859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -9806,7 +9879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -9826,7 +9899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -9846,7 +9919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -9854,7 +9927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -9877,7 +9950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -9897,7 +9970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -9917,7 +9990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -9937,17 +10010,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -9967,7 +10040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -9990,7 +10063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10013,7 +10086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10033,7 +10106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10059,267 +10132,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 10th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -72,16 +72,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -130,7 +122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -413,11 +405,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J282"/>
+  <dimension ref="A1:J283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A282" sqref="A282"/>
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A284" sqref="A284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -9427,7 +9419,68 @@
       </c>
     </row>
     <row r="282" spans="1:10">
-      <c r="A282" s="8"/>
+      <c r="A282" s="8">
+        <v>44295</v>
+      </c>
+      <c r="B282" s="2">
+        <v>8350</v>
+      </c>
+      <c r="C282" s="2">
+        <v>258</v>
+      </c>
+      <c r="D282" s="2">
+        <v>2900</v>
+      </c>
+      <c r="E282" s="2">
+        <v>11508</v>
+      </c>
+      <c r="F282" s="2">
+        <v>2403</v>
+      </c>
+      <c r="G282" s="2">
+        <v>427</v>
+      </c>
+      <c r="H282" s="2">
+        <v>24</v>
+      </c>
+      <c r="I282" s="2">
+        <v>403</v>
+      </c>
+      <c r="J282" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10">
+      <c r="A283" s="1">
+        <v>44296</v>
+      </c>
+      <c r="B283" s="2">
+        <v>8443</v>
+      </c>
+      <c r="C283" s="2">
+        <v>199</v>
+      </c>
+      <c r="D283" s="2">
+        <v>2948</v>
+      </c>
+      <c r="E283" s="2">
+        <v>11580</v>
+      </c>
+      <c r="F283" s="2">
+        <v>2446</v>
+      </c>
+      <c r="G283" s="2">
+        <v>431</v>
+      </c>
+      <c r="H283" s="2">
+        <v>23</v>
+      </c>
+      <c r="I283" s="2">
+        <v>408</v>
+      </c>
+      <c r="J283" s="2">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:J173">

</xml_diff>

<commit_message>
add data until April 11th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,36 +402,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J283"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A284" sqref="A284"/>
+      <selection pane="bottomLeft" activeCell="J284" sqref="J284"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +5007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5359,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7082,7 +7087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7114,7 +7119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7146,7 +7151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7178,7 +7183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7210,7 +7215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7242,7 +7247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7274,7 +7279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7306,7 +7311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7338,7 +7343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7402,7 +7407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7434,7 +7439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7466,7 +7471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7498,7 +7503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7530,7 +7535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7562,7 +7567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7594,7 +7599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7626,7 +7631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7658,7 +7663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7690,7 +7695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7722,7 +7727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7754,7 +7759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7786,7 +7791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7818,7 +7823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7850,7 +7855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7882,7 +7887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7914,7 +7919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7946,7 +7951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7978,7 +7983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8010,7 +8015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8042,7 +8047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8074,7 +8079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8106,7 +8111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8138,7 +8143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8170,7 +8175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8202,7 +8207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8234,7 +8239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8266,7 +8271,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8298,7 +8303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8330,7 +8335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8362,7 +8367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8394,7 +8399,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8426,7 +8431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8458,7 +8463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8490,7 +8495,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8522,7 +8527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8554,7 +8559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8586,7 +8591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8618,7 +8623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8650,7 +8655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8682,7 +8687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8714,7 +8719,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8746,7 +8751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8778,7 +8783,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8810,7 +8815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8842,7 +8847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8874,7 +8879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8906,7 +8911,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8938,7 +8943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8970,7 +8975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9002,7 +9007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9034,7 +9039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9066,7 +9071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9098,7 +9103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9130,7 +9135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9162,7 +9167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9194,7 +9199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9226,7 +9231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9258,7 +9263,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9290,7 +9295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9322,7 +9327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9354,7 +9359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9386,7 +9391,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9418,7 +9423,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9450,7 +9455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9480,6 +9485,38 @@
       </c>
       <c r="J283" s="2">
         <v>71</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>44297</v>
+      </c>
+      <c r="B284" s="2">
+        <v>8461</v>
+      </c>
+      <c r="C284" s="2">
+        <v>160</v>
+      </c>
+      <c r="D284" s="2">
+        <v>2959</v>
+      </c>
+      <c r="E284" s="2">
+        <v>11580</v>
+      </c>
+      <c r="F284" s="2">
+        <v>2446</v>
+      </c>
+      <c r="G284" s="2">
+        <v>441</v>
+      </c>
+      <c r="H284" s="2">
+        <v>23</v>
+      </c>
+      <c r="I284" s="2">
+        <v>418</v>
+      </c>
+      <c r="J284" s="2">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -9492,29 +9529,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9549,7 +9586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9572,7 +9609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9595,7 +9632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9618,7 +9655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9641,7 +9678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9664,7 +9701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9687,7 +9724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9707,7 +9744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9727,7 +9764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9747,7 +9784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9767,7 +9804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9787,12 +9824,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -9812,7 +9849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -9832,7 +9869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -9852,7 +9889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -9872,7 +9909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -9892,7 +9929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -9912,7 +9949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -9932,7 +9969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -9952,7 +9989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -9972,7 +10009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -9980,7 +10017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10003,7 +10040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10023,7 +10060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10043,7 +10080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10063,17 +10100,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10093,7 +10130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10116,7 +10153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10139,7 +10176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10159,7 +10196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10185,267 +10222,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 12th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -190,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -225,7 +225,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -410,11 +410,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J284"/>
+  <dimension ref="A1:J285"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J284" sqref="J284"/>
+      <selection pane="bottomLeft" activeCell="A286" sqref="A286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9516,6 +9516,38 @@
         <v>418</v>
       </c>
       <c r="J284" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>44298</v>
+      </c>
+      <c r="B285" s="2">
+        <v>8489</v>
+      </c>
+      <c r="C285" s="2">
+        <v>202</v>
+      </c>
+      <c r="D285" s="2">
+        <v>2974</v>
+      </c>
+      <c r="E285" s="2">
+        <v>11665</v>
+      </c>
+      <c r="F285" s="2">
+        <v>2490</v>
+      </c>
+      <c r="G285" s="2">
+        <v>412</v>
+      </c>
+      <c r="H285" s="2">
+        <v>23</v>
+      </c>
+      <c r="I285" s="2">
+        <v>389</v>
+      </c>
+      <c r="J285" s="2">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add data until April 13th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -225,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -402,36 +397,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J285"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A286" sqref="A286"/>
+      <selection pane="bottomLeft" activeCell="B287" sqref="B287"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -495,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -527,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -559,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -591,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -623,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -655,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -687,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -719,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -751,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -783,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -815,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -847,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -879,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -911,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -943,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -975,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1007,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1039,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1071,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1103,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1167,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1199,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1231,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1263,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1295,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1359,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1391,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1423,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1487,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1519,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1551,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1583,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1615,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1647,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1679,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1711,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1743,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1807,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1839,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1871,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1903,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1935,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1967,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2031,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2063,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2095,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2127,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2159,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2191,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2255,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2287,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2319,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2383,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2415,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2447,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2479,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2543,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2575,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2607,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2639,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2671,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2703,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2735,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2767,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2799,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2831,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2863,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2895,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2927,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3023,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3055,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3087,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3119,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3151,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3183,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3279,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3311,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3343,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3375,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3407,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3439,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3471,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3535,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3567,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3599,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3663,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3695,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3759,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3823,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3855,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3887,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3919,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3951,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3983,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4015,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4047,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4079,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4111,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4143,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4175,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4207,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4239,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4399,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4431,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4463,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4495,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4527,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4559,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4623,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4655,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4687,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4719,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4751,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4783,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4815,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4847,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4879,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4911,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4943,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4975,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5039,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5071,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5103,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5135,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5167,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5199,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5231,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5263,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5295,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5327,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5359,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5391,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5423,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5455,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5519,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5551,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5583,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5615,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5647,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5679,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5711,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5743,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5775,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5807,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5839,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5903,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5935,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5967,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5999,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6031,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6063,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6095,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6127,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6159,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6191,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6223,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6255,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6287,7 +6282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6319,7 +6314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6351,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6383,7 +6378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6415,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6447,7 +6442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6479,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6511,7 +6506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6543,7 +6538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6607,7 +6602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6639,7 +6634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6671,7 +6666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6703,7 +6698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6735,7 +6730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6767,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6799,7 +6794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6831,7 +6826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6863,7 +6858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6895,7 +6890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6927,7 +6922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6959,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6991,7 +6986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7023,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7055,7 +7050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7087,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7119,7 +7114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7151,7 +7146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7183,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7215,7 +7210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7247,7 +7242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7279,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7343,7 +7338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7375,7 +7370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7407,7 +7402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7439,7 +7434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7471,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7503,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7535,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7567,7 +7562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7599,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7631,7 +7626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7663,7 +7658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7695,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7727,7 +7722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7759,7 +7754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7791,7 +7786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7823,7 +7818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7855,7 +7850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7887,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7919,7 +7914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7951,7 +7946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7983,7 +7978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8015,7 +8010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8047,7 +8042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8079,7 +8074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8111,7 +8106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8143,7 +8138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8175,7 +8170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8207,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8239,7 +8234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8271,7 +8266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8303,7 +8298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8335,7 +8330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8367,7 +8362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8399,7 +8394,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8431,7 +8426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8463,7 +8458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8495,7 +8490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8527,7 +8522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8559,7 +8554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8591,7 +8586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8623,7 +8618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8655,7 +8650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8687,7 +8682,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8719,7 +8714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8751,7 +8746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8783,7 +8778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8815,7 +8810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8847,7 +8842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8879,7 +8874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8911,7 +8906,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8943,7 +8938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8975,7 +8970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9007,7 +9002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9039,7 +9034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9071,7 +9066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9103,7 +9098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9135,7 +9130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9167,7 +9162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9199,7 +9194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9231,7 +9226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9263,7 +9258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9295,7 +9290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9327,7 +9322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9359,7 +9354,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9391,7 +9386,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9423,7 +9418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9455,7 +9450,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9487,7 +9482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9519,7 +9514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9549,6 +9544,38 @@
       </c>
       <c r="J285" s="2">
         <v>72</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10">
+      <c r="A286" s="1">
+        <v>44299</v>
+      </c>
+      <c r="B286" s="2">
+        <v>8513</v>
+      </c>
+      <c r="C286" s="2">
+        <v>219</v>
+      </c>
+      <c r="D286" s="2">
+        <v>3031</v>
+      </c>
+      <c r="E286" s="2">
+        <v>11763</v>
+      </c>
+      <c r="F286" s="2">
+        <v>2543</v>
+      </c>
+      <c r="G286" s="2">
+        <v>415</v>
+      </c>
+      <c r="H286" s="2">
+        <v>22</v>
+      </c>
+      <c r="I286" s="2">
+        <v>393</v>
+      </c>
+      <c r="J286" s="2">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -9561,29 +9588,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9618,7 +9645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9641,7 +9668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9664,7 +9691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9687,7 +9714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9710,7 +9737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9733,7 +9760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9756,7 +9783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9776,7 +9803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9796,7 +9823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9816,7 +9843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9836,7 +9863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9856,12 +9883,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -9881,7 +9908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -9901,7 +9928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -9921,7 +9948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -9941,7 +9968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -9961,7 +9988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -9981,7 +10008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10001,7 +10028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10021,7 +10048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10041,7 +10068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10049,7 +10076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10072,7 +10099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10092,7 +10119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10112,7 +10139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10132,17 +10159,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10162,7 +10189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10185,7 +10212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10208,7 +10235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10228,7 +10255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10254,267 +10281,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 14th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,36 +402,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J286"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B287" sqref="B287"/>
+      <selection pane="bottomLeft" activeCell="J274" sqref="J274"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +5007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5359,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7082,7 +7087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7114,7 +7119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7146,7 +7151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7178,7 +7183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7210,7 +7215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7242,7 +7247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7274,7 +7279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7306,7 +7311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7338,7 +7343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7402,7 +7407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7434,7 +7439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7466,7 +7471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7498,7 +7503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7530,7 +7535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7562,7 +7567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7594,7 +7599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7626,7 +7631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7658,7 +7663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7690,7 +7695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7722,7 +7727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7754,7 +7759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7786,7 +7791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7818,7 +7823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7850,7 +7855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7882,7 +7887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7914,7 +7919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7946,7 +7951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7978,7 +7983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8010,7 +8015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8042,7 +8047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8074,7 +8079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8106,7 +8111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8138,7 +8143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8170,7 +8175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8202,7 +8207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8234,7 +8239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8266,7 +8271,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8298,7 +8303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8330,7 +8335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8362,7 +8367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8394,7 +8399,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8426,7 +8431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8458,7 +8463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8490,7 +8495,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8522,7 +8527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8554,7 +8559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8586,7 +8591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8618,7 +8623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8650,7 +8655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8682,7 +8687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8714,7 +8719,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8746,7 +8751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8778,7 +8783,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8810,7 +8815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8842,7 +8847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8874,7 +8879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8906,7 +8911,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8938,7 +8943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8970,7 +8975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9002,7 +9007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9034,7 +9039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9066,7 +9071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9098,7 +9103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9130,7 +9135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9162,7 +9167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9194,7 +9199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9226,7 +9231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9258,7 +9263,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9290,7 +9295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9322,7 +9327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9354,7 +9359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9386,7 +9391,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9418,7 +9423,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9450,7 +9455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9482,7 +9487,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9514,7 +9519,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9546,7 +9551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9576,6 +9581,38 @@
       </c>
       <c r="J286" s="2">
         <v>73</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
+        <v>44300</v>
+      </c>
+      <c r="B287" s="2">
+        <v>8585</v>
+      </c>
+      <c r="C287" s="2">
+        <v>241</v>
+      </c>
+      <c r="D287" s="2">
+        <v>3073</v>
+      </c>
+      <c r="E287" s="2">
+        <v>11899</v>
+      </c>
+      <c r="F287" s="2">
+        <v>2621</v>
+      </c>
+      <c r="G287" s="2">
+        <v>376</v>
+      </c>
+      <c r="H287" s="2">
+        <v>23</v>
+      </c>
+      <c r="I287" s="2">
+        <v>353</v>
+      </c>
+      <c r="J287" s="2">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -9588,29 +9625,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9645,7 +9682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9668,7 +9705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9691,7 +9728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9714,7 +9751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9737,7 +9774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9760,7 +9797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9783,7 +9820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9803,7 +9840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9823,7 +9860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9843,7 +9880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9863,7 +9900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9883,12 +9920,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -9908,7 +9945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -9928,7 +9965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -9948,7 +9985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -9968,7 +10005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -9988,7 +10025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10008,7 +10045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10028,7 +10065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10048,7 +10085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10068,7 +10105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10076,7 +10113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10099,7 +10136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10119,7 +10156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10139,7 +10176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10159,17 +10196,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10189,7 +10226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10212,7 +10249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10235,7 +10272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10255,7 +10292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10281,267 +10318,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 15th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -190,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -225,7 +225,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -410,11 +410,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J287"/>
+  <dimension ref="A1:J288"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J274" sqref="J274"/>
+      <selection pane="bottomLeft" activeCell="H287" sqref="H287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9613,6 +9613,38 @@
       </c>
       <c r="J287" s="2">
         <v>76</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>44301</v>
+      </c>
+      <c r="B288" s="2">
+        <v>8704</v>
+      </c>
+      <c r="C288" s="2">
+        <v>184</v>
+      </c>
+      <c r="D288" s="2">
+        <v>3117</v>
+      </c>
+      <c r="E288" s="2">
+        <v>12005</v>
+      </c>
+      <c r="F288" s="2">
+        <v>2654</v>
+      </c>
+      <c r="G288" s="2">
+        <v>386</v>
+      </c>
+      <c r="H288" s="2">
+        <v>21</v>
+      </c>
+      <c r="I288" s="2">
+        <v>365</v>
+      </c>
+      <c r="J288" s="2">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data April, 16th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -225,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -402,36 +397,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J288"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H287" sqref="H287"/>
+      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A290" sqref="A290"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -495,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -527,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -559,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -591,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -623,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -655,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -687,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -719,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -751,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -783,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -815,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -847,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -879,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -911,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -943,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -975,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1007,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1039,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1071,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1103,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1167,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1199,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1231,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1263,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1295,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1359,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1391,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1423,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1487,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1519,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1551,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1583,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1615,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1647,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1679,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1711,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1743,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1807,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1839,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1871,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1903,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1935,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1967,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2031,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2063,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2095,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2127,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2159,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2191,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2255,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2287,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2319,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2383,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2415,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2447,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2479,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2543,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2575,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2607,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2639,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2671,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2703,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2735,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2767,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2799,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2831,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2863,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2895,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2927,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3023,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3055,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3087,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3119,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3151,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3183,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3279,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3311,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3343,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3375,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3407,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3439,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3471,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3535,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3567,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3599,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3663,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3695,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3759,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3823,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3855,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3887,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3919,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3951,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3983,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4015,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4047,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4079,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4111,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4143,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4175,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4207,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4239,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4399,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4431,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4463,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4495,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4527,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4559,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4623,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4655,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4687,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4719,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4751,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4783,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4815,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4847,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4879,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4911,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4943,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4975,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5039,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5071,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5103,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5135,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5167,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5199,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5231,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5263,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5295,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5327,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5359,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5391,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5423,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5455,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5519,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5551,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5583,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5615,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5647,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5679,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5711,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5743,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5775,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5807,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5839,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5903,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5935,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5967,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5999,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6031,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6063,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6095,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6127,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6159,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6191,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6223,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6255,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6287,7 +6282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6319,7 +6314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6351,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6383,7 +6378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6415,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6447,7 +6442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6479,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6511,7 +6506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6543,7 +6538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6607,7 +6602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6639,7 +6634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6671,7 +6666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6703,7 +6698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6735,7 +6730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6767,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6799,7 +6794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6831,7 +6826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6863,7 +6858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6895,7 +6890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6927,7 +6922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6959,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6991,7 +6986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7023,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7055,7 +7050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7087,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7119,7 +7114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7151,7 +7146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7183,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7215,7 +7210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7247,7 +7242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7279,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7343,7 +7338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7375,7 +7370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7407,7 +7402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7439,7 +7434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7471,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7503,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7535,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7567,7 +7562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7599,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7631,7 +7626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7663,7 +7658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7695,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7727,7 +7722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7759,7 +7754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7791,7 +7786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7823,7 +7818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7855,7 +7850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7887,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7919,7 +7914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7951,7 +7946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7983,7 +7978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8015,7 +8010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8047,7 +8042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8079,7 +8074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8111,7 +8106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8143,7 +8138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8175,7 +8170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8207,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8239,7 +8234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8271,7 +8266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8303,7 +8298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8335,7 +8330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8367,7 +8362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8399,7 +8394,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8431,7 +8426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8463,7 +8458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8495,7 +8490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8527,7 +8522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8559,7 +8554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8591,7 +8586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8623,7 +8618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8655,7 +8650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8687,7 +8682,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8719,7 +8714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8751,7 +8746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8783,7 +8778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8815,7 +8810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8847,7 +8842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8879,7 +8874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8911,7 +8906,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8943,7 +8938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8975,7 +8970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9007,7 +9002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9039,7 +9034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9071,7 +9066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9103,7 +9098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9135,7 +9130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9167,7 +9162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9199,7 +9194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9231,7 +9226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9263,7 +9258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9295,7 +9290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9327,7 +9322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9359,7 +9354,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9391,7 +9386,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9423,7 +9418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9455,7 +9450,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9487,7 +9482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9519,7 +9514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9551,7 +9546,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9583,7 +9578,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9615,7 +9610,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9645,6 +9640,38 @@
       </c>
       <c r="J288" s="2">
         <v>77</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10">
+      <c r="A289" s="1">
+        <v>44302</v>
+      </c>
+      <c r="B289" s="2">
+        <v>8754</v>
+      </c>
+      <c r="C289" s="2">
+        <v>190</v>
+      </c>
+      <c r="D289" s="2">
+        <v>3157</v>
+      </c>
+      <c r="E289" s="2">
+        <v>12101</v>
+      </c>
+      <c r="F289" s="2">
+        <v>2672</v>
+      </c>
+      <c r="G289" s="2">
+        <v>407</v>
+      </c>
+      <c r="H289" s="2">
+        <v>21</v>
+      </c>
+      <c r="I289" s="2">
+        <v>386</v>
+      </c>
+      <c r="J289" s="2">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -9657,29 +9684,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9714,7 +9741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9737,7 +9764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9760,7 +9787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9783,7 +9810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9806,7 +9833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9829,7 +9856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9852,7 +9879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9872,7 +9899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9892,7 +9919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9912,7 +9939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9932,7 +9959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9952,12 +9979,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -9977,7 +10004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -9997,7 +10024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10017,7 +10044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10037,7 +10064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10057,7 +10084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10077,7 +10104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10097,7 +10124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10117,7 +10144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10137,7 +10164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10145,7 +10172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10168,7 +10195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10188,7 +10215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10208,7 +10235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10228,17 +10255,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10258,7 +10285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10281,7 +10308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10304,7 +10331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10324,7 +10351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10350,267 +10377,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 19th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,36 +402,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J289"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A290" sqref="A290"/>
+      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B293" sqref="B293"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +5007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5359,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7082,7 +7087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7114,7 +7119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7146,7 +7151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7178,7 +7183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7210,7 +7215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7242,7 +7247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7274,7 +7279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7306,7 +7311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7338,7 +7343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7402,7 +7407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7434,7 +7439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7466,7 +7471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7498,7 +7503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7530,7 +7535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7562,7 +7567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7594,7 +7599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7626,7 +7631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7658,7 +7663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7690,7 +7695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7722,7 +7727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7754,7 +7759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7786,7 +7791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7818,7 +7823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7850,7 +7855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7882,7 +7887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7914,7 +7919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7946,7 +7951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7978,7 +7983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8010,7 +8015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8042,7 +8047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8074,7 +8079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8106,7 +8111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8138,7 +8143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8170,7 +8175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8202,7 +8207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8234,7 +8239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8266,7 +8271,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8298,7 +8303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8330,7 +8335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8362,7 +8367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8394,7 +8399,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8426,7 +8431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8458,7 +8463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8490,7 +8495,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8522,7 +8527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8554,7 +8559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8586,7 +8591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8618,7 +8623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8650,7 +8655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8682,7 +8687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8714,7 +8719,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8746,7 +8751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8778,7 +8783,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8810,7 +8815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8842,7 +8847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8874,7 +8879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8906,7 +8911,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8938,7 +8943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8970,7 +8975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9002,7 +9007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9034,7 +9039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9066,7 +9071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9098,7 +9103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9130,7 +9135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9162,7 +9167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9194,7 +9199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9226,7 +9231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9258,7 +9263,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9290,7 +9295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9322,7 +9327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9354,7 +9359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9386,7 +9391,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9418,7 +9423,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9450,7 +9455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9482,7 +9487,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9514,7 +9519,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9546,7 +9551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9578,7 +9583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9610,7 +9615,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9642,7 +9647,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>44302</v>
       </c>
@@ -9672,6 +9677,102 @@
       </c>
       <c r="J289" s="2">
         <v>78</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>44303</v>
+      </c>
+      <c r="B290" s="2">
+        <v>8806</v>
+      </c>
+      <c r="C290" s="2">
+        <v>174</v>
+      </c>
+      <c r="D290" s="2">
+        <v>3187</v>
+      </c>
+      <c r="E290" s="2">
+        <v>12167</v>
+      </c>
+      <c r="F290" s="2">
+        <v>2685</v>
+      </c>
+      <c r="G290" s="2">
+        <v>424</v>
+      </c>
+      <c r="H290" s="2">
+        <v>21</v>
+      </c>
+      <c r="I290" s="2">
+        <v>403</v>
+      </c>
+      <c r="J290" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>44304</v>
+      </c>
+      <c r="B291" s="2">
+        <v>8832</v>
+      </c>
+      <c r="C291" s="2">
+        <v>123</v>
+      </c>
+      <c r="D291" s="2">
+        <v>3212</v>
+      </c>
+      <c r="E291" s="2">
+        <v>12167</v>
+      </c>
+      <c r="F291" s="2">
+        <v>2689</v>
+      </c>
+      <c r="G291" s="2">
+        <v>444</v>
+      </c>
+      <c r="H291" s="2">
+        <v>20</v>
+      </c>
+      <c r="I291" s="2">
+        <v>424</v>
+      </c>
+      <c r="J291" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B292" s="2">
+        <v>8874</v>
+      </c>
+      <c r="C292" s="2">
+        <v>145</v>
+      </c>
+      <c r="D292" s="2">
+        <v>3222</v>
+      </c>
+      <c r="E292" s="2">
+        <v>12241</v>
+      </c>
+      <c r="F292" s="2">
+        <v>2730</v>
+      </c>
+      <c r="G292" s="2">
+        <v>413</v>
+      </c>
+      <c r="H292" s="2">
+        <v>21</v>
+      </c>
+      <c r="I292" s="2">
+        <v>392</v>
+      </c>
+      <c r="J292" s="2">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -9684,29 +9785,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9741,7 +9842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9764,7 +9865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9787,7 +9888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9810,7 +9911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9833,7 +9934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9856,7 +9957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9879,7 +9980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -9899,7 +10000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -9919,7 +10020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -9939,7 +10040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -9959,7 +10060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -9979,12 +10080,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -10004,7 +10105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -10024,7 +10125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10044,7 +10145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10064,7 +10165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10084,7 +10185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10104,7 +10205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10124,7 +10225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10144,7 +10245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10164,7 +10265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10172,7 +10273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10195,7 +10296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10215,7 +10316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10235,7 +10336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10255,17 +10356,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10285,7 +10386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10308,7 +10409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10331,7 +10432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10351,7 +10452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10377,267 +10478,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April, 21th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,36 +397,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J292"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B293" sqref="B293"/>
+      <selection pane="bottomLeft" activeCell="A295" sqref="A295"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -495,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -527,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -559,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -591,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -623,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -655,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -687,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -719,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -751,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -783,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -815,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -847,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -879,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -911,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -943,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -975,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1007,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1039,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1071,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1103,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1167,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1199,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1231,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1263,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1295,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1359,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1391,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1423,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1487,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1519,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1551,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1583,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1615,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1647,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1679,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1711,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1743,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1807,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1839,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1871,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1903,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1935,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1967,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2031,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2063,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2095,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2127,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2159,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2191,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2255,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2287,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2319,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2383,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2415,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2447,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2479,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2543,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2575,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2607,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2639,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2671,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2703,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2735,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2767,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2799,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2831,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2863,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2895,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2927,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3023,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3055,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3087,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3119,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3151,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3183,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3279,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3311,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3343,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3375,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3407,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3439,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3471,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3535,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3567,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3599,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3663,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3695,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3759,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3823,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3855,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3887,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3919,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3951,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3983,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4015,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4047,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4079,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4111,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4143,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4175,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4207,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4239,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4399,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4431,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4463,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4495,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4527,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4559,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4623,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4655,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4687,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4719,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4751,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4783,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4815,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4847,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4879,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4911,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4943,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4975,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5039,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5071,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5103,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5135,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5167,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5199,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5231,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5263,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5295,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5327,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5359,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5391,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5423,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5455,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5519,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5551,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5583,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5615,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5647,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5679,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5711,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5743,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5775,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5807,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5839,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5903,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5935,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5967,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5999,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6031,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6063,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6095,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6127,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6159,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6191,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6223,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6255,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6287,7 +6282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6319,7 +6314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6351,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6383,7 +6378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6415,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6447,7 +6442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6479,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6511,7 +6506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6543,7 +6538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6607,7 +6602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6639,7 +6634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6671,7 +6666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6703,7 +6698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6735,7 +6730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6767,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6799,7 +6794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6831,7 +6826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6863,7 +6858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6895,7 +6890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6927,7 +6922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6959,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6991,7 +6986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7023,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7055,7 +7050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7087,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7119,7 +7114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7151,7 +7146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7183,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7215,7 +7210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7247,7 +7242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7279,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7343,7 +7338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7375,7 +7370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7407,7 +7402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7439,7 +7434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7471,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7503,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7535,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7567,7 +7562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7599,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7631,7 +7626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7663,7 +7658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7695,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7727,7 +7722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7759,7 +7754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7791,7 +7786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7823,7 +7818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7855,7 +7850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7887,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7919,7 +7914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7951,7 +7946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7983,7 +7978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8015,7 +8010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8047,7 +8042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8079,7 +8074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8111,7 +8106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8143,7 +8138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8175,7 +8170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8207,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8239,7 +8234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8271,7 +8266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8303,7 +8298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8335,7 +8330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8367,7 +8362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8399,7 +8394,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8431,7 +8426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8463,7 +8458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8495,7 +8490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8527,7 +8522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8559,7 +8554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8591,7 +8586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8623,7 +8618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8655,7 +8650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8687,7 +8682,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8719,7 +8714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8751,7 +8746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8783,7 +8778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8815,7 +8810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8847,7 +8842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8879,7 +8874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8911,7 +8906,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8943,7 +8938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8975,7 +8970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9007,7 +9002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9039,7 +9034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9071,7 +9066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9103,7 +9098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9135,7 +9130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9167,7 +9162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9199,7 +9194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9231,7 +9226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9263,7 +9258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9295,7 +9290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9327,7 +9322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9359,7 +9354,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9391,7 +9386,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9423,7 +9418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9455,7 +9450,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9487,7 +9482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9519,7 +9514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9551,7 +9546,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9583,7 +9578,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9615,7 +9610,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9647,7 +9642,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10">
       <c r="A289" s="1">
         <v>44302</v>
       </c>
@@ -9679,7 +9674,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10">
       <c r="A290" s="1">
         <v>44303</v>
       </c>
@@ -9711,7 +9706,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10">
       <c r="A291" s="1">
         <v>44304</v>
       </c>
@@ -9743,7 +9738,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10">
       <c r="A292" s="1">
         <v>44305</v>
       </c>
@@ -9772,6 +9767,70 @@
         <v>392</v>
       </c>
       <c r="J292" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10">
+      <c r="A293" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B293" s="2">
+        <v>8921</v>
+      </c>
+      <c r="C293" s="2">
+        <v>236</v>
+      </c>
+      <c r="D293" s="2">
+        <v>3245</v>
+      </c>
+      <c r="E293" s="2">
+        <v>12402</v>
+      </c>
+      <c r="F293" s="2">
+        <v>2775</v>
+      </c>
+      <c r="G293" s="2">
+        <v>391</v>
+      </c>
+      <c r="H293" s="2">
+        <v>22</v>
+      </c>
+      <c r="I293" s="2">
+        <v>369</v>
+      </c>
+      <c r="J293" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10">
+      <c r="A294" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B294" s="2">
+        <v>8943</v>
+      </c>
+      <c r="C294" s="2">
+        <v>228</v>
+      </c>
+      <c r="D294" s="2">
+        <v>3270</v>
+      </c>
+      <c r="E294" s="2">
+        <v>12441</v>
+      </c>
+      <c r="F294" s="2">
+        <v>2812</v>
+      </c>
+      <c r="G294" s="2">
+        <v>379</v>
+      </c>
+      <c r="H294" s="2">
+        <v>23</v>
+      </c>
+      <c r="I294" s="2">
+        <v>356</v>
+      </c>
+      <c r="J294" s="2">
         <v>79</v>
       </c>
     </row>
@@ -9785,29 +9844,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9842,7 +9901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9865,7 +9924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9888,7 +9947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9911,7 +9970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9934,7 +9993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -9957,7 +10016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -9980,7 +10039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -10000,7 +10059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -10020,7 +10079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -10040,7 +10099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -10060,7 +10119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -10080,12 +10139,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -10105,7 +10164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -10125,7 +10184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10145,7 +10204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10165,7 +10224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10185,7 +10244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10205,7 +10264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10225,7 +10284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10245,7 +10304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10265,7 +10324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10273,7 +10332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10296,7 +10355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10316,7 +10375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10336,7 +10395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10356,17 +10415,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10386,7 +10445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10409,7 +10468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10432,7 +10491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10452,7 +10511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10478,267 +10537,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 22th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,36 +402,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J294"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A295" sqref="A295"/>
+      <selection pane="bottomLeft" activeCell="E304" sqref="E304:E305"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +5007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5359,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7082,7 +7087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7114,7 +7119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7146,7 +7151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7178,7 +7183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7210,7 +7215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7242,7 +7247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7274,7 +7279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7306,7 +7311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7338,7 +7343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7402,7 +7407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7434,7 +7439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7466,7 +7471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7498,7 +7503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7530,7 +7535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7562,7 +7567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7594,7 +7599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7626,7 +7631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7658,7 +7663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7690,7 +7695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7722,7 +7727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7754,7 +7759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7786,7 +7791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7818,7 +7823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7850,7 +7855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7882,7 +7887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7914,7 +7919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7946,7 +7951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7978,7 +7983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8010,7 +8015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8042,7 +8047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8074,7 +8079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8106,7 +8111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8138,7 +8143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8170,7 +8175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8202,7 +8207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8234,7 +8239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8266,7 +8271,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8298,7 +8303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8330,7 +8335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8362,7 +8367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8394,7 +8399,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8426,7 +8431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8458,7 +8463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8490,7 +8495,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8522,7 +8527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8554,7 +8559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8586,7 +8591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8618,7 +8623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8650,7 +8655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8682,7 +8687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8714,7 +8719,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8746,7 +8751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8778,7 +8783,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8810,7 +8815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8842,7 +8847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8874,7 +8879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8906,7 +8911,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8938,7 +8943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8970,7 +8975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9002,7 +9007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9034,7 +9039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9066,7 +9071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9098,7 +9103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9130,7 +9135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9162,7 +9167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9194,7 +9199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9226,7 +9231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9258,7 +9263,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9290,7 +9295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9322,7 +9327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9354,7 +9359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9386,7 +9391,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9418,7 +9423,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9450,7 +9455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9482,7 +9487,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9514,7 +9519,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9546,7 +9551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9578,7 +9583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9610,7 +9615,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9642,7 +9647,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>44302</v>
       </c>
@@ -9674,7 +9679,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>44303</v>
       </c>
@@ -9706,7 +9711,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>44304</v>
       </c>
@@ -9738,7 +9743,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>44305</v>
       </c>
@@ -9770,7 +9775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>44306</v>
       </c>
@@ -9802,7 +9807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>44307</v>
       </c>
@@ -9832,6 +9837,38 @@
       </c>
       <c r="J294" s="2">
         <v>79</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B295" s="2">
+        <v>8989</v>
+      </c>
+      <c r="C295" s="2">
+        <v>219</v>
+      </c>
+      <c r="D295" s="2">
+        <v>3315</v>
+      </c>
+      <c r="E295" s="2">
+        <v>12523</v>
+      </c>
+      <c r="F295" s="2">
+        <v>2847</v>
+      </c>
+      <c r="G295" s="2">
+        <v>388</v>
+      </c>
+      <c r="H295" s="2">
+        <v>26</v>
+      </c>
+      <c r="I295" s="2">
+        <v>362</v>
+      </c>
+      <c r="J295" s="2">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -9844,29 +9881,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9901,7 +9938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9924,7 +9961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9947,7 +9984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -9970,7 +10007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -9993,7 +10030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -10016,7 +10053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -10039,7 +10076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -10059,7 +10096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -10079,7 +10116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -10099,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -10119,7 +10156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -10139,12 +10176,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -10164,7 +10201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -10184,7 +10221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10204,7 +10241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10224,7 +10261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10244,7 +10281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10264,7 +10301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10284,7 +10321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10304,7 +10341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10324,7 +10361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10332,7 +10369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10355,7 +10392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10375,7 +10412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10395,7 +10432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10415,17 +10452,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10445,7 +10482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10468,7 +10505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10491,7 +10528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10511,7 +10548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10537,267 +10574,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 23th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,36 +397,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J295"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E304" sqref="E304:E305"/>
+      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A297" sqref="A297"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -495,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -527,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -559,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -591,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -623,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -655,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -687,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -719,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -751,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -783,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -815,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -847,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -879,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -911,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -943,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -975,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1007,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1039,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1071,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1103,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1167,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1199,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1231,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1263,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1295,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1359,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1391,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1423,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1487,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1519,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1551,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1583,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1615,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1647,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1679,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1711,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1743,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1807,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1839,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1871,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1903,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1935,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1967,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2031,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2063,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2095,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2127,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2159,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2191,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2255,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2287,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2319,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2383,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2415,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2447,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2479,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2543,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2575,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2607,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2639,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2671,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2703,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2735,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2767,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2799,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2831,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2863,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2895,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2927,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3023,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3055,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3087,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3119,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3151,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3183,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3279,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3311,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3343,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3375,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3407,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3439,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3471,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3535,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3567,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3599,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3663,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3695,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3759,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3823,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3855,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3887,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3919,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3951,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3983,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4015,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4047,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4079,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4111,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4143,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4175,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4207,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4239,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4399,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4431,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4463,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4495,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4527,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4559,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4623,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4655,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4687,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4719,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4751,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4783,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4815,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4847,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4879,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4911,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4943,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4975,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5039,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5071,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5103,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5135,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5167,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5199,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5231,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5263,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5295,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5327,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5359,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5391,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5423,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5455,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5519,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5551,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5583,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5615,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5647,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5679,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5711,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5743,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5775,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5807,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5839,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5903,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5935,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5967,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5999,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6031,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6063,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6095,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6127,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6159,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6191,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6223,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6255,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6287,7 +6282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6319,7 +6314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6351,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6383,7 +6378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6415,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6447,7 +6442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6479,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6511,7 +6506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6543,7 +6538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6607,7 +6602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6639,7 +6634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6671,7 +6666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6703,7 +6698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6735,7 +6730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6767,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6799,7 +6794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6831,7 +6826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6863,7 +6858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6895,7 +6890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6927,7 +6922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6959,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6991,7 +6986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7023,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7055,7 +7050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7087,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7119,7 +7114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7151,7 +7146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7183,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7215,7 +7210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7247,7 +7242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7279,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7343,7 +7338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7375,7 +7370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7407,7 +7402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7439,7 +7434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7471,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7503,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7535,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7567,7 +7562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7599,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7631,7 +7626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7663,7 +7658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7695,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7727,7 +7722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7759,7 +7754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7791,7 +7786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7823,7 +7818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7855,7 +7850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7887,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7919,7 +7914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7951,7 +7946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7983,7 +7978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8015,7 +8010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8047,7 +8042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8079,7 +8074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8111,7 +8106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8143,7 +8138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8175,7 +8170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8207,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8239,7 +8234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8271,7 +8266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8303,7 +8298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8335,7 +8330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8367,7 +8362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8399,7 +8394,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8431,7 +8426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8463,7 +8458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8495,7 +8490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8527,7 +8522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8559,7 +8554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8591,7 +8586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8623,7 +8618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8655,7 +8650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8687,7 +8682,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8719,7 +8714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8751,7 +8746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8783,7 +8778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8815,7 +8810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8847,7 +8842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8879,7 +8874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8911,7 +8906,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8943,7 +8938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8975,7 +8970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9007,7 +9002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9039,7 +9034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9071,7 +9066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9103,7 +9098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9135,7 +9130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9167,7 +9162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9199,7 +9194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9231,7 +9226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9263,7 +9258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9295,7 +9290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9327,7 +9322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9359,7 +9354,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9391,7 +9386,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9423,7 +9418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9455,7 +9450,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9487,7 +9482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9519,7 +9514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9551,7 +9546,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9583,7 +9578,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9615,7 +9610,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9647,7 +9642,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10">
       <c r="A289" s="1">
         <v>44302</v>
       </c>
@@ -9679,7 +9674,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10">
       <c r="A290" s="1">
         <v>44303</v>
       </c>
@@ -9711,7 +9706,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10">
       <c r="A291" s="1">
         <v>44304</v>
       </c>
@@ -9743,7 +9738,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10">
       <c r="A292" s="1">
         <v>44305</v>
       </c>
@@ -9775,7 +9770,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10">
       <c r="A293" s="1">
         <v>44306</v>
       </c>
@@ -9807,7 +9802,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10">
       <c r="A294" s="1">
         <v>44307</v>
       </c>
@@ -9839,7 +9834,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10">
       <c r="A295" s="1">
         <v>44308</v>
       </c>
@@ -9868,6 +9863,38 @@
         <v>362</v>
       </c>
       <c r="J295" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10">
+      <c r="A296" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B296" s="2">
+        <v>9020</v>
+      </c>
+      <c r="C296" s="2">
+        <v>225</v>
+      </c>
+      <c r="D296" s="2">
+        <v>3340</v>
+      </c>
+      <c r="E296" s="2">
+        <v>12585</v>
+      </c>
+      <c r="F296" s="2">
+        <v>2878</v>
+      </c>
+      <c r="G296" s="2">
+        <v>382</v>
+      </c>
+      <c r="H296" s="2">
+        <v>23</v>
+      </c>
+      <c r="I296" s="2">
+        <v>359</v>
+      </c>
+      <c r="J296" s="2">
         <v>80</v>
       </c>
     </row>
@@ -9881,29 +9908,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9938,7 +9965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9961,7 +9988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -9984,7 +10011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -10007,7 +10034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -10030,7 +10057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -10053,7 +10080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -10076,7 +10103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -10096,7 +10123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -10116,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -10136,7 +10163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -10156,7 +10183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -10176,12 +10203,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -10201,7 +10228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -10221,7 +10248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10241,7 +10268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10261,7 +10288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10281,7 +10308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10301,7 +10328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10321,7 +10348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10341,7 +10368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10361,7 +10388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10369,7 +10396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10392,7 +10419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10412,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10432,7 +10459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10452,17 +10479,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10482,7 +10509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10505,7 +10532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10528,7 +10555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10548,7 +10575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10574,267 +10601,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 26th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,36 +402,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J296"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A297" sqref="A297"/>
+      <selection pane="bottomLeft" activeCell="B300" sqref="B300"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +5007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5359,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7082,7 +7087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7114,7 +7119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7146,7 +7151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7178,7 +7183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7210,7 +7215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7242,7 +7247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7274,7 +7279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7306,7 +7311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7338,7 +7343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7402,7 +7407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7434,7 +7439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7466,7 +7471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7498,7 +7503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7530,7 +7535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7562,7 +7567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7594,7 +7599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7626,7 +7631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7658,7 +7663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7690,7 +7695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7722,7 +7727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7754,7 +7759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7786,7 +7791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7818,7 +7823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7850,7 +7855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7882,7 +7887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7914,7 +7919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7946,7 +7951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7978,7 +7983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8010,7 +8015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8042,7 +8047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8074,7 +8079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8106,7 +8111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8138,7 +8143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8170,7 +8175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8202,7 +8207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8234,7 +8239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8266,7 +8271,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8298,7 +8303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8330,7 +8335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8362,7 +8367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8394,7 +8399,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8426,7 +8431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8458,7 +8463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8490,7 +8495,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8522,7 +8527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8554,7 +8559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8586,7 +8591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8618,7 +8623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8650,7 +8655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8682,7 +8687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8714,7 +8719,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8746,7 +8751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8778,7 +8783,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8810,7 +8815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8842,7 +8847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8874,7 +8879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8906,7 +8911,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8938,7 +8943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8970,7 +8975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9002,7 +9007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9034,7 +9039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9066,7 +9071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9098,7 +9103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9130,7 +9135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9162,7 +9167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9194,7 +9199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9226,7 +9231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9258,7 +9263,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9290,7 +9295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9322,7 +9327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9354,7 +9359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9386,7 +9391,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9418,7 +9423,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9450,7 +9455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9482,7 +9487,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9514,7 +9519,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9546,7 +9551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9578,7 +9583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9610,7 +9615,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9642,7 +9647,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>44302</v>
       </c>
@@ -9674,7 +9679,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>44303</v>
       </c>
@@ -9706,7 +9711,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>44304</v>
       </c>
@@ -9738,7 +9743,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>44305</v>
       </c>
@@ -9770,7 +9775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>44306</v>
       </c>
@@ -9802,7 +9807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>44307</v>
       </c>
@@ -9834,7 +9839,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>44308</v>
       </c>
@@ -9866,7 +9871,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>44309</v>
       </c>
@@ -9895,6 +9900,102 @@
         <v>359</v>
       </c>
       <c r="J296" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>44310</v>
+      </c>
+      <c r="B297" s="2">
+        <v>9072</v>
+      </c>
+      <c r="C297" s="2">
+        <v>180</v>
+      </c>
+      <c r="D297" s="2">
+        <v>3375</v>
+      </c>
+      <c r="E297" s="2">
+        <v>12627</v>
+      </c>
+      <c r="F297" s="2">
+        <v>2884</v>
+      </c>
+      <c r="G297" s="2">
+        <v>411</v>
+      </c>
+      <c r="H297" s="2">
+        <v>25</v>
+      </c>
+      <c r="I297" s="2">
+        <v>386</v>
+      </c>
+      <c r="J297" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>44311</v>
+      </c>
+      <c r="B298" s="2">
+        <v>9121</v>
+      </c>
+      <c r="C298" s="2">
+        <v>110</v>
+      </c>
+      <c r="D298" s="2">
+        <v>3397</v>
+      </c>
+      <c r="E298" s="2">
+        <v>12628</v>
+      </c>
+      <c r="F298" s="2">
+        <v>2887</v>
+      </c>
+      <c r="G298" s="2">
+        <v>430</v>
+      </c>
+      <c r="H298" s="2">
+        <v>25</v>
+      </c>
+      <c r="I298" s="2">
+        <v>405</v>
+      </c>
+      <c r="J298" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B299" s="2">
+        <v>9126</v>
+      </c>
+      <c r="C299" s="2">
+        <v>154</v>
+      </c>
+      <c r="D299" s="2">
+        <v>3413</v>
+      </c>
+      <c r="E299" s="2">
+        <v>12693</v>
+      </c>
+      <c r="F299" s="2">
+        <v>2934</v>
+      </c>
+      <c r="G299" s="2">
+        <v>399</v>
+      </c>
+      <c r="H299" s="2">
+        <v>23</v>
+      </c>
+      <c r="I299" s="2">
+        <v>376</v>
+      </c>
+      <c r="J299" s="2">
         <v>80</v>
       </c>
     </row>
@@ -9908,29 +10009,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9965,7 +10066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -9988,7 +10089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -10011,7 +10112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -10034,7 +10135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -10057,7 +10158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -10080,7 +10181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -10103,7 +10204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -10123,7 +10224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -10143,7 +10244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -10163,7 +10264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -10183,7 +10284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -10203,12 +10304,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -10228,7 +10329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -10248,7 +10349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10268,7 +10369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10288,7 +10389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10308,7 +10409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10328,7 +10429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10348,7 +10449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10368,7 +10469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10388,7 +10489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10396,7 +10497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10419,7 +10520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10439,7 +10540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10459,7 +10560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10479,17 +10580,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10509,7 +10610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10532,7 +10633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10555,7 +10656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10575,7 +10676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10601,267 +10702,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until April 30th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,36 +397,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J299"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B300" sqref="B300"/>
+      <selection pane="bottomLeft" activeCell="A304" sqref="A304"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -495,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -527,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -559,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -591,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -623,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -655,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -687,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -719,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -751,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -783,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -815,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -847,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -879,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -911,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -943,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -975,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1007,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1039,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1071,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1103,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1167,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1199,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1231,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1263,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1295,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1359,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1391,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1423,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1487,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1519,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1551,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1583,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1615,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1647,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1679,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1711,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1743,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1807,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1839,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1871,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1903,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1935,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1967,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2031,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2063,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2095,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2127,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2159,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2191,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2255,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2287,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2319,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2383,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2415,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2447,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2479,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2543,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2575,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2607,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2639,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2671,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2703,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2735,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2767,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2799,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2831,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2863,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2895,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2927,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3023,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3055,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3087,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3119,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3151,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3183,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3279,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3311,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3343,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3375,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3407,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3439,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3471,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3535,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3567,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3599,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3663,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3695,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3759,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3823,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3855,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3887,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3919,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3951,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3983,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4015,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4047,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4079,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4111,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4143,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4175,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4207,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4239,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4399,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4431,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4463,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4495,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4527,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4559,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4623,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4655,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4687,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4719,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4751,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4783,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4815,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4847,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4879,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4911,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4943,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4975,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5039,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5071,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5103,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5135,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5167,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5199,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5231,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5263,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5295,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5327,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5359,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5391,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5423,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5455,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5519,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5551,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5583,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5615,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5647,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5679,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5711,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5743,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5775,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5807,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5839,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5903,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5935,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5967,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5999,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6031,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6063,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6095,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6127,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6159,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6191,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6223,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6255,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6287,7 +6282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6319,7 +6314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6351,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6383,7 +6378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6415,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6447,7 +6442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6479,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6511,7 +6506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6543,7 +6538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6607,7 +6602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6639,7 +6634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6671,7 +6666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6703,7 +6698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6735,7 +6730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6767,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6799,7 +6794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6831,7 +6826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6863,7 +6858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6895,7 +6890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6927,7 +6922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6959,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6991,7 +6986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7023,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7055,7 +7050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7087,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7119,7 +7114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7151,7 +7146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7183,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7215,7 +7210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7247,7 +7242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7279,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7343,7 +7338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7375,7 +7370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7407,7 +7402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7439,7 +7434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7471,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7503,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7535,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7567,7 +7562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7599,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7631,7 +7626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7663,7 +7658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7695,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7727,7 +7722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7759,7 +7754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7791,7 +7786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7823,7 +7818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7855,7 +7850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7887,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7919,7 +7914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7951,7 +7946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7983,7 +7978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8015,7 +8010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8047,7 +8042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8079,7 +8074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8111,7 +8106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8143,7 +8138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8175,7 +8170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8207,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8239,7 +8234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8271,7 +8266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8303,7 +8298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8335,7 +8330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8367,7 +8362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8399,7 +8394,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8431,7 +8426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8463,7 +8458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8495,7 +8490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8527,7 +8522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8559,7 +8554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8591,7 +8586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8623,7 +8618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8655,7 +8650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8687,7 +8682,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8719,7 +8714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8751,7 +8746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8783,7 +8778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8815,7 +8810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8847,7 +8842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8879,7 +8874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8911,7 +8906,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8943,7 +8938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8975,7 +8970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9007,7 +9002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9039,7 +9034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9071,7 +9066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9103,7 +9098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9135,7 +9130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9167,7 +9162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9199,7 +9194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9231,7 +9226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9263,7 +9258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9295,7 +9290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9327,7 +9322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9359,7 +9354,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9391,7 +9386,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9423,7 +9418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9455,7 +9450,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9487,7 +9482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9519,7 +9514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9551,7 +9546,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9583,7 +9578,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9615,7 +9610,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9647,7 +9642,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10">
       <c r="A289" s="1">
         <v>44302</v>
       </c>
@@ -9679,7 +9674,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10">
       <c r="A290" s="1">
         <v>44303</v>
       </c>
@@ -9711,7 +9706,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10">
       <c r="A291" s="1">
         <v>44304</v>
       </c>
@@ -9743,7 +9738,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10">
       <c r="A292" s="1">
         <v>44305</v>
       </c>
@@ -9775,7 +9770,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10">
       <c r="A293" s="1">
         <v>44306</v>
       </c>
@@ -9807,7 +9802,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10">
       <c r="A294" s="1">
         <v>44307</v>
       </c>
@@ -9839,7 +9834,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10">
       <c r="A295" s="1">
         <v>44308</v>
       </c>
@@ -9871,7 +9866,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10">
       <c r="A296" s="1">
         <v>44309</v>
       </c>
@@ -9903,7 +9898,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10">
       <c r="A297" s="1">
         <v>44310</v>
       </c>
@@ -9935,7 +9930,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10">
       <c r="A298" s="1">
         <v>44311</v>
       </c>
@@ -9967,7 +9962,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10">
       <c r="A299" s="1">
         <v>44312</v>
       </c>
@@ -9997,6 +9992,134 @@
       </c>
       <c r="J299" s="2">
         <v>80</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10">
+      <c r="A300" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B300" s="2">
+        <v>9201</v>
+      </c>
+      <c r="C300" s="2">
+        <v>167</v>
+      </c>
+      <c r="D300" s="2">
+        <v>3442</v>
+      </c>
+      <c r="E300" s="2">
+        <v>12810</v>
+      </c>
+      <c r="F300" s="2">
+        <v>3000</v>
+      </c>
+      <c r="G300" s="2">
+        <v>361</v>
+      </c>
+      <c r="H300" s="2">
+        <v>22</v>
+      </c>
+      <c r="I300" s="2">
+        <v>339</v>
+      </c>
+      <c r="J300" s="2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10">
+      <c r="A301" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B301" s="2">
+        <v>9249</v>
+      </c>
+      <c r="C301" s="2">
+        <v>154</v>
+      </c>
+      <c r="D301" s="2">
+        <v>3464</v>
+      </c>
+      <c r="E301" s="2">
+        <v>12867</v>
+      </c>
+      <c r="F301" s="2">
+        <v>3042</v>
+      </c>
+      <c r="G301" s="2">
+        <v>340</v>
+      </c>
+      <c r="H301" s="2">
+        <v>22</v>
+      </c>
+      <c r="I301" s="2">
+        <v>318</v>
+      </c>
+      <c r="J301" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10">
+      <c r="A302" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B302" s="2">
+        <v>9317</v>
+      </c>
+      <c r="C302" s="2">
+        <v>159</v>
+      </c>
+      <c r="D302" s="2">
+        <v>3513</v>
+      </c>
+      <c r="E302" s="2">
+        <v>12989</v>
+      </c>
+      <c r="F302" s="2">
+        <v>3075</v>
+      </c>
+      <c r="G302" s="2">
+        <v>354</v>
+      </c>
+      <c r="H302" s="2">
+        <v>22</v>
+      </c>
+      <c r="I302" s="2">
+        <v>332</v>
+      </c>
+      <c r="J302" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10">
+      <c r="A303" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B303" s="2">
+        <v>9349</v>
+      </c>
+      <c r="C303" s="2">
+        <v>152</v>
+      </c>
+      <c r="D303" s="2">
+        <v>3539</v>
+      </c>
+      <c r="E303" s="2">
+        <v>13040</v>
+      </c>
+      <c r="F303" s="2">
+        <v>3101</v>
+      </c>
+      <c r="G303" s="2">
+        <v>353</v>
+      </c>
+      <c r="H303" s="2">
+        <v>22</v>
+      </c>
+      <c r="I303" s="2">
+        <v>331</v>
+      </c>
+      <c r="J303" s="2">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -10009,29 +10132,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -10066,7 +10189,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -10089,7 +10212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -10112,7 +10235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -10135,7 +10258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -10158,7 +10281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -10181,7 +10304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -10204,7 +10327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -10224,7 +10347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -10244,7 +10367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -10264,7 +10387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -10284,7 +10407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -10304,12 +10427,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -10329,7 +10452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -10349,7 +10472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10369,7 +10492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10389,7 +10512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10409,7 +10532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10429,7 +10552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10449,7 +10572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10469,7 +10592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10489,7 +10612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10497,7 +10620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10520,7 +10643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10540,7 +10663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10560,7 +10683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10580,17 +10703,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10610,7 +10733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10633,7 +10756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10656,7 +10779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10676,7 +10799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10702,267 +10825,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until May 3th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -71,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,36 +402,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J303"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A304" sqref="A304"/>
+      <selection pane="bottomLeft" activeCell="B307" sqref="B307"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -490,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -522,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -554,7 +559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -586,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -618,7 +623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -650,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -682,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -714,7 +719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -746,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -778,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -810,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -842,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -874,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -906,7 +911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -938,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -970,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1098,7 +1103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1194,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1322,7 +1327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1354,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1386,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1418,7 +1423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1450,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1546,7 +1551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1578,7 +1583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1610,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1642,7 +1647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1674,7 +1679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1706,7 +1711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1738,7 +1743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1770,7 +1775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1802,7 +1807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1834,7 +1839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1898,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1994,7 +1999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2058,7 +2063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2090,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2122,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2186,7 +2191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2218,7 +2223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2250,7 +2255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2282,7 +2287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2346,7 +2351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2506,7 +2511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2538,7 +2543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2666,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2698,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2826,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2858,7 +2863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2890,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2922,7 +2927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2986,7 +2991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3050,7 +3055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3114,7 +3119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3146,7 +3151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3178,7 +3183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3274,7 +3279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3306,7 +3311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3338,7 +3343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3658,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3690,7 +3695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3722,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3754,7 +3759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3786,7 +3791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3818,7 +3823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3914,7 +3919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3946,7 +3951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3978,7 +3983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4010,7 +4015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4042,7 +4047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4106,7 +4111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4138,7 +4143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4170,7 +4175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4202,7 +4207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4234,7 +4239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4330,7 +4335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4362,7 +4367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4394,7 +4399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4426,7 +4431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4458,7 +4463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4490,7 +4495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4522,7 +4527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4554,7 +4559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4586,7 +4591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4618,7 +4623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4650,7 +4655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4682,7 +4687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4714,7 +4719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4746,7 +4751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4778,7 +4783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4810,7 +4815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4842,7 +4847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4874,7 +4879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4906,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4938,7 +4943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5002,7 +5007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5034,7 +5039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5066,7 +5071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5098,7 +5103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5130,7 +5135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5162,7 +5167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5194,7 +5199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5226,7 +5231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5258,7 +5263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5290,7 +5295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5322,7 +5327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5354,7 +5359,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5386,7 +5391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5450,7 +5455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5514,7 +5519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5546,7 +5551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5578,7 +5583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5610,7 +5615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5674,7 +5679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5706,7 +5711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5738,7 +5743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5770,7 +5775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5802,7 +5807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5834,7 +5839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5866,7 +5871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5898,7 +5903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5930,7 +5935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5962,7 +5967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5994,7 +5999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6026,7 +6031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6058,7 +6063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6122,7 +6127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6154,7 +6159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6186,7 +6191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6218,7 +6223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6250,7 +6255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6282,7 +6287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6314,7 +6319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6378,7 +6383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6410,7 +6415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6442,7 +6447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6474,7 +6479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6506,7 +6511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6538,7 +6543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6570,7 +6575,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6602,7 +6607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6634,7 +6639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6666,7 +6671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6698,7 +6703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6730,7 +6735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6762,7 +6767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6794,7 +6799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6826,7 +6831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6858,7 +6863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6890,7 +6895,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6922,7 +6927,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6954,7 +6959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7018,7 +7023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7050,7 +7055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7082,7 +7087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7114,7 +7119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7146,7 +7151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7178,7 +7183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7210,7 +7215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7242,7 +7247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7274,7 +7279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7306,7 +7311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7338,7 +7343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7402,7 +7407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7434,7 +7439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7466,7 +7471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7498,7 +7503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7530,7 +7535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7562,7 +7567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7594,7 +7599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7626,7 +7631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7658,7 +7663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7690,7 +7695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7722,7 +7727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7754,7 +7759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7786,7 +7791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7818,7 +7823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7850,7 +7855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7882,7 +7887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7914,7 +7919,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7946,7 +7951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7978,7 +7983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8010,7 +8015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8042,7 +8047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8074,7 +8079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8106,7 +8111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8138,7 +8143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8170,7 +8175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8202,7 +8207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8234,7 +8239,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8266,7 +8271,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8298,7 +8303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8330,7 +8335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8362,7 +8367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8394,7 +8399,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8426,7 +8431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8458,7 +8463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8490,7 +8495,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8522,7 +8527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8554,7 +8559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8586,7 +8591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8618,7 +8623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8650,7 +8655,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8682,7 +8687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8714,7 +8719,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8746,7 +8751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8778,7 +8783,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8810,7 +8815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8842,7 +8847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8874,7 +8879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8906,7 +8911,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8938,7 +8943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8970,7 +8975,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9002,7 +9007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9034,7 +9039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9066,7 +9071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9098,7 +9103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9130,7 +9135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9162,7 +9167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9194,7 +9199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9226,7 +9231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9258,7 +9263,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9290,7 +9295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9322,7 +9327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9354,7 +9359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9386,7 +9391,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9418,7 +9423,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9450,7 +9455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9482,7 +9487,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9514,7 +9519,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9546,7 +9551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9578,7 +9583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9610,7 +9615,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9642,7 +9647,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>44302</v>
       </c>
@@ -9674,7 +9679,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>44303</v>
       </c>
@@ -9706,7 +9711,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>44304</v>
       </c>
@@ -9738,7 +9743,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>44305</v>
       </c>
@@ -9770,7 +9775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>44306</v>
       </c>
@@ -9802,7 +9807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>44307</v>
       </c>
@@ -9834,7 +9839,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>44308</v>
       </c>
@@ -9866,7 +9871,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>44309</v>
       </c>
@@ -9898,7 +9903,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="297" spans="1:10">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>44310</v>
       </c>
@@ -9930,7 +9935,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>44311</v>
       </c>
@@ -9962,7 +9967,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>44312</v>
       </c>
@@ -9994,7 +9999,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>44313</v>
       </c>
@@ -10026,7 +10031,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>44314</v>
       </c>
@@ -10058,7 +10063,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="302" spans="1:10">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>44315</v>
       </c>
@@ -10090,7 +10095,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="303" spans="1:10">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>44316</v>
       </c>
@@ -10120,6 +10125,102 @@
       </c>
       <c r="J303" s="2">
         <v>85</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B304" s="2">
+        <v>9403</v>
+      </c>
+      <c r="C304" s="2">
+        <v>91</v>
+      </c>
+      <c r="D304" s="2">
+        <v>3568</v>
+      </c>
+      <c r="E304" s="2">
+        <v>13062</v>
+      </c>
+      <c r="F304" s="2">
+        <v>3118</v>
+      </c>
+      <c r="G304" s="2">
+        <v>364</v>
+      </c>
+      <c r="H304" s="2">
+        <v>22</v>
+      </c>
+      <c r="I304" s="2">
+        <v>342</v>
+      </c>
+      <c r="J304" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
+        <v>44318</v>
+      </c>
+      <c r="B305" s="2">
+        <v>9431</v>
+      </c>
+      <c r="C305" s="2">
+        <v>50</v>
+      </c>
+      <c r="D305" s="2">
+        <v>3586</v>
+      </c>
+      <c r="E305" s="2">
+        <v>13067</v>
+      </c>
+      <c r="F305" s="2">
+        <v>3118</v>
+      </c>
+      <c r="G305" s="2">
+        <v>381</v>
+      </c>
+      <c r="H305" s="2">
+        <v>20</v>
+      </c>
+      <c r="I305" s="2">
+        <v>361</v>
+      </c>
+      <c r="J305" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B306" s="2">
+        <v>9431</v>
+      </c>
+      <c r="C306" s="2">
+        <v>98</v>
+      </c>
+      <c r="D306" s="2">
+        <v>3595</v>
+      </c>
+      <c r="E306" s="2">
+        <v>13124</v>
+      </c>
+      <c r="F306" s="2">
+        <v>3183</v>
+      </c>
+      <c r="G306" s="2">
+        <v>323</v>
+      </c>
+      <c r="H306" s="2">
+        <v>20</v>
+      </c>
+      <c r="I306" s="2">
+        <v>303</v>
+      </c>
+      <c r="J306" s="2">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -10132,29 +10233,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -10189,7 +10290,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -10212,7 +10313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -10235,7 +10336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -10258,7 +10359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -10281,7 +10382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -10304,7 +10405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -10327,7 +10428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -10347,7 +10448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -10367,7 +10468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -10387,7 +10488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -10407,7 +10508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -10427,12 +10528,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -10452,7 +10553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -10472,7 +10573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10492,7 +10593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10512,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10532,7 +10633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10552,7 +10653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10572,7 +10673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10592,7 +10693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10612,7 +10713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10620,7 +10721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10643,7 +10744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10663,7 +10764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10683,7 +10784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10703,17 +10804,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10733,7 +10834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10756,7 +10857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>43986</v>
       </c>
@@ -10779,7 +10880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43985</v>
       </c>
@@ -10799,7 +10900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>43984</v>
       </c>
@@ -10825,267 +10926,267 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43983</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43982</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43981</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>43980</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>43979</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>43978</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>43977</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43976</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43975</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43974</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43973</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43971</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>43970</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>43969</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>43968</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>43967</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43966</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>43965</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>43964</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>43963</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>43962</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>43961</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>43960</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>43959</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>43958</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>43957</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>43956</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43955</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43954</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>43953</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43952</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>43951</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>43950</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>43949</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>43948</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>43947</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>43946</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>43945</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>43944</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>43943</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43942</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43941</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>43940</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>43939</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>43938</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>43937</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>43936</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until May 5th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -190,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -225,7 +225,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -410,11 +410,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J306"/>
+  <dimension ref="A1:J308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B307" sqref="B307"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J304" sqref="J304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10221,6 +10221,70 @@
       </c>
       <c r="J306" s="2">
         <v>89</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B307" s="2">
+        <v>9465</v>
+      </c>
+      <c r="C307" s="2">
+        <v>140</v>
+      </c>
+      <c r="D307" s="2">
+        <v>3629</v>
+      </c>
+      <c r="E307" s="2">
+        <v>13234</v>
+      </c>
+      <c r="F307" s="2">
+        <v>3226</v>
+      </c>
+      <c r="G307" s="2">
+        <v>313</v>
+      </c>
+      <c r="H307" s="2">
+        <v>20</v>
+      </c>
+      <c r="I307" s="2">
+        <v>293</v>
+      </c>
+      <c r="J307" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B308" s="2">
+        <v>9500</v>
+      </c>
+      <c r="C308" s="2">
+        <v>183</v>
+      </c>
+      <c r="D308" s="2">
+        <v>3689</v>
+      </c>
+      <c r="E308" s="2">
+        <v>13372</v>
+      </c>
+      <c r="F308" s="2">
+        <v>3237</v>
+      </c>
+      <c r="G308" s="2">
+        <v>360</v>
+      </c>
+      <c r="H308" s="2">
+        <v>22</v>
+      </c>
+      <c r="I308" s="2">
+        <v>338</v>
+      </c>
+      <c r="J308" s="2">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data until May 7th
</commit_message>
<xml_diff>
--- a/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
+++ b/data/raw/BOLETIM_DIARIO_CORONAVIRUS_SAP.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Development\projects\covid-sap-city\data\raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -76,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -225,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -402,36 +397,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J308"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J304" sqref="J304"/>
+      <selection pane="bottomLeft" activeCell="A311" sqref="A311"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>44015</v>
       </c>
@@ -495,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>44016</v>
       </c>
@@ -527,7 +522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>44017</v>
       </c>
@@ -559,7 +554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>44018</v>
       </c>
@@ -591,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>44019</v>
       </c>
@@ -623,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>44020</v>
       </c>
@@ -655,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>44021</v>
       </c>
@@ -687,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>44022</v>
       </c>
@@ -719,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>44023</v>
       </c>
@@ -751,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>44024</v>
       </c>
@@ -783,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>44025</v>
       </c>
@@ -815,7 +810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>44026</v>
       </c>
@@ -847,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44027</v>
       </c>
@@ -879,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>44028</v>
       </c>
@@ -911,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>44029</v>
       </c>
@@ -943,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>44030</v>
       </c>
@@ -975,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>44031</v>
       </c>
@@ -1007,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>44032</v>
       </c>
@@ -1039,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>44033</v>
       </c>
@@ -1071,7 +1066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>44034</v>
       </c>
@@ -1103,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>44035</v>
       </c>
@@ -1135,7 +1130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>44036</v>
       </c>
@@ -1167,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>44037</v>
       </c>
@@ -1199,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>44038</v>
       </c>
@@ -1231,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>44039</v>
       </c>
@@ -1263,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>44040</v>
       </c>
@@ -1295,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>44041</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>44042</v>
       </c>
@@ -1359,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -1391,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>44044</v>
       </c>
@@ -1423,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>44045</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>44046</v>
       </c>
@@ -1487,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>44047</v>
       </c>
@@ -1519,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>44048</v>
       </c>
@@ -1551,7 +1546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>44049</v>
       </c>
@@ -1583,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>44050</v>
       </c>
@@ -1615,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>44051</v>
       </c>
@@ -1647,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>44052</v>
       </c>
@@ -1679,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>44053</v>
       </c>
@@ -1711,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>44054</v>
       </c>
@@ -1743,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>44055</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>44056</v>
       </c>
@@ -1807,7 +1802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>44057</v>
       </c>
@@ -1839,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>44058</v>
       </c>
@@ -1871,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44059</v>
       </c>
@@ -1903,7 +1898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>44060</v>
       </c>
@@ -1935,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>44061</v>
       </c>
@@ -1967,7 +1962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>44062</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>44063</v>
       </c>
@@ -2031,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>44064</v>
       </c>
@@ -2063,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>44065</v>
       </c>
@@ -2095,7 +2090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>44066</v>
       </c>
@@ -2127,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>44067</v>
       </c>
@@ -2159,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>44068</v>
       </c>
@@ -2191,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>44069</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>44070</v>
       </c>
@@ -2255,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>44071</v>
       </c>
@@ -2287,7 +2282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>44072</v>
       </c>
@@ -2319,7 +2314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>44073</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>44074</v>
       </c>
@@ -2383,7 +2378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>44075</v>
       </c>
@@ -2415,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>44076</v>
       </c>
@@ -2447,7 +2442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>44077</v>
       </c>
@@ -2479,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>44078</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>44079</v>
       </c>
@@ -2543,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>44080</v>
       </c>
@@ -2575,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>44081</v>
       </c>
@@ -2607,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>44082</v>
       </c>
@@ -2639,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>44083</v>
       </c>
@@ -2671,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>44084</v>
       </c>
@@ -2703,7 +2698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>44085</v>
       </c>
@@ -2735,7 +2730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>44086</v>
       </c>
@@ -2767,7 +2762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>44087</v>
       </c>
@@ -2799,7 +2794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>44088</v>
       </c>
@@ -2831,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>44089</v>
       </c>
@@ -2863,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>44090</v>
       </c>
@@ -2895,7 +2890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>44091</v>
       </c>
@@ -2927,7 +2922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>44092</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>44093</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>44094</v>
       </c>
@@ -3023,7 +3018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>44095</v>
       </c>
@@ -3055,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>44096</v>
       </c>
@@ -3087,7 +3082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>44097</v>
       </c>
@@ -3119,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>44098</v>
       </c>
@@ -3151,7 +3146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>44099</v>
       </c>
@@ -3183,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>44100</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>44101</v>
       </c>
@@ -3247,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>44102</v>
       </c>
@@ -3279,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>44103</v>
       </c>
@@ -3311,7 +3306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>44104</v>
       </c>
@@ -3343,7 +3338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -3375,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>44106</v>
       </c>
@@ -3407,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>44107</v>
       </c>
@@ -3439,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>44108</v>
       </c>
@@ -3471,7 +3466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>44109</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>44110</v>
       </c>
@@ -3535,7 +3530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>44111</v>
       </c>
@@ -3567,7 +3562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -3599,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>44113</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>44114</v>
       </c>
@@ -3663,7 +3658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>44115</v>
       </c>
@@ -3695,7 +3690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>44116</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>44117</v>
       </c>
@@ -3759,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>44118</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>44119</v>
       </c>
@@ -3823,7 +3818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>44120</v>
       </c>
@@ -3855,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>44121</v>
       </c>
@@ -3887,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>44122</v>
       </c>
@@ -3919,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>44123</v>
       </c>
@@ -3951,7 +3946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>44124</v>
       </c>
@@ -3983,7 +3978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>44125</v>
       </c>
@@ -4015,7 +4010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>44126</v>
       </c>
@@ -4047,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>44127</v>
       </c>
@@ -4079,7 +4074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>44128</v>
       </c>
@@ -4111,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>44129</v>
       </c>
@@ -4143,7 +4138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>44130</v>
       </c>
@@ -4175,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>44131</v>
       </c>
@@ -4207,7 +4202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>44132</v>
       </c>
@@ -4239,7 +4234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>44133</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>44134</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>44135</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>44136</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>44137</v>
       </c>
@@ -4399,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>44138</v>
       </c>
@@ -4431,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>44139</v>
       </c>
@@ -4463,7 +4458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>44140</v>
       </c>
@@ -4495,7 +4490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>44141</v>
       </c>
@@ -4527,7 +4522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>44142</v>
       </c>
@@ -4559,7 +4554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>44143</v>
       </c>
@@ -4591,7 +4586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>44144</v>
       </c>
@@ -4623,7 +4618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>44145</v>
       </c>
@@ -4655,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>44146</v>
       </c>
@@ -4687,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>44147</v>
       </c>
@@ -4719,7 +4714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>44148</v>
       </c>
@@ -4751,7 +4746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>44149</v>
       </c>
@@ -4783,7 +4778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>44150</v>
       </c>
@@ -4815,7 +4810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>44151</v>
       </c>
@@ -4847,7 +4842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>44152</v>
       </c>
@@ -4879,7 +4874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>44153</v>
       </c>
@@ -4911,7 +4906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>44154</v>
       </c>
@@ -4943,7 +4938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>44155</v>
       </c>
@@ -4975,7 +4970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>44156</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>44157</v>
       </c>
@@ -5039,7 +5034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>44158</v>
       </c>
@@ -5071,7 +5066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>44159</v>
       </c>
@@ -5103,7 +5098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>44160</v>
       </c>
@@ -5135,7 +5130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>44161</v>
       </c>
@@ -5167,7 +5162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>44162</v>
       </c>
@@ -5199,7 +5194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>44163</v>
       </c>
@@ -5231,7 +5226,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>44164</v>
       </c>
@@ -5263,7 +5258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>44165</v>
       </c>
@@ -5295,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>44166</v>
       </c>
@@ -5327,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>44167</v>
       </c>
@@ -5359,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>44168</v>
       </c>
@@ -5391,7 +5386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>44169</v>
       </c>
@@ -5423,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>44170</v>
       </c>
@@ -5455,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>44171</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>44172</v>
       </c>
@@ -5519,7 +5514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>44173</v>
       </c>
@@ -5551,7 +5546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>44174</v>
       </c>
@@ -5583,7 +5578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>44175</v>
       </c>
@@ -5615,7 +5610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>44176</v>
       </c>
@@ -5647,7 +5642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>44177</v>
       </c>
@@ -5679,7 +5674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>44178</v>
       </c>
@@ -5711,7 +5706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>44179</v>
       </c>
@@ -5743,7 +5738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>44180</v>
       </c>
@@ -5775,7 +5770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>44181</v>
       </c>
@@ -5807,7 +5802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>44182</v>
       </c>
@@ -5839,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>44183</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>44184</v>
       </c>
@@ -5903,7 +5898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>44185</v>
       </c>
@@ -5935,7 +5930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>44186</v>
       </c>
@@ -5967,7 +5962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>44187</v>
       </c>
@@ -5999,7 +5994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>44188</v>
       </c>
@@ -6031,7 +6026,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>44189</v>
       </c>
@@ -6063,7 +6058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <v>44190</v>
       </c>
@@ -6095,7 +6090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <v>44191</v>
       </c>
@@ -6127,7 +6122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <v>44192</v>
       </c>
@@ -6159,7 +6154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <v>44193</v>
       </c>
@@ -6191,7 +6186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <v>44194</v>
       </c>
@@ -6223,7 +6218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <v>44195</v>
       </c>
@@ -6255,7 +6250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <v>44196</v>
       </c>
@@ -6287,7 +6282,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <v>44197</v>
       </c>
@@ -6319,7 +6314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <v>44198</v>
       </c>
@@ -6351,7 +6346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <v>44199</v>
       </c>
@@ -6383,7 +6378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <v>44200</v>
       </c>
@@ -6415,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <v>44201</v>
       </c>
@@ -6447,7 +6442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <v>44202</v>
       </c>
@@ -6479,7 +6474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <v>44203</v>
       </c>
@@ -6511,7 +6506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <v>44204</v>
       </c>
@@ -6543,7 +6538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <v>44205</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <v>44206</v>
       </c>
@@ -6607,7 +6602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <v>44207</v>
       </c>
@@ -6639,7 +6634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <v>44208</v>
       </c>
@@ -6671,7 +6666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <v>44209</v>
       </c>
@@ -6703,7 +6698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <v>44210</v>
       </c>
@@ -6735,7 +6730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <v>44211</v>
       </c>
@@ -6767,7 +6762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <v>44212</v>
       </c>
@@ -6799,7 +6794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <v>44213</v>
       </c>
@@ -6831,7 +6826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <v>44214</v>
       </c>
@@ -6863,7 +6858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <v>44215</v>
       </c>
@@ -6895,7 +6890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <v>44216</v>
       </c>
@@ -6927,7 +6922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <v>44217</v>
       </c>
@@ -6959,7 +6954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <v>44218</v>
       </c>
@@ -6991,7 +6986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <v>44219</v>
       </c>
@@ -7023,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <v>44220</v>
       </c>
@@ -7055,7 +7050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <v>44221</v>
       </c>
@@ -7087,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <v>44222</v>
       </c>
@@ -7119,7 +7114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <v>44223</v>
       </c>
@@ -7151,7 +7146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <v>44224</v>
       </c>
@@ -7183,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <v>44225</v>
       </c>
@@ -7215,7 +7210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <v>44226</v>
       </c>
@@ -7247,7 +7242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <v>44227</v>
       </c>
@@ -7279,7 +7274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <v>44228</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <v>44229</v>
       </c>
@@ -7343,7 +7338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <v>44230</v>
       </c>
@@ -7375,7 +7370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <v>44231</v>
       </c>
@@ -7407,7 +7402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <v>44232</v>
       </c>
@@ -7439,7 +7434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <v>44233</v>
       </c>
@@ -7471,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <v>44234</v>
       </c>
@@ -7503,7 +7498,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <v>44235</v>
       </c>
@@ -7535,7 +7530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <v>44236</v>
       </c>
@@ -7567,7 +7562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="1">
         <v>44237</v>
       </c>
@@ -7599,7 +7594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="1">
         <v>44238</v>
       </c>
@@ -7631,7 +7626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="1">
         <v>44239</v>
       </c>
@@ -7663,7 +7658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="1">
         <v>44240</v>
       </c>
@@ -7695,7 +7690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="1">
         <v>44241</v>
       </c>
@@ -7727,7 +7722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="1">
         <v>44242</v>
       </c>
@@ -7759,7 +7754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="1">
         <v>44243</v>
       </c>
@@ -7791,7 +7786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="1">
         <v>44244</v>
       </c>
@@ -7823,7 +7818,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="1">
         <v>44245</v>
       </c>
@@ -7855,7 +7850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="1">
         <v>44246</v>
       </c>
@@ -7887,7 +7882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="1">
         <v>44247</v>
       </c>
@@ -7919,7 +7914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="1">
         <v>44248</v>
       </c>
@@ -7951,7 +7946,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="1">
         <v>44249</v>
       </c>
@@ -7983,7 +7978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="1">
         <v>44250</v>
       </c>
@@ -8015,7 +8010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="1">
         <v>44251</v>
       </c>
@@ -8047,7 +8042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="1">
         <v>44252</v>
       </c>
@@ -8079,7 +8074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="1">
         <v>44253</v>
       </c>
@@ -8111,7 +8106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="1">
         <v>44254</v>
       </c>
@@ -8143,7 +8138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="1">
         <v>44255</v>
       </c>
@@ -8175,7 +8170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="1">
         <v>44256</v>
       </c>
@@ -8207,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="1">
         <v>44257</v>
       </c>
@@ -8239,7 +8234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="1">
         <v>44258</v>
       </c>
@@ -8271,7 +8266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="1">
         <v>44259</v>
       </c>
@@ -8303,7 +8298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="1">
         <v>44260</v>
       </c>
@@ -8335,7 +8330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="1">
         <v>44261</v>
       </c>
@@ -8367,7 +8362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="1">
         <v>44262</v>
       </c>
@@ -8399,7 +8394,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="1">
         <v>44263</v>
       </c>
@@ -8431,7 +8426,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="1">
         <v>44264</v>
       </c>
@@ -8463,7 +8458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="1">
         <v>44265</v>
       </c>
@@ -8495,7 +8490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="1">
         <v>44266</v>
       </c>
@@ -8527,7 +8522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="1">
         <v>44267</v>
       </c>
@@ -8559,7 +8554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="1">
         <v>44268</v>
       </c>
@@ -8591,7 +8586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="1">
         <v>44269</v>
       </c>
@@ -8623,7 +8618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="1">
         <v>44270</v>
       </c>
@@ -8655,7 +8650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="1">
         <v>44271</v>
       </c>
@@ -8687,7 +8682,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="1">
         <v>44272</v>
       </c>
@@ -8719,7 +8714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="1">
         <v>44273</v>
       </c>
@@ -8751,7 +8746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="1">
         <v>44274</v>
       </c>
@@ -8783,7 +8778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="1">
         <v>44275</v>
       </c>
@@ -8815,7 +8810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="1">
         <v>44276</v>
       </c>
@@ -8847,7 +8842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" s="1">
         <v>44277</v>
       </c>
@@ -8879,7 +8874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" s="1">
         <v>44278</v>
       </c>
@@ -8911,7 +8906,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" s="1">
         <v>44279</v>
       </c>
@@ -8943,7 +8938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" s="1">
         <v>44280</v>
       </c>
@@ -8975,7 +8970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" s="1">
         <v>44281</v>
       </c>
@@ -9007,7 +9002,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" s="1">
         <v>44282</v>
       </c>
@@ -9039,7 +9034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" s="1">
         <v>44283</v>
       </c>
@@ -9071,7 +9066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" s="1">
         <v>44284</v>
       </c>
@@ -9103,7 +9098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" s="1">
         <v>44285</v>
       </c>
@@ -9135,7 +9130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" s="1">
         <v>44286</v>
       </c>
@@ -9167,7 +9162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" s="1">
         <v>44287</v>
       </c>
@@ -9199,7 +9194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" s="1">
         <v>44288</v>
       </c>
@@ -9231,7 +9226,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" s="1">
         <v>44289</v>
       </c>
@@ -9263,7 +9258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" s="1">
         <v>44290</v>
       </c>
@@ -9295,7 +9290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" s="1">
         <v>44291</v>
       </c>
@@ -9327,7 +9322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" s="1">
         <v>44292</v>
       </c>
@@ -9359,7 +9354,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" s="1">
         <v>44293</v>
       </c>
@@ -9391,7 +9386,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" s="1">
         <v>44294</v>
       </c>
@@ -9423,7 +9418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" s="8">
         <v>44295</v>
       </c>
@@ -9455,7 +9450,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" s="1">
         <v>44296</v>
       </c>
@@ -9487,7 +9482,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" s="1">
         <v>44297</v>
       </c>
@@ -9519,7 +9514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" s="1">
         <v>44298</v>
       </c>
@@ -9551,7 +9546,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10">
       <c r="A286" s="1">
         <v>44299</v>
       </c>
@@ -9583,7 +9578,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10">
       <c r="A287" s="1">
         <v>44300</v>
       </c>
@@ -9615,7 +9610,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10">
       <c r="A288" s="1">
         <v>44301</v>
       </c>
@@ -9647,7 +9642,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10">
       <c r="A289" s="1">
         <v>44302</v>
       </c>
@@ -9679,7 +9674,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10">
       <c r="A290" s="1">
         <v>44303</v>
       </c>
@@ -9711,7 +9706,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10">
       <c r="A291" s="1">
         <v>44304</v>
       </c>
@@ -9743,7 +9738,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10">
       <c r="A292" s="1">
         <v>44305</v>
       </c>
@@ -9775,7 +9770,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10">
       <c r="A293" s="1">
         <v>44306</v>
       </c>
@@ -9807,7 +9802,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10">
       <c r="A294" s="1">
         <v>44307</v>
       </c>
@@ -9839,7 +9834,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10">
       <c r="A295" s="1">
         <v>44308</v>
       </c>
@@ -9871,7 +9866,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10">
       <c r="A296" s="1">
         <v>44309</v>
       </c>
@@ -9903,7 +9898,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10">
       <c r="A297" s="1">
         <v>44310</v>
       </c>
@@ -9935,7 +9930,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10">
       <c r="A298" s="1">
         <v>44311</v>
       </c>
@@ -9967,7 +9962,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10">
       <c r="A299" s="1">
         <v>44312</v>
       </c>
@@ -9999,7 +9994,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10">
       <c r="A300" s="1">
         <v>44313</v>
       </c>
@@ -10031,7 +10026,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10">
       <c r="A301" s="1">
         <v>44314</v>
       </c>
@@ -10063,7 +10058,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10">
       <c r="A302" s="1">
         <v>44315</v>
       </c>
@@ -10095,7 +10090,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10">
       <c r="A303" s="1">
         <v>44316</v>
       </c>
@@ -10127,7 +10122,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10">
       <c r="A304" s="1">
         <v>44317</v>
       </c>
@@ -10159,7 +10154,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10">
       <c r="A305" s="1">
         <v>44318</v>
       </c>
@@ -10191,7 +10186,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10">
       <c r="A306" s="1">
         <v>44319</v>
       </c>
@@ -10223,7 +10218,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10">
       <c r="A307" s="1">
         <v>44320</v>
       </c>
@@ -10255,7 +10250,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10">
       <c r="A308" s="1">
         <v>44321</v>
       </c>
@@ -10285,6 +10280,70 @@
       </c>
       <c r="J308" s="2">
         <v>92</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10">
+      <c r="A309" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B309" s="2">
+        <v>9527</v>
+      </c>
+      <c r="C309" s="2">
+        <v>189</v>
+      </c>
+      <c r="D309" s="2">
+        <v>3715</v>
+      </c>
+      <c r="E309" s="2">
+        <v>13431</v>
+      </c>
+      <c r="F309" s="2">
+        <v>3272</v>
+      </c>
+      <c r="G309" s="2">
+        <v>350</v>
+      </c>
+      <c r="H309" s="2">
+        <v>21</v>
+      </c>
+      <c r="I309" s="2">
+        <v>329</v>
+      </c>
+      <c r="J309" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10">
+      <c r="A310" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B310" s="2">
+        <v>9584</v>
+      </c>
+      <c r="C310" s="2">
+        <v>212</v>
+      </c>
+      <c r="D310" s="2">
+        <v>3771</v>
+      </c>
+      <c r="E310" s="2">
+        <v>13567</v>
+      </c>
+      <c r="F310" s="2">
+        <v>3290</v>
+      </c>
+      <c r="G310" s="2">
+        <v>386</v>
+      </c>
+      <c r="H310" s="2">
+        <v>20</v>
+      </c>
+      <c r="I310" s="2">
+        <v>366</v>
+      </c>
+      <c r="J310" s="2">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -10297,29 +10356,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -10354,7 +10413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>44014</v>
       </c>
@@ -10377,7 +10436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3">
         <v>44013</v>
       </c>
@@ -10400,7 +10459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>44012</v>
       </c>
@@ -10423,7 +10482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="3">
         <v>44011</v>
       </c>
@@ -10446,7 +10505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="3">
         <v>44010</v>
       </c>
@@ -10469,7 +10528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="3">
         <v>44009</v>
       </c>
@@ -10492,7 +10551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="3">
         <v>44008</v>
       </c>
@@ -10512,7 +10571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="3">
         <v>44007</v>
       </c>
@@ -10532,7 +10591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="3">
         <v>44006</v>
       </c>
@@ -10552,7 +10611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="3">
         <v>44005</v>
       </c>
@@ -10572,7 +10631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="3">
         <v>44004</v>
       </c>
@@ -10592,12 +10651,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="3">
         <v>44003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="3">
         <v>44002</v>
       </c>
@@ -10617,7 +10676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="3">
         <v>44001</v>
       </c>
@@ -10637,7 +10696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="3">
         <v>44000</v>
       </c>
@@ -10657,7 +10716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="3">
         <v>43999</v>
       </c>
@@ -10677,7 +10736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3">
         <v>43998</v>
       </c>
@@ -10697,7 +10756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3">
         <v>43997</v>
       </c>
@@ -10717,7 +10776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3">
         <v>43996</v>
       </c>
@@ -10737,7 +10796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="3">
         <v>43995</v>
       </c>
@@ -10757,7 +10816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="3">
         <v>43994</v>
       </c>
@@ -10777,7 +10836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3">
         <v>43993</v>
       </c>
@@ -10785,7 +10844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="3">
         <v>43992</v>
       </c>
@@ -10808,7 +10867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3">
         <v>43992</v>
       </c>
@@ -10828,7 +10887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3">
         <v>43991</v>
       </c>
@@ -10848,7 +10907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="3">
         <v>43990</v>
       </c>
@@ -10868,17 +10927,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3">
         <v>43989</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>43988</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>43987</v>
       </c>
@@ -10898,7 +10957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>43986</v>
       </c>
@@ -10921,7 +10980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       